<commit_message>
kospi kosdaq save file add
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>code</t>
   </si>
@@ -85,91 +85,217 @@
     <t>이득20</t>
   </si>
   <si>
+    <t>097520</t>
+  </si>
+  <si>
+    <t>208710</t>
+  </si>
+  <si>
+    <t>230360</t>
+  </si>
+  <si>
+    <t>049070</t>
+  </si>
+  <si>
+    <t>053450</t>
+  </si>
+  <si>
+    <t>017890</t>
+  </si>
+  <si>
+    <t>083450</t>
+  </si>
+  <si>
+    <t>061970</t>
+  </si>
+  <si>
+    <t>076610</t>
+  </si>
+  <si>
+    <t>009830</t>
+  </si>
+  <si>
+    <t>067170</t>
+  </si>
+  <si>
+    <t>243070</t>
+  </si>
+  <si>
+    <t>131030</t>
+  </si>
+  <si>
+    <t>067010</t>
+  </si>
+  <si>
+    <t>004650</t>
+  </si>
+  <si>
+    <t>014130</t>
+  </si>
+  <si>
+    <t>220630</t>
+  </si>
+  <si>
     <t>001820</t>
   </si>
   <si>
     <t>008490</t>
   </si>
   <si>
+    <t>217190</t>
+  </si>
+  <si>
+    <t>037460</t>
+  </si>
+  <si>
+    <t>284740</t>
+  </si>
+  <si>
+    <t>194370</t>
+  </si>
+  <si>
+    <t>071200</t>
+  </si>
+  <si>
+    <t>064290</t>
+  </si>
+  <si>
     <t>009150</t>
   </si>
   <si>
+    <t>189690</t>
+  </si>
+  <si>
+    <t>222080</t>
+  </si>
+  <si>
+    <t>089980</t>
+  </si>
+  <si>
+    <t>073490</t>
+  </si>
+  <si>
+    <t>131370</t>
+  </si>
+  <si>
+    <t>217820</t>
+  </si>
+  <si>
+    <t>033640</t>
+  </si>
+  <si>
+    <t>206640</t>
+  </si>
+  <si>
+    <t>241590</t>
+  </si>
+  <si>
+    <t>046890</t>
+  </si>
+  <si>
+    <t>099320</t>
+  </si>
+  <si>
+    <t>134060</t>
+  </si>
+  <si>
+    <t>070300</t>
+  </si>
+  <si>
+    <t>131970</t>
+  </si>
+  <si>
+    <t>214450</t>
+  </si>
+  <si>
+    <t>133750</t>
+  </si>
+  <si>
+    <t>161890</t>
+  </si>
+  <si>
+    <t>094360</t>
+  </si>
+  <si>
+    <t>057680</t>
+  </si>
+  <si>
+    <t>189300</t>
+  </si>
+  <si>
+    <t>242040</t>
+  </si>
+  <si>
     <t>026890</t>
   </si>
   <si>
-    <t>037460</t>
-  </si>
-  <si>
-    <t>046890</t>
-  </si>
-  <si>
-    <t>049070</t>
-  </si>
-  <si>
-    <t>053450</t>
-  </si>
-  <si>
-    <t>061970</t>
-  </si>
-  <si>
-    <t>064290</t>
-  </si>
-  <si>
-    <t>065130</t>
-  </si>
-  <si>
-    <t>071200</t>
-  </si>
-  <si>
-    <t>073490</t>
-  </si>
-  <si>
-    <t>076610</t>
-  </si>
-  <si>
-    <t>083450</t>
-  </si>
-  <si>
-    <t>089980</t>
-  </si>
-  <si>
     <t>093370</t>
   </si>
   <si>
-    <t>094360</t>
-  </si>
-  <si>
-    <t>097520</t>
-  </si>
-  <si>
-    <t>099320</t>
-  </si>
-  <si>
-    <t>161890</t>
-  </si>
-  <si>
-    <t>189300</t>
-  </si>
-  <si>
-    <t>194370</t>
-  </si>
-  <si>
-    <t>206640</t>
-  </si>
-  <si>
-    <t>220630</t>
-  </si>
-  <si>
-    <t>230360</t>
-  </si>
-  <si>
-    <t>243070</t>
+    <t>148250</t>
+  </si>
+  <si>
+    <t>215380</t>
+  </si>
+  <si>
+    <t>213420</t>
+  </si>
+  <si>
+    <t>000250</t>
   </si>
   <si>
     <t>253450</t>
   </si>
   <si>
-    <t>284740</t>
+    <t>엠씨넥스</t>
+  </si>
+  <si>
+    <t>바이오로그디바이스</t>
+  </si>
+  <si>
+    <t>에코마케팅</t>
+  </si>
+  <si>
+    <t>인탑스</t>
+  </si>
+  <si>
+    <t>세코닉스</t>
+  </si>
+  <si>
+    <t>한국알콜</t>
+  </si>
+  <si>
+    <t>GST</t>
+  </si>
+  <si>
+    <t>엘비세미콘</t>
+  </si>
+  <si>
+    <t>해성옵틱스</t>
+  </si>
+  <si>
+    <t>한화솔루션</t>
+  </si>
+  <si>
+    <t>오텍</t>
+  </si>
+  <si>
+    <t>휴온스</t>
+  </si>
+  <si>
+    <t>디에이치피코리아</t>
+  </si>
+  <si>
+    <t>이씨에스</t>
+  </si>
+  <si>
+    <t>창해에탄올</t>
+  </si>
+  <si>
+    <t>한익스프레스</t>
+  </si>
+  <si>
+    <t>해마로푸드서비스</t>
   </si>
   <si>
     <t>삼화콘덴서</t>
@@ -178,85 +304,109 @@
     <t>서흥</t>
   </si>
   <si>
+    <t>제너셈</t>
+  </si>
+  <si>
+    <t>삼지전자</t>
+  </si>
+  <si>
+    <t>쿠쿠홈시스</t>
+  </si>
+  <si>
+    <t>제이에스코퍼레이션</t>
+  </si>
+  <si>
+    <t>인피니트헬스케어</t>
+  </si>
+  <si>
+    <t>인텍플러스</t>
+  </si>
+  <si>
     <t>삼성전기</t>
   </si>
   <si>
+    <t>포시에스</t>
+  </si>
+  <si>
+    <t>씨아이에스</t>
+  </si>
+  <si>
+    <t>상아프론테크</t>
+  </si>
+  <si>
+    <t>이노와이어리스</t>
+  </si>
+  <si>
+    <t>알서포트</t>
+  </si>
+  <si>
+    <t>엔에스</t>
+  </si>
+  <si>
+    <t>네패스</t>
+  </si>
+  <si>
+    <t>바디텍메드</t>
+  </si>
+  <si>
+    <t>화승엔터프라이즈</t>
+  </si>
+  <si>
+    <t>서울반도체</t>
+  </si>
+  <si>
+    <t>쎄트렉아이</t>
+  </si>
+  <si>
+    <t>이퓨쳐</t>
+  </si>
+  <si>
+    <t>한솔시큐어</t>
+  </si>
+  <si>
+    <t>테스나</t>
+  </si>
+  <si>
+    <t>파마리서치프로덕트</t>
+  </si>
+  <si>
+    <t>메가엠디</t>
+  </si>
+  <si>
+    <t>한국콜마</t>
+  </si>
+  <si>
+    <t>칩스앤미디어</t>
+  </si>
+  <si>
+    <t>옴니텔</t>
+  </si>
+  <si>
+    <t>인텔리안테크</t>
+  </si>
+  <si>
+    <t>나무기술</t>
+  </si>
+  <si>
     <t>디피씨</t>
   </si>
   <si>
-    <t>삼지전자</t>
-  </si>
-  <si>
-    <t>서울반도체</t>
-  </si>
-  <si>
-    <t>인탑스</t>
-  </si>
-  <si>
-    <t>세코닉스</t>
-  </si>
-  <si>
-    <t>엘비세미콘</t>
-  </si>
-  <si>
-    <t>인텍플러스</t>
-  </si>
-  <si>
-    <t>탑엔지니어링</t>
-  </si>
-  <si>
-    <t>인피니트헬스케어</t>
-  </si>
-  <si>
-    <t>이노와이어리스</t>
-  </si>
-  <si>
-    <t>해성옵틱스</t>
-  </si>
-  <si>
-    <t>GST</t>
-  </si>
-  <si>
-    <t>상아프론테크</t>
-  </si>
-  <si>
     <t>후성</t>
   </si>
   <si>
-    <t>칩스앤미디어</t>
-  </si>
-  <si>
-    <t>엠씨넥스</t>
-  </si>
-  <si>
-    <t>쎄트렉아이</t>
-  </si>
-  <si>
-    <t>한국콜마</t>
-  </si>
-  <si>
-    <t>인텔리안테크</t>
-  </si>
-  <si>
-    <t>제이에스코퍼레이션</t>
-  </si>
-  <si>
-    <t>바디텍메드</t>
-  </si>
-  <si>
-    <t>해마로푸드서비스</t>
-  </si>
-  <si>
-    <t>에코마케팅</t>
-  </si>
-  <si>
-    <t>휴온스</t>
+    <t>알엔투테크놀로지</t>
+  </si>
+  <si>
+    <t>우정바이오</t>
+  </si>
+  <si>
+    <t>덕산네오룩스</t>
+  </si>
+  <si>
+    <t>삼천당제약</t>
   </si>
   <si>
     <t>스튜디오드래곤</t>
-  </si>
-  <si>
-    <t>쿠쿠홈시스</t>
   </si>
 </sst>
 </file>
@@ -614,7 +764,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X30"/>
+  <dimension ref="A1:X55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -699,70 +849,70 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="D2">
-        <v>68000</v>
+        <v>39700</v>
       </c>
       <c r="E2">
-        <v>11.57161556705366</v>
+        <v>10.32497616399473</v>
       </c>
       <c r="F2">
-        <v>12.98780532537563</v>
+        <v>0.6600709489047745</v>
       </c>
       <c r="G2">
-        <v>29.39297451711403</v>
+        <v>1.755630050070565</v>
       </c>
       <c r="H2">
-        <v>41.08137332404019</v>
+        <v>28.27399615653999</v>
       </c>
       <c r="I2">
-        <v>28.90000000000003</v>
+        <v>38.12000000000003</v>
       </c>
       <c r="J2">
-        <v>4307</v>
+        <v>4572</v>
       </c>
       <c r="K2">
-        <v>14903</v>
+        <v>11881</v>
       </c>
       <c r="L2">
-        <v>0.6</v>
+        <v>2.3</v>
       </c>
       <c r="M2">
-        <v>15.78825168330625</v>
+        <v>8.683289588801399</v>
       </c>
       <c r="N2">
-        <v>4.562839696705361</v>
+        <v>3.341469573268244</v>
       </c>
       <c r="O2">
-        <v>196056.2393309899</v>
+        <v>14139.61136631557</v>
       </c>
       <c r="P2">
-        <v>11.16988989377581</v>
+        <v>-9.808689657847081</v>
       </c>
       <c r="Q2">
-        <v>120361.5237646538</v>
+        <v>8680.494817696692</v>
       </c>
       <c r="R2">
-        <v>177.0022408303732</v>
+        <v>21.8652262410496</v>
       </c>
       <c r="S2">
-        <v>75588.16742485332</v>
+        <v>5451.432277424497</v>
       </c>
       <c r="T2">
-        <v>111.1590697424313</v>
+        <v>13.73156744943198</v>
       </c>
       <c r="U2">
-        <v>48462.10390238895</v>
+        <v>3495.095680260109</v>
       </c>
       <c r="V2">
-        <v>71.26779985645433</v>
+        <v>8.803767456574581</v>
       </c>
       <c r="W2">
-        <v>31664.17721234264</v>
+        <v>2283.626175552685</v>
       </c>
       <c r="X2">
-        <v>46.56496648873917</v>
+        <v>5.752206991316588</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -773,70 +923,70 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="D3">
-        <v>39700</v>
+        <v>1880</v>
       </c>
       <c r="E3">
-        <v>8.003743285250167</v>
+        <v>34.35131625501245</v>
       </c>
       <c r="F3">
-        <v>9.637970928865741</v>
+        <v>18.11424148373618</v>
       </c>
       <c r="G3">
-        <v>9.940922606544959</v>
+        <v>11.91931581011643</v>
       </c>
       <c r="H3">
-        <v>10.53175146909021</v>
+        <v>12.77337607124542</v>
       </c>
       <c r="I3">
-        <v>11.79999999999998</v>
+        <v>14.76999999999997</v>
       </c>
       <c r="J3">
-        <v>3006</v>
+        <v>299</v>
       </c>
       <c r="K3">
-        <v>25487</v>
+        <v>1961</v>
       </c>
       <c r="L3">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>13.20691949434464</v>
+        <v>6.287625418060201</v>
       </c>
       <c r="N3">
-        <v>1.557656844665908</v>
+        <v>0.958694543600204</v>
       </c>
       <c r="O3">
-        <v>65752.53342123679</v>
+        <v>6046.834177686939</v>
       </c>
       <c r="P3">
-        <v>5.174921948178124</v>
+        <v>12.39241962998265</v>
       </c>
       <c r="Q3">
-        <v>40366.35172117898</v>
+        <v>3712.23164364525</v>
       </c>
       <c r="R3">
-        <v>101.678467811534</v>
+        <v>197.4591299811303</v>
       </c>
       <c r="S3">
-        <v>25350.44802354883</v>
+        <v>2331.316339500338</v>
       </c>
       <c r="T3">
-        <v>63.85503280490889</v>
+        <v>124.0061882712946</v>
       </c>
       <c r="U3">
-        <v>16253.02065049658</v>
+        <v>1494.6849291792</v>
       </c>
       <c r="V3">
-        <v>40.9395986158604</v>
+        <v>79.50451750953194</v>
       </c>
       <c r="W3">
-        <v>10619.40123668091</v>
+        <v>976.5974785055705</v>
       </c>
       <c r="X3">
-        <v>26.7491215029746</v>
+        <v>51.94667438859418</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -847,70 +997,70 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="D4">
-        <v>146000</v>
+        <v>28350</v>
       </c>
       <c r="E4">
-        <v>7.830830248293978</v>
+        <v>25.18787091785846</v>
       </c>
       <c r="F4">
-        <v>5.673093905494596</v>
+        <v>22.63709255896887</v>
       </c>
       <c r="G4">
-        <v>7.184947541800824</v>
+        <v>16.54584517318082</v>
       </c>
       <c r="H4">
-        <v>14.26640113409157</v>
+        <v>25.01326749741341</v>
       </c>
       <c r="I4">
-        <v>13.46000000000001</v>
+        <v>31.53999999999999</v>
       </c>
       <c r="J4">
-        <v>9308</v>
+        <v>2004</v>
       </c>
       <c r="K4">
-        <v>69165</v>
+        <v>6354</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>3.4</v>
       </c>
       <c r="M4">
-        <v>15.68543188654921</v>
+        <v>14.14670658682635</v>
       </c>
       <c r="N4">
-        <v>2.110894238415383</v>
+        <v>4.461756373937677</v>
       </c>
       <c r="O4">
-        <v>138428.1384477472</v>
+        <v>29377.52246516888</v>
       </c>
       <c r="P4">
-        <v>-0.5311373182445789</v>
+        <v>0.3566626304315923</v>
       </c>
       <c r="Q4">
-        <v>84982.86885604713</v>
+        <v>18035.25039755857</v>
       </c>
       <c r="R4">
-        <v>58.20744442195009</v>
+        <v>63.61640351872511</v>
       </c>
       <c r="S4">
-        <v>53370.03984675104</v>
+        <v>11326.30664651117</v>
       </c>
       <c r="T4">
-        <v>36.55482181284317</v>
+        <v>39.95169892949266</v>
       </c>
       <c r="U4">
-        <v>34217.31872120335</v>
+        <v>7261.674257141283</v>
       </c>
       <c r="V4">
-        <v>23.43651967205709</v>
+        <v>25.6143712773943</v>
       </c>
       <c r="W4">
-        <v>22356.91718835968</v>
+        <v>4744.63388959664</v>
       </c>
       <c r="X4">
-        <v>15.31295697832855</v>
+        <v>16.73592200915922</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -921,70 +1071,70 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="D5">
-        <v>11750</v>
+        <v>13700</v>
       </c>
       <c r="E5">
-        <v>6.786090547831165</v>
+        <v>6.784710160772605</v>
       </c>
       <c r="F5">
-        <v>8.063858202242528</v>
+        <v>3.397155874696452</v>
       </c>
       <c r="G5">
-        <v>6.805380515713665</v>
+        <v>5.960450358089915</v>
       </c>
       <c r="H5">
-        <v>6.188691576477694</v>
+        <v>7.723227615342381</v>
       </c>
       <c r="I5">
-        <v>5.640000000000015</v>
+        <v>9.029999999999959</v>
       </c>
       <c r="J5">
-        <v>207</v>
+        <v>2276</v>
       </c>
       <c r="K5">
-        <v>3664</v>
+        <v>25205</v>
       </c>
       <c r="L5">
-        <v>1.2</v>
+        <v>1.7</v>
       </c>
       <c r="M5">
-        <v>56.76328502415459</v>
+        <v>6.019332161687171</v>
       </c>
       <c r="N5">
-        <v>3.206877729257642</v>
+        <v>0.543542947827812</v>
       </c>
       <c r="O5">
-        <v>7077.612498493862</v>
+        <v>44970.18318433803</v>
       </c>
       <c r="P5">
-        <v>-4.942827607569711</v>
+        <v>12.62126701630899</v>
       </c>
       <c r="Q5">
-        <v>4345.040116251108</v>
+        <v>27607.79147102089</v>
       </c>
       <c r="R5">
-        <v>36.97906481915837</v>
+        <v>201.5167260658459</v>
       </c>
       <c r="S5">
-        <v>2728.726003976888</v>
+        <v>17337.95235113828</v>
       </c>
       <c r="T5">
-        <v>23.22320003384586</v>
+        <v>126.5543967236371</v>
       </c>
       <c r="U5">
-        <v>1749.47756548465</v>
+        <v>11115.94151466707</v>
       </c>
       <c r="V5">
-        <v>14.88917077008213</v>
+        <v>81.13825923114649</v>
       </c>
       <c r="W5">
-        <v>1143.073932037709</v>
+        <v>7262.935647849655</v>
       </c>
       <c r="X5">
-        <v>9.728288783299652</v>
+        <v>53.01412881642084</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -995,70 +1145,70 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="D6">
-        <v>11200</v>
+        <v>7830</v>
       </c>
       <c r="E6">
-        <v>4.763907634449509</v>
+        <v>7.766207062970892</v>
       </c>
       <c r="F6">
-        <v>9.30689726518024</v>
+        <v>4.215437490805499</v>
       </c>
       <c r="G6">
-        <v>11.83297375633879</v>
+        <v>0.8210067253720581</v>
       </c>
       <c r="H6">
-        <v>7.163996652458891</v>
+        <v>1.171708580322999</v>
       </c>
       <c r="I6">
-        <v>6.889999999999972</v>
+        <v>4.550000000000026</v>
       </c>
       <c r="J6">
-        <v>842</v>
+        <v>537</v>
       </c>
       <c r="K6">
-        <v>12221</v>
+        <v>11809</v>
       </c>
       <c r="L6">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>13.30166270783848</v>
+        <v>14.58100558659218</v>
       </c>
       <c r="N6">
-        <v>0.9164552818918256</v>
+        <v>0.6630536031840122</v>
       </c>
       <c r="O6">
-        <v>37394.30604425666</v>
+        <v>12815.14189750114</v>
       </c>
       <c r="P6">
-        <v>12.81289534456267</v>
+        <v>5.050026362187543</v>
       </c>
       <c r="Q6">
-        <v>22956.86008752848</v>
+        <v>7867.385456881421</v>
       </c>
       <c r="R6">
-        <v>204.9719650672185</v>
+        <v>100.4774643279875</v>
       </c>
       <c r="S6">
-        <v>14417.12375823732</v>
+        <v>4940.791961668796</v>
       </c>
       <c r="T6">
-        <v>128.7243192699761</v>
+        <v>63.10079133676623</v>
       </c>
       <c r="U6">
-        <v>9243.300550180695</v>
+        <v>3167.707083843829</v>
       </c>
       <c r="V6">
-        <v>82.52946919804191</v>
+        <v>40.456029167865</v>
       </c>
       <c r="W6">
-        <v>6039.389194438955</v>
+        <v>2069.716961972006</v>
       </c>
       <c r="X6">
-        <v>53.92311780749067</v>
+        <v>26.43316681956584</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -1069,70 +1219,70 @@
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D7">
-        <v>18950</v>
+        <v>14450</v>
       </c>
       <c r="E7">
-        <v>4.310988145912432</v>
+        <v>8.191662932123933</v>
       </c>
       <c r="F7">
-        <v>4.76951311414723</v>
+        <v>9.002955936466662</v>
       </c>
       <c r="G7">
-        <v>7.854132035005819</v>
+        <v>9.618336740356312</v>
       </c>
       <c r="H7">
-        <v>9.67928990222093</v>
+        <v>10.10468881870398</v>
       </c>
       <c r="I7">
-        <v>9.289999999999978</v>
+        <v>10.00000000000004</v>
       </c>
       <c r="J7">
-        <v>1070</v>
+        <v>1490</v>
       </c>
       <c r="K7">
-        <v>11519</v>
+        <v>14907</v>
       </c>
       <c r="L7">
-        <v>1.5</v>
+        <v>0.7</v>
       </c>
       <c r="M7">
-        <v>17.71028037383178</v>
+        <v>9.697986577181208</v>
       </c>
       <c r="N7">
-        <v>1.645108082298811</v>
+        <v>0.9693432615549742</v>
       </c>
       <c r="O7">
-        <v>24534.80778105288</v>
+        <v>37344.12886514056</v>
       </c>
       <c r="P7">
-        <v>2.616534665734305</v>
+        <v>9.960181645373511</v>
       </c>
       <c r="Q7">
-        <v>15062.24366986331</v>
+        <v>22926.05565224382</v>
       </c>
       <c r="R7">
-        <v>79.4841354610201</v>
+        <v>158.6578245830022</v>
       </c>
       <c r="S7">
-        <v>9459.230497428391</v>
+        <v>14397.7782835466</v>
       </c>
       <c r="T7">
-        <v>49.91678362759045</v>
+        <v>99.6386040383848</v>
       </c>
       <c r="U7">
-        <v>6064.629251116025</v>
+        <v>9230.897518906857</v>
       </c>
       <c r="V7">
-        <v>32.00332058636425</v>
+        <v>63.88164372945921</v>
       </c>
       <c r="W7">
-        <v>3962.508431769269</v>
+        <v>6031.285299878041</v>
       </c>
       <c r="X7">
-        <v>20.91033473229166</v>
+        <v>41.73899861507294</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -1143,70 +1293,70 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="D8">
-        <v>14100</v>
+        <v>16400</v>
       </c>
       <c r="E8">
-        <v>6.784710160772605</v>
+        <v>12.51383096407281</v>
       </c>
       <c r="F8">
-        <v>3.397155874696452</v>
+        <v>12.73578739073582</v>
       </c>
       <c r="G8">
-        <v>5.960450358089915</v>
+        <v>14.969282939232</v>
       </c>
       <c r="H8">
-        <v>7.723227615342381</v>
+        <v>11.38565937649192</v>
       </c>
       <c r="I8">
-        <v>9.029999999999959</v>
+        <v>15.80999999999996</v>
       </c>
       <c r="J8">
-        <v>2276</v>
+        <v>1586</v>
       </c>
       <c r="K8">
-        <v>25205</v>
+        <v>10034</v>
       </c>
       <c r="L8">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>6.195079086115993</v>
+        <v>10.34047919293821</v>
       </c>
       <c r="N8">
-        <v>0.559412814917675</v>
+        <v>1.634442894159857</v>
       </c>
       <c r="O8">
-        <v>44970.18318433803</v>
+        <v>40484.83033276202</v>
       </c>
       <c r="P8">
-        <v>12.29762060501225</v>
+        <v>9.457329341636234</v>
       </c>
       <c r="Q8">
-        <v>27607.79147102089</v>
+        <v>24854.17390863154</v>
       </c>
       <c r="R8">
-        <v>195.7999395107865</v>
+        <v>151.5498409062899</v>
       </c>
       <c r="S8">
-        <v>17337.95235113828</v>
+        <v>15608.65465848954</v>
       </c>
       <c r="T8">
-        <v>122.9642010719027</v>
+        <v>95.17472352737524</v>
       </c>
       <c r="U8">
-        <v>11115.94151466707</v>
+        <v>10007.23088819738</v>
       </c>
       <c r="V8">
-        <v>78.83646464302886</v>
+        <v>61.0197005377889</v>
       </c>
       <c r="W8">
-        <v>7262.935647849655</v>
+        <v>6538.526121089239</v>
       </c>
       <c r="X8">
-        <v>51.51018189964294</v>
+        <v>39.86906171395877</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -1217,70 +1367,70 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="D9">
-        <v>8500</v>
+        <v>8340</v>
       </c>
       <c r="E9">
-        <v>7.766207062970892</v>
+        <v>12.87673684478015</v>
       </c>
       <c r="F9">
-        <v>4.215437490805499</v>
+        <v>3.839137463505551</v>
       </c>
       <c r="G9">
-        <v>0.8210067253720581</v>
+        <v>12.48736101508194</v>
       </c>
       <c r="H9">
-        <v>1.171708580322999</v>
+        <v>18.87827195790587</v>
       </c>
       <c r="I9">
-        <v>4.550000000000026</v>
+        <v>21.73999999999999</v>
       </c>
       <c r="J9">
-        <v>537</v>
+        <v>703</v>
       </c>
       <c r="K9">
-        <v>11809</v>
+        <v>3235</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>15.82867783985103</v>
+        <v>11.86344238975818</v>
       </c>
       <c r="N9">
-        <v>0.7197899906850707</v>
+        <v>2.578052550231839</v>
       </c>
       <c r="O9">
-        <v>12815.14189750114</v>
+        <v>10493.28738518514</v>
       </c>
       <c r="P9">
-        <v>4.191058311807727</v>
+        <v>2.323303217970518</v>
       </c>
       <c r="Q9">
-        <v>7867.385456881421</v>
+        <v>6441.968198977213</v>
       </c>
       <c r="R9">
-        <v>92.55747596331084</v>
+        <v>77.24182492778432</v>
       </c>
       <c r="S9">
-        <v>4940.791961668796</v>
+        <v>4045.616535413684</v>
       </c>
       <c r="T9">
-        <v>58.12696425492702</v>
+        <v>48.50859155172283</v>
       </c>
       <c r="U9">
-        <v>3167.707083843829</v>
+        <v>2593.78015855927</v>
       </c>
       <c r="V9">
-        <v>37.26714216286858</v>
+        <v>31.10048151749724</v>
       </c>
       <c r="W9">
-        <v>2069.716961972006</v>
+        <v>1694.724495574991</v>
       </c>
       <c r="X9">
-        <v>24.34961131731772</v>
+        <v>20.32043759682244</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -1291,70 +1441,70 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="D10">
-        <v>9230</v>
+        <v>2375</v>
       </c>
       <c r="E10">
-        <v>12.87673684478015</v>
+        <v>-0.1354724601163184</v>
       </c>
       <c r="F10">
-        <v>3.839137463505551</v>
+        <v>-7.255873447235714</v>
       </c>
       <c r="G10">
-        <v>12.48736101508194</v>
+        <v>-12.03146453983929</v>
       </c>
       <c r="H10">
-        <v>18.87827195790587</v>
+        <v>-6.247253650647892</v>
       </c>
       <c r="I10">
-        <v>21.73999999999999</v>
+        <v>4.039999999999964</v>
       </c>
       <c r="J10">
-        <v>703</v>
+        <v>130</v>
       </c>
       <c r="K10">
-        <v>3235</v>
+        <v>2494</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>13.12944523470839</v>
+        <v>18.26923076923077</v>
       </c>
       <c r="N10">
-        <v>2.853168469860897</v>
+        <v>0.9522854851643946</v>
       </c>
       <c r="O10">
-        <v>10493.28738518514</v>
+        <v>692.1019392907139</v>
       </c>
       <c r="P10">
-        <v>1.291029825286993</v>
+        <v>-11.60032970611693</v>
       </c>
       <c r="Q10">
-        <v>6441.968198977213</v>
+        <v>424.8905533318311</v>
       </c>
       <c r="R10">
-        <v>69.79380497266753</v>
+        <v>17.89012856134026</v>
       </c>
       <c r="S10">
-        <v>4045.616535413684</v>
+        <v>266.8352582946997</v>
       </c>
       <c r="T10">
-        <v>43.83116506407025</v>
+        <v>11.23516877030314</v>
       </c>
       <c r="U10">
-        <v>2593.78015855927</v>
+        <v>171.0770144699486</v>
       </c>
       <c r="V10">
-        <v>28.10162685329654</v>
+        <v>7.20324271452415</v>
       </c>
       <c r="W10">
-        <v>1694.724495574991</v>
+        <v>111.7783271243394</v>
       </c>
       <c r="X10">
-        <v>18.36104545585039</v>
+        <v>4.706455878919554</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -1365,70 +1515,70 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="D11">
-        <v>8250</v>
+        <v>20300</v>
       </c>
       <c r="E11">
-        <v>-5.62941063390349</v>
+        <v>6.344578431437967</v>
       </c>
       <c r="F11">
-        <v>-20.67834516482944</v>
+        <v>7.143662310234333</v>
       </c>
       <c r="G11">
-        <v>-14.09437256107617</v>
+        <v>8.916260803268102</v>
       </c>
       <c r="H11">
-        <v>-15.08144974910515</v>
+        <v>0.09557694835909558</v>
       </c>
       <c r="I11">
-        <v>2.679999999999978</v>
+        <v>-0.2599999999999767</v>
       </c>
       <c r="J11">
-        <v>43</v>
+        <v>-92</v>
       </c>
       <c r="K11">
-        <v>1595</v>
+        <v>38516</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11">
-        <v>191.8604651162791</v>
+        <v>-220.6521739130435</v>
       </c>
       <c r="N11">
-        <v>5.172413793103448</v>
+        <v>0.5270536919721674</v>
       </c>
       <c r="O11">
-        <v>349.1216884400737</v>
+        <v>90483.29555142291</v>
       </c>
       <c r="P11">
-        <v>-27.11262861733866</v>
+        <v>16.12005616023897</v>
       </c>
       <c r="Q11">
-        <v>214.3304316318889</v>
+        <v>55548.89436306414</v>
       </c>
       <c r="R11">
-        <v>2.597944625841077</v>
+        <v>273.6398737096756</v>
       </c>
       <c r="S11">
-        <v>134.601524172378</v>
+        <v>34885.22740532007</v>
       </c>
       <c r="T11">
-        <v>1.631533626331855</v>
+        <v>171.8484108636457</v>
       </c>
       <c r="U11">
-        <v>86.29754195782922</v>
+        <v>22366.08681981641</v>
       </c>
       <c r="V11">
-        <v>1.046030811610051</v>
+        <v>110.1777675853025</v>
       </c>
       <c r="W11">
-        <v>56.38510179100124</v>
+        <v>14613.55738982675</v>
       </c>
       <c r="X11">
-        <v>0.6834557792848636</v>
+        <v>71.98796743757019</v>
       </c>
     </row>
     <row r="12" spans="1:24">
@@ -1439,70 +1589,70 @@
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="D12">
-        <v>12200</v>
+        <v>12650</v>
       </c>
       <c r="E12">
-        <v>6.156493080320431</v>
+        <v>9.11548705561944</v>
       </c>
       <c r="F12">
-        <v>6.926901568434246</v>
+        <v>8.02974707468978</v>
       </c>
       <c r="G12">
-        <v>10.88494559777639</v>
+        <v>12.54457416663756</v>
       </c>
       <c r="H12">
-        <v>12.90065061341473</v>
+        <v>11.58412784658975</v>
       </c>
       <c r="I12">
-        <v>15.36999999999996</v>
+        <v>11.45</v>
       </c>
       <c r="J12">
-        <v>2064</v>
+        <v>1141</v>
       </c>
       <c r="K12">
-        <v>13428</v>
+        <v>9969</v>
       </c>
       <c r="L12">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <v>5.910852713178294</v>
+        <v>11.08676599474146</v>
       </c>
       <c r="N12">
-        <v>0.9085492999702115</v>
+        <v>1.268933694452804</v>
       </c>
       <c r="O12">
-        <v>37734.37924603753</v>
+        <v>32501.03704899139</v>
       </c>
       <c r="P12">
-        <v>11.95351610183963</v>
+        <v>9.89569231915619</v>
       </c>
       <c r="Q12">
-        <v>23165.6355332758</v>
+        <v>19952.81739819506</v>
       </c>
       <c r="R12">
-        <v>189.8822584694738</v>
+        <v>157.7297818039135</v>
       </c>
       <c r="S12">
-        <v>14548.23669909875</v>
+        <v>12530.55673373921</v>
       </c>
       <c r="T12">
-        <v>119.2478417958914</v>
+        <v>99.05578445643646</v>
       </c>
       <c r="U12">
-        <v>9327.361444622822</v>
+        <v>8033.759291610811</v>
       </c>
       <c r="V12">
-        <v>76.45378233297396</v>
+        <v>63.50797858980879</v>
       </c>
       <c r="W12">
-        <v>6094.312915117792</v>
+        <v>5249.098933121828</v>
       </c>
       <c r="X12">
-        <v>49.95338455014583</v>
+        <v>41.49485322625951</v>
       </c>
     </row>
     <row r="13" spans="1:24">
@@ -1513,70 +1663,70 @@
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="D13">
-        <v>6190</v>
+        <v>48100</v>
       </c>
       <c r="E13">
-        <v>4.907650159011212</v>
+        <v>24.07530428025683</v>
       </c>
       <c r="F13">
-        <v>6.311045998066092</v>
+        <v>24.07530428025683</v>
       </c>
       <c r="G13">
-        <v>6.109339139414985</v>
+        <v>26.05208807369344</v>
       </c>
       <c r="H13">
-        <v>9.438734374630513</v>
+        <v>25.52748725977094</v>
       </c>
       <c r="I13">
-        <v>13.36</v>
+        <v>21.96999999999994</v>
       </c>
       <c r="J13">
-        <v>468</v>
+        <v>4102</v>
       </c>
       <c r="K13">
-        <v>3507</v>
+        <v>18674</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13">
-        <v>13.22649572649573</v>
+        <v>11.72598732325695</v>
       </c>
       <c r="N13">
-        <v>1.765041345879669</v>
+        <v>2.575773803148763</v>
       </c>
       <c r="O13">
-        <v>6345.587879201983</v>
+        <v>189120.147008489</v>
       </c>
       <c r="P13">
-        <v>0.24855501241281</v>
+        <v>14.67249769820269</v>
       </c>
       <c r="Q13">
-        <v>3895.640500549695</v>
+        <v>116103.3647600882</v>
       </c>
       <c r="R13">
-        <v>62.93441842568166</v>
+        <v>241.37913671536</v>
       </c>
       <c r="S13">
-        <v>2446.498824311696</v>
+        <v>72914.0035750494</v>
       </c>
       <c r="T13">
-        <v>39.52340588548783</v>
+        <v>151.5883650208927</v>
       </c>
       <c r="U13">
-        <v>1568.532275091016</v>
+        <v>46747.60796001743</v>
       </c>
       <c r="V13">
-        <v>25.33977827287587</v>
+        <v>97.18837413725036</v>
       </c>
       <c r="W13">
-        <v>1024.847869209257</v>
+        <v>30543.95957881934</v>
       </c>
       <c r="X13">
-        <v>16.55650838787168</v>
+        <v>63.50095546532089</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -1587,70 +1737,70 @@
         <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="D14">
-        <v>46350</v>
+        <v>8230</v>
       </c>
       <c r="E14">
-        <v>3.245641701310845</v>
+        <v>8.753508289263223</v>
       </c>
       <c r="F14">
-        <v>-3.847251041198177</v>
+        <v>14.63533513288652</v>
       </c>
       <c r="G14">
-        <v>-2.839361416564969</v>
+        <v>13.36101936106328</v>
       </c>
       <c r="H14">
-        <v>8.279621130351202</v>
+        <v>11.11912785693265</v>
       </c>
       <c r="I14">
-        <v>16.68999999999998</v>
+        <v>11.67999999999998</v>
       </c>
       <c r="J14">
-        <v>2178</v>
+        <v>735</v>
       </c>
       <c r="K14">
-        <v>13056</v>
+        <v>6295</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="M14">
-        <v>21.28099173553719</v>
+        <v>11.19727891156463</v>
       </c>
       <c r="N14">
-        <v>3.550091911764706</v>
+        <v>1.307386814932486</v>
       </c>
       <c r="O14">
-        <v>9788.445939846259</v>
+        <v>22061.40459774504</v>
       </c>
       <c r="P14">
-        <v>-14.40145141454783</v>
+        <v>10.36295807612626</v>
       </c>
       <c r="Q14">
-        <v>6009.256694038851</v>
+        <v>13543.78867428072</v>
       </c>
       <c r="R14">
-        <v>12.96495511119493</v>
+        <v>164.5660835271048</v>
       </c>
       <c r="S14">
-        <v>3773.869646051467</v>
+        <v>8505.626498050413</v>
       </c>
       <c r="T14">
-        <v>8.14211358371406</v>
+        <v>103.3490461488507</v>
       </c>
       <c r="U14">
-        <v>2419.554133030669</v>
+        <v>5453.241812129189</v>
       </c>
       <c r="V14">
-        <v>5.220181516786772</v>
+        <v>66.26053234664872</v>
       </c>
       <c r="W14">
-        <v>1580.888667100614</v>
+        <v>3563.040008927537</v>
       </c>
       <c r="X14">
-        <v>3.410763035815781</v>
+        <v>43.29331724091783</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -1661,70 +1811,70 @@
         <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="D15">
-        <v>2510</v>
+        <v>5100</v>
       </c>
       <c r="E15">
-        <v>-0.1354724601163184</v>
+        <v>10.03245933433847</v>
       </c>
       <c r="F15">
-        <v>-7.255873447235714</v>
+        <v>8.489499228947949</v>
       </c>
       <c r="G15">
-        <v>-12.03146453983929</v>
+        <v>5.808990692691296</v>
       </c>
       <c r="H15">
-        <v>-6.247253650647892</v>
+        <v>5.804327403657638</v>
       </c>
       <c r="I15">
-        <v>4.039999999999964</v>
+        <v>9.419999999999987</v>
       </c>
       <c r="J15">
-        <v>130</v>
+        <v>528</v>
       </c>
       <c r="K15">
-        <v>2494</v>
+        <v>6370</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="M15">
-        <v>19.30769230769231</v>
+        <v>9.659090909090908</v>
       </c>
       <c r="N15">
-        <v>1.006415396952687</v>
+        <v>0.8006279434850864</v>
       </c>
       <c r="O15">
-        <v>692.1019392907139</v>
+        <v>11203.79488308754</v>
       </c>
       <c r="P15">
-        <v>-12.08770160690358</v>
+        <v>8.188100880939597</v>
       </c>
       <c r="Q15">
-        <v>424.8905533318311</v>
+        <v>6878.158168679583</v>
       </c>
       <c r="R15">
-        <v>16.92791049130801</v>
+        <v>134.8658464446977</v>
       </c>
       <c r="S15">
-        <v>266.8352582946997</v>
+        <v>4319.547933319323</v>
       </c>
       <c r="T15">
-        <v>10.63088678464939</v>
+        <v>84.69701830037889</v>
       </c>
       <c r="U15">
-        <v>171.0770144699486</v>
+        <v>2769.406745625659</v>
       </c>
       <c r="V15">
-        <v>6.815817309559703</v>
+        <v>54.30209305148351</v>
       </c>
       <c r="W15">
-        <v>111.7783271243394</v>
+        <v>1809.475423171325</v>
       </c>
       <c r="X15">
-        <v>4.453319805750574</v>
+        <v>35.47991025826128</v>
       </c>
     </row>
     <row r="16" spans="1:24">
@@ -1735,70 +1885,70 @@
         <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D16">
-        <v>17300</v>
+        <v>22000</v>
       </c>
       <c r="E16">
-        <v>12.51383096407281</v>
+        <v>5.825241907004738</v>
       </c>
       <c r="F16">
-        <v>12.73578739073582</v>
+        <v>5.747773299362734</v>
       </c>
       <c r="G16">
-        <v>14.969282939232</v>
+        <v>3.759207507267291</v>
       </c>
       <c r="H16">
-        <v>11.38565937649192</v>
+        <v>7.121663423233443</v>
       </c>
       <c r="I16">
-        <v>15.80999999999996</v>
+        <v>9.810000000000016</v>
       </c>
       <c r="J16">
-        <v>1586</v>
+        <v>1178</v>
       </c>
       <c r="K16">
-        <v>10034</v>
+        <v>12003</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="M16">
-        <v>10.90794451450189</v>
+        <v>18.67572156196944</v>
       </c>
       <c r="N16">
-        <v>1.724137931034483</v>
+        <v>1.832875114554695</v>
       </c>
       <c r="O16">
-        <v>40484.83033276202</v>
+        <v>17360.26164738289</v>
       </c>
       <c r="P16">
-        <v>8.874111049195665</v>
+        <v>-2.340755874146894</v>
       </c>
       <c r="Q16">
-        <v>24854.17390863154</v>
+        <v>10657.69471026369</v>
       </c>
       <c r="R16">
-        <v>143.6657451365985</v>
+        <v>48.44406686483495</v>
       </c>
       <c r="S16">
-        <v>15608.65465848954</v>
+        <v>6693.132380889335</v>
       </c>
       <c r="T16">
-        <v>90.22343733230947</v>
+        <v>30.42332900404243</v>
       </c>
       <c r="U16">
-        <v>10007.23088819738</v>
+        <v>4291.191173507039</v>
       </c>
       <c r="V16">
-        <v>57.84526524969584</v>
+        <v>19.50541442503199</v>
       </c>
       <c r="W16">
-        <v>6538.526121089239</v>
+        <v>2803.779176480808</v>
       </c>
       <c r="X16">
-        <v>37.79494867681641</v>
+        <v>12.74445080218549</v>
       </c>
     </row>
     <row r="17" spans="1:24">
@@ -1809,70 +1959,70 @@
         <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="D17">
-        <v>18000</v>
+        <v>5500</v>
       </c>
       <c r="E17">
-        <v>8.010916726028213</v>
+        <v>11.67346950326535</v>
       </c>
       <c r="F17">
-        <v>7.140539757216771</v>
+        <v>16.1039328701859</v>
       </c>
       <c r="G17">
-        <v>8.631246856550362</v>
+        <v>8.909004525030113</v>
       </c>
       <c r="H17">
-        <v>11.66866476625067</v>
+        <v>8.460523091841907</v>
       </c>
       <c r="I17">
-        <v>12.01999999999997</v>
+        <v>9.200000000000003</v>
       </c>
       <c r="J17">
-        <v>1191</v>
+        <v>547</v>
       </c>
       <c r="K17">
-        <v>9449</v>
+        <v>5948</v>
       </c>
       <c r="L17">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="M17">
-        <v>15.11335012594459</v>
+        <v>10.05484460694698</v>
       </c>
       <c r="N17">
-        <v>1.904963488199809</v>
+        <v>0.9246805648957633</v>
       </c>
       <c r="O17">
-        <v>21623.87351885062</v>
+        <v>13963.96797336251</v>
       </c>
       <c r="P17">
-        <v>1.851187935460796</v>
+        <v>9.765185443834689</v>
       </c>
       <c r="Q17">
-        <v>13275.18254611145</v>
+        <v>8572.665010865941</v>
       </c>
       <c r="R17">
-        <v>73.75101414506361</v>
+        <v>155.866636561199</v>
       </c>
       <c r="S17">
-        <v>8336.939326665804</v>
+        <v>5383.71414593881</v>
       </c>
       <c r="T17">
-        <v>46.3163295925878</v>
+        <v>97.885711744342</v>
       </c>
       <c r="U17">
-        <v>5345.090820973488</v>
+        <v>3451.67931979076</v>
       </c>
       <c r="V17">
-        <v>29.69494900540827</v>
+        <v>62.75780581437744</v>
       </c>
       <c r="W17">
-        <v>3492.37629699827</v>
+        <v>2255.258786993051</v>
       </c>
       <c r="X17">
-        <v>19.40209053887928</v>
+        <v>41.00470521805548</v>
       </c>
     </row>
     <row r="18" spans="1:24">
@@ -1883,70 +2033,70 @@
         <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="D18">
-        <v>9020</v>
+        <v>2980</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>39.19724373085737</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>33.32555038443081</v>
       </c>
       <c r="G18">
-        <v>21.08431887353571</v>
+        <v>21.27892711259751</v>
       </c>
       <c r="H18">
-        <v>11.42332578814282</v>
+        <v>21.58904631415018</v>
       </c>
       <c r="I18">
-        <v>8.379999999999953</v>
+        <v>20.67000000000004</v>
       </c>
       <c r="J18">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="K18">
-        <v>2403</v>
+        <v>870</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="M18">
-        <v>44.87562189054727</v>
+        <v>16.46408839779005</v>
       </c>
       <c r="N18">
-        <v>3.75364128173117</v>
+        <v>3.425287356321839</v>
       </c>
       <c r="O18">
-        <v>16279.19037239439</v>
+        <v>5989.253785547922</v>
       </c>
       <c r="P18">
-        <v>6.082226529518797</v>
+        <v>7.229836846536308</v>
       </c>
       <c r="Q18">
-        <v>9994.010726526041</v>
+        <v>3676.882277767033</v>
       </c>
       <c r="R18">
-        <v>110.7983450834373</v>
+        <v>123.3853113344642</v>
       </c>
       <c r="S18">
-        <v>6276.332605422491</v>
+        <v>2309.116605708419</v>
       </c>
       <c r="T18">
-        <v>69.58240139049325</v>
+        <v>77.4871344197456</v>
       </c>
       <c r="U18">
-        <v>4023.966888102215</v>
+        <v>1480.451936869936</v>
       </c>
       <c r="V18">
-        <v>44.61160629825072</v>
+        <v>49.67959519697771</v>
       </c>
       <c r="W18">
-        <v>2629.180130068321</v>
+        <v>967.2979237101326</v>
       </c>
       <c r="X18">
-        <v>29.14833847082397</v>
+        <v>32.45966186946754</v>
       </c>
     </row>
     <row r="19" spans="1:24">
@@ -1957,70 +2107,70 @@
         <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="D19">
-        <v>12200</v>
+        <v>66700</v>
       </c>
       <c r="E19">
-        <v>11.11869713005345</v>
+        <v>11.57161556705366</v>
       </c>
       <c r="F19">
-        <v>7.672052723707523</v>
+        <v>12.98780532537563</v>
       </c>
       <c r="G19">
-        <v>4.345699453579428</v>
+        <v>29.39297451711403</v>
       </c>
       <c r="H19">
-        <v>11.1948007007024</v>
+        <v>41.08137332404019</v>
       </c>
       <c r="I19">
-        <v>12.88000000000002</v>
+        <v>28.90000000000003</v>
       </c>
       <c r="J19">
-        <v>530</v>
+        <v>4307</v>
       </c>
       <c r="K19">
-        <v>4115</v>
+        <v>14903</v>
       </c>
       <c r="L19">
-        <v>1.1</v>
+        <v>0.6</v>
       </c>
       <c r="M19">
-        <v>23.0188679245283</v>
+        <v>15.48641745994892</v>
       </c>
       <c r="N19">
-        <v>2.964763061968408</v>
+        <v>4.475608937797759</v>
       </c>
       <c r="O19">
-        <v>6296.734551582196</v>
+        <v>196056.2393309899</v>
       </c>
       <c r="P19">
-        <v>-6.400063206363294</v>
+        <v>11.38468561879398</v>
       </c>
       <c r="Q19">
-        <v>3865.648795244339</v>
+        <v>120361.5237646538</v>
       </c>
       <c r="R19">
-        <v>31.68564586265852</v>
+        <v>180.4520596171721</v>
       </c>
       <c r="S19">
-        <v>2427.663751681585</v>
+        <v>75588.16742485332</v>
       </c>
       <c r="T19">
-        <v>19.8988832105048</v>
+        <v>113.3255883431084</v>
       </c>
       <c r="U19">
-        <v>1556.456479660244</v>
+        <v>48462.10390238895</v>
       </c>
       <c r="V19">
-        <v>12.75783999721511</v>
+        <v>72.65682743986349</v>
       </c>
       <c r="W19">
-        <v>1016.957784055914</v>
+        <v>31664.17721234264</v>
       </c>
       <c r="X19">
-        <v>8.33571954144192</v>
+        <v>47.47252955373709</v>
       </c>
     </row>
     <row r="20" spans="1:24">
@@ -2031,70 +2181,70 @@
         <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="D20">
-        <v>43350</v>
+        <v>39850</v>
       </c>
       <c r="E20">
-        <v>10.32497616399473</v>
+        <v>8.003743285250167</v>
       </c>
       <c r="F20">
-        <v>0.6600709489047745</v>
+        <v>9.637970928865741</v>
       </c>
       <c r="G20">
-        <v>1.755630050070565</v>
+        <v>9.940922606544959</v>
       </c>
       <c r="H20">
-        <v>28.27399615653999</v>
+        <v>10.53175146909021</v>
       </c>
       <c r="I20">
-        <v>38.12000000000003</v>
+        <v>11.79999999999998</v>
       </c>
       <c r="J20">
-        <v>4572</v>
+        <v>3006</v>
       </c>
       <c r="K20">
-        <v>11881</v>
+        <v>25487</v>
       </c>
       <c r="L20">
-        <v>2.3</v>
+        <v>1.5</v>
       </c>
       <c r="M20">
-        <v>9.481627296587927</v>
+        <v>13.25681969394544</v>
       </c>
       <c r="N20">
-        <v>3.648682770810538</v>
+        <v>1.563542197983286</v>
       </c>
       <c r="O20">
-        <v>14139.61136631557</v>
+        <v>65752.53342123679</v>
       </c>
       <c r="P20">
-        <v>-10.59849350568524</v>
+        <v>5.135265675195444</v>
       </c>
       <c r="Q20">
-        <v>8680.494817696692</v>
+        <v>40366.35172117898</v>
       </c>
       <c r="R20">
-        <v>20.02420949872362</v>
+        <v>101.2957383216537</v>
       </c>
       <c r="S20">
-        <v>5451.432277424497</v>
+        <v>25350.44802354883</v>
       </c>
       <c r="T20">
-        <v>12.57539164342444</v>
+        <v>63.61467509046131</v>
       </c>
       <c r="U20">
-        <v>3495.095680260109</v>
+        <v>16253.02065049658</v>
       </c>
       <c r="V20">
-        <v>8.062504452733815</v>
+        <v>40.78549724089481</v>
       </c>
       <c r="W20">
-        <v>2283.626175552685</v>
+        <v>10619.40123668091</v>
       </c>
       <c r="X20">
-        <v>5.267880451101926</v>
+        <v>26.64843472190945</v>
       </c>
     </row>
     <row r="21" spans="1:24">
@@ -2105,70 +2255,70 @@
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="D21">
-        <v>23900</v>
+        <v>4220</v>
       </c>
       <c r="E21">
-        <v>8.741483856132689</v>
+        <v>7.527198037421655</v>
       </c>
       <c r="F21">
-        <v>7.460271512345912</v>
+        <v>-1.464164464733344</v>
       </c>
       <c r="G21">
-        <v>9.203214946692526</v>
+        <v>-15.31744609928846</v>
       </c>
       <c r="H21">
-        <v>10.0466953627209</v>
+        <v>-19.82504108442026</v>
       </c>
       <c r="I21">
-        <v>11.63999999999999</v>
+        <v>-3.720000000000027</v>
       </c>
       <c r="J21">
-        <v>1001</v>
+        <v>-86</v>
       </c>
       <c r="K21">
-        <v>8602</v>
+        <v>2318</v>
       </c>
       <c r="L21">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="M21">
-        <v>23.87612387612388</v>
+        <v>-49.06976744186046</v>
       </c>
       <c r="N21">
-        <v>2.778423622413392</v>
+        <v>1.82053494391717</v>
       </c>
       <c r="O21">
-        <v>20746.92228980272</v>
+        <v>439.5951617579238</v>
       </c>
       <c r="P21">
-        <v>-1.404844127100824</v>
+        <v>-20.2420385376653</v>
       </c>
       <c r="Q21">
-        <v>12736.81056389008</v>
+        <v>269.8732959955833</v>
       </c>
       <c r="R21">
-        <v>53.29209440958194</v>
+        <v>6.395101800843205</v>
       </c>
       <c r="S21">
-        <v>7998.836665149406</v>
+        <v>169.4829646814569</v>
       </c>
       <c r="T21">
-        <v>33.46793583744521</v>
+        <v>4.016183997190922</v>
       </c>
       <c r="U21">
-        <v>5128.321889138073</v>
+        <v>108.6612008717265</v>
       </c>
       <c r="V21">
-        <v>21.45741376208399</v>
+        <v>2.574909973263661</v>
       </c>
       <c r="W21">
-        <v>3350.743777584922</v>
+        <v>70.99707283526953</v>
       </c>
       <c r="X21">
-        <v>14.01984844177792</v>
+        <v>1.682395090883164</v>
       </c>
     </row>
     <row r="22" spans="1:24">
@@ -2179,70 +2329,70 @@
         <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D22">
-        <v>48450</v>
+        <v>10450</v>
       </c>
       <c r="E22">
-        <v>13.76126028758577</v>
+        <v>4.763907634449509</v>
       </c>
       <c r="F22">
-        <v>16.66606638243547</v>
+        <v>9.30689726518024</v>
       </c>
       <c r="G22">
-        <v>13.78973793185716</v>
+        <v>11.83297375633879</v>
       </c>
       <c r="H22">
-        <v>9.514113381344245</v>
+        <v>7.163996652458891</v>
       </c>
       <c r="I22">
-        <v>9.949999999999974</v>
+        <v>6.889999999999972</v>
       </c>
       <c r="J22">
-        <v>2124</v>
+        <v>842</v>
       </c>
       <c r="K22">
-        <v>20879</v>
+        <v>12221</v>
       </c>
       <c r="L22">
-        <v>0.5</v>
+        <v>1.4</v>
       </c>
       <c r="M22">
-        <v>22.81073446327684</v>
+        <v>12.41092636579572</v>
       </c>
       <c r="N22">
-        <v>2.320513434551463</v>
+        <v>0.8550855085508551</v>
       </c>
       <c r="O22">
-        <v>75987.2392869766</v>
+        <v>37394.30604425666</v>
       </c>
       <c r="P22">
-        <v>4.603132056512105</v>
+        <v>13.59753793552569</v>
       </c>
       <c r="Q22">
-        <v>46649.573298248</v>
+        <v>22956.86008752848</v>
       </c>
       <c r="R22">
-        <v>96.28394901599175</v>
+        <v>219.6828716509903</v>
       </c>
       <c r="S22">
-        <v>29296.37018936988</v>
+        <v>14417.12375823732</v>
       </c>
       <c r="T22">
-        <v>60.46722433306477</v>
+        <v>137.9629067773906</v>
       </c>
       <c r="U22">
-        <v>18782.88341216321</v>
+        <v>9243.300550180695</v>
       </c>
       <c r="V22">
-        <v>38.76756122221509</v>
+        <v>88.4526368438344</v>
       </c>
       <c r="W22">
-        <v>12272.36337323335</v>
+        <v>6039.389194438955</v>
       </c>
       <c r="X22">
-        <v>25.32995536271073</v>
+        <v>57.79319803290866</v>
       </c>
     </row>
     <row r="23" spans="1:24">
@@ -2253,70 +2403,70 @@
         <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="D23">
-        <v>36950</v>
+        <v>36350</v>
       </c>
       <c r="E23">
-        <v>13.25957157769272</v>
+        <v>4.861462892713917</v>
       </c>
       <c r="F23">
-        <v>14.49259047881405</v>
+        <v>4.861462892713917</v>
       </c>
       <c r="G23">
-        <v>11.06073938306021</v>
+        <v>10.40719402213277</v>
       </c>
       <c r="H23">
-        <v>11.72036267095088</v>
+        <v>10.63011322024147</v>
       </c>
       <c r="I23">
-        <v>8.429999999999964</v>
+        <v>12.04000000000001</v>
       </c>
       <c r="J23">
-        <v>961</v>
+        <v>2253</v>
       </c>
       <c r="K23">
-        <v>10956</v>
+        <v>18714</v>
       </c>
       <c r="L23">
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
       <c r="M23">
-        <v>38.44953173777315</v>
+        <v>16.13404349755881</v>
       </c>
       <c r="N23">
-        <v>3.372581234027017</v>
+        <v>1.942396067115528</v>
       </c>
       <c r="O23">
-        <v>31279.34340389993</v>
+        <v>50366.33505369631</v>
       </c>
       <c r="P23">
-        <v>-1.652274920630481</v>
+        <v>3.315050783030626</v>
       </c>
       <c r="Q23">
-        <v>19202.80347770689</v>
+        <v>30920.56062173869</v>
       </c>
       <c r="R23">
-        <v>51.96969818053285</v>
+        <v>85.06344049996888</v>
       </c>
       <c r="S23">
-        <v>12059.54094713549</v>
+        <v>19418.40249311199</v>
       </c>
       <c r="T23">
-        <v>32.63745858494044</v>
+        <v>53.42063959590644</v>
       </c>
       <c r="U23">
-        <v>7731.775306977927</v>
+        <v>12449.78772868335</v>
       </c>
       <c r="V23">
-        <v>20.92496700129344</v>
+        <v>34.24975991384692</v>
       </c>
       <c r="W23">
-        <v>5051.788588858512</v>
+        <v>8134.444300872496</v>
       </c>
       <c r="X23">
-        <v>13.67195829190396</v>
+        <v>22.37811362000686</v>
       </c>
     </row>
     <row r="24" spans="1:24">
@@ -2327,10 +2477,10 @@
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="D24">
-        <v>11950</v>
+        <v>11250</v>
       </c>
       <c r="E24">
         <v>11.01976456805946</v>
@@ -2357,40 +2507,40 @@
         <v>4.1</v>
       </c>
       <c r="M24">
-        <v>19.52614379084967</v>
+        <v>18.38235294117647</v>
       </c>
       <c r="N24">
-        <v>1.011169402606194</v>
+        <v>0.9519377221188018</v>
       </c>
       <c r="O24">
         <v>19549.51155876396</v>
       </c>
       <c r="P24">
-        <v>5.045342296626365</v>
+        <v>5.681346699416046</v>
       </c>
       <c r="Q24">
         <v>12001.70424617346</v>
       </c>
       <c r="R24">
-        <v>100.4326715160959</v>
+        <v>106.6818155215418</v>
       </c>
       <c r="S24">
         <v>7537.182993106501</v>
       </c>
       <c r="T24">
-        <v>63.07266103017992</v>
+        <v>66.99718216094668</v>
       </c>
       <c r="U24">
         <v>4832.340269479088</v>
       </c>
       <c r="V24">
-        <v>40.43799388685429</v>
+        <v>42.95413572870301</v>
       </c>
       <c r="W24">
         <v>3157.35525950995</v>
       </c>
       <c r="X24">
-        <v>26.42138292476946</v>
+        <v>28.06538008453289</v>
       </c>
     </row>
     <row r="25" spans="1:24">
@@ -2401,70 +2551,70 @@
         <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D25">
-        <v>10550</v>
+        <v>6410</v>
       </c>
       <c r="E25">
-        <v>13.24684556536035</v>
+        <v>4.907650159011212</v>
       </c>
       <c r="F25">
-        <v>5.246899430256832</v>
+        <v>6.311045998066092</v>
       </c>
       <c r="G25">
-        <v>2.835992848178577</v>
+        <v>6.109339139414985</v>
       </c>
       <c r="H25">
-        <v>1.287819412956864</v>
+        <v>9.438734374630513</v>
       </c>
       <c r="I25">
-        <v>5.430000000000021</v>
+        <v>13.36</v>
       </c>
       <c r="J25">
-        <v>163</v>
+        <v>468</v>
       </c>
       <c r="K25">
-        <v>3005</v>
+        <v>3507</v>
       </c>
       <c r="L25">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M25">
-        <v>64.7239263803681</v>
+        <v>13.6965811965812</v>
       </c>
       <c r="N25">
-        <v>3.510815307820299</v>
+        <v>1.827773025377816</v>
       </c>
       <c r="O25">
-        <v>3974.622898663406</v>
+        <v>6345.587879201983</v>
       </c>
       <c r="P25">
-        <v>-9.300613999796703</v>
+        <v>-0.1009442340125455</v>
       </c>
       <c r="Q25">
-        <v>2440.073675316055</v>
+        <v>3895.640500549695</v>
       </c>
       <c r="R25">
-        <v>23.12866042953607</v>
+        <v>60.77442278548666</v>
       </c>
       <c r="S25">
-        <v>1532.389186592629</v>
+        <v>2446.498824311696</v>
       </c>
       <c r="T25">
-        <v>14.52501598665999</v>
+        <v>38.16690833559589</v>
       </c>
       <c r="U25">
-        <v>982.4659931513528</v>
+        <v>1568.532275091016</v>
       </c>
       <c r="V25">
-        <v>9.312473868733202</v>
+        <v>24.47008229471164</v>
       </c>
       <c r="W25">
-        <v>641.9237880159619</v>
+        <v>1024.847869209257</v>
       </c>
       <c r="X25">
-        <v>6.084585668397743</v>
+        <v>15.98826629031602</v>
       </c>
     </row>
     <row r="26" spans="1:24">
@@ -2475,70 +2625,70 @@
         <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D26">
-        <v>3080</v>
+        <v>7940</v>
       </c>
       <c r="E26">
-        <v>39.19724373085737</v>
+        <v>-5.62941063390349</v>
       </c>
       <c r="F26">
-        <v>33.32555038443081</v>
+        <v>-20.67834516482944</v>
       </c>
       <c r="G26">
-        <v>21.27892711259751</v>
+        <v>-14.09437256107617</v>
       </c>
       <c r="H26">
-        <v>21.58904631415018</v>
+        <v>-15.08144974910515</v>
       </c>
       <c r="I26">
-        <v>20.67000000000004</v>
+        <v>2.679999999999978</v>
       </c>
       <c r="J26">
-        <v>181</v>
+        <v>43</v>
       </c>
       <c r="K26">
-        <v>870</v>
+        <v>1595</v>
       </c>
       <c r="L26">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="M26">
-        <v>17.01657458563536</v>
+        <v>184.6511627906977</v>
       </c>
       <c r="N26">
-        <v>3.540229885057471</v>
+        <v>4.978056426332288</v>
       </c>
       <c r="O26">
-        <v>5989.253785547922</v>
+        <v>349.1216884400737</v>
       </c>
       <c r="P26">
-        <v>6.876494315215131</v>
+        <v>-26.83293526112881</v>
       </c>
       <c r="Q26">
-        <v>3676.882277767033</v>
+        <v>214.3304316318889</v>
       </c>
       <c r="R26">
-        <v>119.3792947326959</v>
+        <v>2.699375713247971</v>
       </c>
       <c r="S26">
-        <v>2309.116605708419</v>
+        <v>134.601524172378</v>
       </c>
       <c r="T26">
-        <v>74.97131836715647</v>
+        <v>1.695233301919119</v>
       </c>
       <c r="U26">
-        <v>1480.451936869936</v>
+        <v>86.29754195782922</v>
       </c>
       <c r="V26">
-        <v>48.06662132694596</v>
+        <v>1.086870805514222</v>
       </c>
       <c r="W26">
-        <v>967.2979237101326</v>
+        <v>56.38510179100124</v>
       </c>
       <c r="X26">
-        <v>31.40577674383547</v>
+        <v>0.7101398210453557</v>
       </c>
     </row>
     <row r="27" spans="1:24">
@@ -2549,70 +2699,70 @@
         <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="D27">
-        <v>29850</v>
+        <v>143500</v>
       </c>
       <c r="E27">
-        <v>25.18787091785846</v>
+        <v>7.830830248293978</v>
       </c>
       <c r="F27">
-        <v>22.63709255896887</v>
+        <v>5.673093905494596</v>
       </c>
       <c r="G27">
-        <v>16.54584517318082</v>
+        <v>7.184947541800824</v>
       </c>
       <c r="H27">
-        <v>25.01326749741341</v>
+        <v>14.26640113409157</v>
       </c>
       <c r="I27">
-        <v>31.53999999999999</v>
+        <v>13.46000000000001</v>
       </c>
       <c r="J27">
-        <v>2004</v>
+        <v>9308</v>
       </c>
       <c r="K27">
-        <v>6354</v>
+        <v>69165</v>
       </c>
       <c r="L27">
-        <v>3.4</v>
+        <v>1</v>
       </c>
       <c r="M27">
-        <v>14.89520958083832</v>
+        <v>15.41684572410829</v>
       </c>
       <c r="N27">
-        <v>4.697828139754486</v>
+        <v>2.074748789127449</v>
       </c>
       <c r="O27">
-        <v>29377.52246516888</v>
+        <v>138428.1384477472</v>
       </c>
       <c r="P27">
-        <v>-0.1594227857174779</v>
+        <v>-0.3591903644818872</v>
       </c>
       <c r="Q27">
-        <v>18035.25039755857</v>
+        <v>84982.86885604713</v>
       </c>
       <c r="R27">
-        <v>60.41959932180426</v>
+        <v>59.22151139794225</v>
       </c>
       <c r="S27">
-        <v>11326.30664651117</v>
+        <v>53370.03984675104</v>
       </c>
       <c r="T27">
-        <v>37.9440758677091</v>
+        <v>37.19166539843278</v>
       </c>
       <c r="U27">
-        <v>7261.674257141283</v>
+        <v>34217.31872120335</v>
       </c>
       <c r="V27">
-        <v>24.32721694184685</v>
+        <v>23.84482140850408</v>
       </c>
       <c r="W27">
-        <v>4744.63388959664</v>
+        <v>22356.91718835968</v>
       </c>
       <c r="X27">
-        <v>15.89492090317132</v>
+        <v>15.5797332323064</v>
       </c>
     </row>
     <row r="28" spans="1:24">
@@ -2623,70 +2773,70 @@
         <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="D28">
-        <v>48650</v>
+        <v>6790</v>
       </c>
       <c r="E28">
-        <v>24.07530428025683</v>
+        <v>16.00472807946176</v>
       </c>
       <c r="F28">
-        <v>24.07530428025683</v>
+        <v>8.790483559269205</v>
       </c>
       <c r="G28">
-        <v>26.05208807369344</v>
+        <v>7.908283717566206</v>
       </c>
       <c r="H28">
-        <v>25.52748725977094</v>
+        <v>6.748555312217832</v>
       </c>
       <c r="I28">
-        <v>21.96999999999994</v>
+        <v>4.929999999999964</v>
       </c>
       <c r="J28">
-        <v>4102</v>
+        <v>315</v>
       </c>
       <c r="K28">
-        <v>18674</v>
+        <v>6389</v>
       </c>
       <c r="L28">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="M28">
-        <v>11.86006825938567</v>
+        <v>21.55555555555556</v>
       </c>
       <c r="N28">
-        <v>2.605226518153582</v>
+        <v>1.06276412584129</v>
       </c>
       <c r="O28">
-        <v>189120.147008489</v>
+        <v>13676.68169548652</v>
       </c>
       <c r="P28">
-        <v>14.5421933834077</v>
+        <v>7.253406924150685</v>
       </c>
       <c r="Q28">
-        <v>116103.3647600882</v>
+        <v>8396.296157317476</v>
       </c>
       <c r="R28">
-        <v>238.6502872766457</v>
+        <v>123.6567917130703</v>
       </c>
       <c r="S28">
-        <v>72914.0035750494</v>
+        <v>5272.952849358534</v>
       </c>
       <c r="T28">
-        <v>149.8746219425476</v>
+        <v>77.65762664740109</v>
       </c>
       <c r="U28">
-        <v>46747.60796001743</v>
+        <v>3380.666545621138</v>
       </c>
       <c r="V28">
-        <v>96.08963609458876</v>
+        <v>49.78890347011985</v>
       </c>
       <c r="W28">
-        <v>30543.95957881934</v>
+        <v>2208.860449228435</v>
       </c>
       <c r="X28">
-        <v>62.78306182696679</v>
+        <v>32.53108172648652</v>
       </c>
     </row>
     <row r="29" spans="1:24">
@@ -2697,70 +2847,70 @@
         <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="D29">
-        <v>83900</v>
+        <v>4350</v>
       </c>
       <c r="E29">
-        <v>7.118929602918357</v>
+        <v>13.61023543555848</v>
       </c>
       <c r="F29">
-        <v>7.118929602918357</v>
+        <v>-3.31800189359133</v>
       </c>
       <c r="G29">
-        <v>8.359150513787284</v>
+        <v>-11.7636537790312</v>
       </c>
       <c r="H29">
-        <v>8.359150513787284</v>
+        <v>-13.13740660872928</v>
       </c>
       <c r="I29">
-        <v>6.930000000000007</v>
+        <v>8.909999999999968</v>
       </c>
       <c r="J29">
-        <v>1063</v>
+        <v>77</v>
       </c>
       <c r="K29">
-        <v>15325</v>
+        <v>863</v>
       </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
-        <v>78.92756349952964</v>
+        <v>56.49350649350649</v>
       </c>
       <c r="N29">
-        <v>5.474714518760195</v>
+        <v>5.040556199304751</v>
       </c>
       <c r="O29">
-        <v>34202.38570145993</v>
+        <v>246.8800273034721</v>
       </c>
       <c r="P29">
-        <v>-8.582478213046318</v>
+        <v>-24.94153647794843</v>
       </c>
       <c r="Q29">
-        <v>20997.29788483921</v>
+        <v>151.562920796106</v>
       </c>
       <c r="R29">
-        <v>25.02657673997522</v>
+        <v>3.484205075772552</v>
       </c>
       <c r="S29">
-        <v>13186.50028967843</v>
+        <v>95.18293782103318</v>
       </c>
       <c r="T29">
-        <v>15.71692525587417</v>
+        <v>2.1881135131272</v>
       </c>
       <c r="U29">
-        <v>8454.306658282081</v>
+        <v>61.02496699636698</v>
       </c>
       <c r="V29">
-        <v>10.07664679175457</v>
+        <v>1.402872804514183</v>
       </c>
       <c r="W29">
-        <v>5523.876238937614</v>
+        <v>39.87250271350831</v>
       </c>
       <c r="X29">
-        <v>6.583881095277253</v>
+        <v>0.9166092577818002</v>
       </c>
     </row>
     <row r="30" spans="1:24">
@@ -2771,70 +2921,1920 @@
         <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="D30">
-        <v>39050</v>
+        <v>16450</v>
       </c>
       <c r="E30">
-        <v>4.861462892713917</v>
+        <v>8.010916726028213</v>
       </c>
       <c r="F30">
-        <v>4.861462892713917</v>
+        <v>7.140539757216771</v>
       </c>
       <c r="G30">
-        <v>10.40719402213277</v>
+        <v>8.631246856550362</v>
       </c>
       <c r="H30">
-        <v>10.63011322024147</v>
+        <v>11.66866476625067</v>
       </c>
       <c r="I30">
-        <v>12.04000000000001</v>
+        <v>12.01999999999997</v>
       </c>
       <c r="J30">
-        <v>2253</v>
+        <v>1191</v>
       </c>
       <c r="K30">
-        <v>18714</v>
+        <v>9449</v>
       </c>
       <c r="L30">
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
       <c r="M30">
-        <v>17.33244562805149</v>
+        <v>13.81192275398825</v>
       </c>
       <c r="N30">
-        <v>2.086673078978305</v>
+        <v>1.740924965604826</v>
       </c>
       <c r="O30">
-        <v>50366.33505369631</v>
+        <v>21623.87351885062</v>
       </c>
       <c r="P30">
-        <v>2.577457694898011</v>
+        <v>2.772461639693957</v>
       </c>
       <c r="Q30">
-        <v>30920.56062173869</v>
+        <v>13275.18254611145</v>
       </c>
       <c r="R30">
-        <v>79.18197342314645</v>
+        <v>80.70019784870182</v>
       </c>
       <c r="S30">
-        <v>19418.40249311199</v>
+        <v>8336.939326665804</v>
       </c>
       <c r="T30">
-        <v>49.72702302973621</v>
+        <v>50.68048222897146</v>
       </c>
       <c r="U30">
-        <v>12449.78772868335</v>
+        <v>5345.090820973488</v>
       </c>
       <c r="V30">
-        <v>31.88165871621857</v>
+        <v>32.49295331898777</v>
       </c>
       <c r="W30">
-        <v>8134.444300872496</v>
+        <v>3492.37629699827</v>
       </c>
       <c r="X30">
-        <v>20.83084328008322</v>
+        <v>21.23025104558219</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31">
+        <v>41350</v>
+      </c>
+      <c r="E31">
+        <v>3.245641701310845</v>
+      </c>
+      <c r="F31">
+        <v>-3.847251041198177</v>
+      </c>
+      <c r="G31">
+        <v>-2.839361416564969</v>
+      </c>
+      <c r="H31">
+        <v>8.279621130351202</v>
+      </c>
+      <c r="I31">
+        <v>16.68999999999998</v>
+      </c>
+      <c r="J31">
+        <v>2178</v>
+      </c>
+      <c r="K31">
+        <v>13056</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>18.98530762167126</v>
+      </c>
+      <c r="N31">
+        <v>3.167126225490196</v>
+      </c>
+      <c r="O31">
+        <v>9788.445939846259</v>
+      </c>
+      <c r="P31">
+        <v>-13.41875564018973</v>
+      </c>
+      <c r="Q31">
+        <v>6009.256694038851</v>
+      </c>
+      <c r="R31">
+        <v>14.53266431448331</v>
+      </c>
+      <c r="S31">
+        <v>3773.869646051467</v>
+      </c>
+      <c r="T31">
+        <v>9.126649688153488</v>
+      </c>
+      <c r="U31">
+        <v>2419.554133030669</v>
+      </c>
+      <c r="V31">
+        <v>5.851400563556635</v>
+      </c>
+      <c r="W31">
+        <v>1580.888667100614</v>
+      </c>
+      <c r="X31">
+        <v>3.823189037728209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32">
+        <v>3815</v>
+      </c>
+      <c r="E32">
+        <v>7.40278118335462</v>
+      </c>
+      <c r="F32">
+        <v>1.759180402786711</v>
+      </c>
+      <c r="G32">
+        <v>7.292597363726841</v>
+      </c>
+      <c r="H32">
+        <v>12.45842177154051</v>
+      </c>
+      <c r="I32">
+        <v>13.45000000000002</v>
+      </c>
+      <c r="J32">
+        <v>154</v>
+      </c>
+      <c r="K32">
+        <v>1145</v>
+      </c>
+      <c r="L32">
+        <v>0.5</v>
+      </c>
+      <c r="M32">
+        <v>24.77272727272727</v>
+      </c>
+      <c r="N32">
+        <v>3.331877729257642</v>
+      </c>
+      <c r="O32">
+        <v>2314.744579978288</v>
+      </c>
+      <c r="P32">
+        <v>-4.873645580114694</v>
+      </c>
+      <c r="Q32">
+        <v>1421.052376210308</v>
+      </c>
+      <c r="R32">
+        <v>37.24907932399235</v>
+      </c>
+      <c r="S32">
+        <v>892.4342395540081</v>
+      </c>
+      <c r="T32">
+        <v>23.39277167900414</v>
+      </c>
+      <c r="U32">
+        <v>572.1694587491148</v>
+      </c>
+      <c r="V32">
+        <v>14.99788882697549</v>
+      </c>
+      <c r="W32">
+        <v>373.8441726305046</v>
+      </c>
+      <c r="X32">
+        <v>9.799323004731445</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33">
+        <v>8390</v>
+      </c>
+      <c r="E33">
+        <v>13.5933167707806</v>
+      </c>
+      <c r="F33">
+        <v>12.21742437679663</v>
+      </c>
+      <c r="G33">
+        <v>8.671327916870027</v>
+      </c>
+      <c r="H33">
+        <v>12.49589919685522</v>
+      </c>
+      <c r="I33">
+        <v>14.15999999999998</v>
+      </c>
+      <c r="J33">
+        <v>431</v>
+      </c>
+      <c r="K33">
+        <v>3045</v>
+      </c>
+      <c r="L33">
+        <v>1.5</v>
+      </c>
+      <c r="M33">
+        <v>19.46635730858469</v>
+      </c>
+      <c r="N33">
+        <v>2.755336617405583</v>
+      </c>
+      <c r="O33">
+        <v>6994.183733613721</v>
+      </c>
+      <c r="P33">
+        <v>-1.803161063388903</v>
+      </c>
+      <c r="Q33">
+        <v>4293.822091764654</v>
+      </c>
+      <c r="R33">
+        <v>51.17785568253461</v>
+      </c>
+      <c r="S33">
+        <v>2696.560603531956</v>
+      </c>
+      <c r="T33">
+        <v>32.14017405878374</v>
+      </c>
+      <c r="U33">
+        <v>1728.855250755642</v>
+      </c>
+      <c r="V33">
+        <v>20.60614124857738</v>
+      </c>
+      <c r="W33">
+        <v>1129.599720735962</v>
+      </c>
+      <c r="X33">
+        <v>13.46364387051206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34">
+        <v>30900</v>
+      </c>
+      <c r="E34">
+        <v>1.145208543460924</v>
+      </c>
+      <c r="F34">
+        <v>3.485399252989851</v>
+      </c>
+      <c r="G34">
+        <v>10.86178997558132</v>
+      </c>
+      <c r="H34">
+        <v>15.99093727193822</v>
+      </c>
+      <c r="I34">
+        <v>13.92999999999998</v>
+      </c>
+      <c r="J34">
+        <v>1218</v>
+      </c>
+      <c r="K34">
+        <v>8747</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>25.36945812807882</v>
+      </c>
+      <c r="N34">
+        <v>3.532639762204184</v>
+      </c>
+      <c r="O34">
+        <v>24528.89538028485</v>
+      </c>
+      <c r="P34">
+        <v>-2.282589174755523</v>
+      </c>
+      <c r="Q34">
+        <v>15058.61396867157</v>
+      </c>
+      <c r="R34">
+        <v>48.7333785393902</v>
+      </c>
+      <c r="S34">
+        <v>9456.951010987859</v>
+      </c>
+      <c r="T34">
+        <v>30.60501945303514</v>
+      </c>
+      <c r="U34">
+        <v>6063.167796069704</v>
+      </c>
+      <c r="V34">
+        <v>19.62190225265276</v>
+      </c>
+      <c r="W34">
+        <v>3961.553546036951</v>
+      </c>
+      <c r="X34">
+        <v>12.82056163766004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35">
+        <v>11650</v>
+      </c>
+      <c r="E35">
+        <v>13.24684556536035</v>
+      </c>
+      <c r="F35">
+        <v>5.246899430256832</v>
+      </c>
+      <c r="G35">
+        <v>2.835992848178577</v>
+      </c>
+      <c r="H35">
+        <v>1.287819412956864</v>
+      </c>
+      <c r="I35">
+        <v>5.430000000000021</v>
+      </c>
+      <c r="J35">
+        <v>163</v>
+      </c>
+      <c r="K35">
+        <v>3005</v>
+      </c>
+      <c r="L35">
+        <v>0.5</v>
+      </c>
+      <c r="M35">
+        <v>71.47239263803681</v>
+      </c>
+      <c r="N35">
+        <v>3.876871880199667</v>
+      </c>
+      <c r="O35">
+        <v>3974.622898663406</v>
+      </c>
+      <c r="P35">
+        <v>-10.19572719519685</v>
+      </c>
+      <c r="Q35">
+        <v>2440.073675316055</v>
+      </c>
+      <c r="R35">
+        <v>20.94483841473009</v>
+      </c>
+      <c r="S35">
+        <v>1532.389186592629</v>
+      </c>
+      <c r="T35">
+        <v>13.15355524972214</v>
+      </c>
+      <c r="U35">
+        <v>982.4659931513528</v>
+      </c>
+      <c r="V35">
+        <v>8.433184490569552</v>
+      </c>
+      <c r="W35">
+        <v>641.9237880159619</v>
+      </c>
+      <c r="X35">
+        <v>5.510075433613407</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36">
+        <v>17250</v>
+      </c>
+      <c r="E36">
+        <v>9.811511319139655</v>
+      </c>
+      <c r="F36">
+        <v>9.811511319139655</v>
+      </c>
+      <c r="G36">
+        <v>13.16202353973539</v>
+      </c>
+      <c r="H36">
+        <v>9.152411695708295</v>
+      </c>
+      <c r="I36">
+        <v>14.06999999999999</v>
+      </c>
+      <c r="J36">
+        <v>776</v>
+      </c>
+      <c r="K36">
+        <v>5512</v>
+      </c>
+      <c r="L36">
+        <v>0.3</v>
+      </c>
+      <c r="M36">
+        <v>22.22938144329897</v>
+      </c>
+      <c r="N36">
+        <v>3.129535558780842</v>
+      </c>
+      <c r="O36">
+        <v>18980.87622240321</v>
+      </c>
+      <c r="P36">
+        <v>0.9607843224635815</v>
+      </c>
+      <c r="Q36">
+        <v>11652.61147674999</v>
+      </c>
+      <c r="R36">
+        <v>67.55137087971008</v>
+      </c>
+      <c r="S36">
+        <v>7317.94945504011</v>
+      </c>
+      <c r="T36">
+        <v>42.42289539153688</v>
+      </c>
+      <c r="U36">
+        <v>4691.782310970249</v>
+      </c>
+      <c r="V36">
+        <v>27.19873803461014</v>
+      </c>
+      <c r="W36">
+        <v>3065.517478059244</v>
+      </c>
+      <c r="X36">
+        <v>17.7711158148362</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37">
+        <v>17850</v>
+      </c>
+      <c r="E37">
+        <v>4.310988145912432</v>
+      </c>
+      <c r="F37">
+        <v>4.76951311414723</v>
+      </c>
+      <c r="G37">
+        <v>7.854132035005819</v>
+      </c>
+      <c r="H37">
+        <v>9.67928990222093</v>
+      </c>
+      <c r="I37">
+        <v>9.289999999999978</v>
+      </c>
+      <c r="J37">
+        <v>1070</v>
+      </c>
+      <c r="K37">
+        <v>11519</v>
+      </c>
+      <c r="L37">
+        <v>1.5</v>
+      </c>
+      <c r="M37">
+        <v>16.68224299065421</v>
+      </c>
+      <c r="N37">
+        <v>1.549613681743207</v>
+      </c>
+      <c r="O37">
+        <v>24534.80778105288</v>
+      </c>
+      <c r="P37">
+        <v>3.232024379889409</v>
+      </c>
+      <c r="Q37">
+        <v>15062.24366986331</v>
+      </c>
+      <c r="R37">
+        <v>84.38231747822581</v>
+      </c>
+      <c r="S37">
+        <v>9459.230497428391</v>
+      </c>
+      <c r="T37">
+        <v>52.9928879407753</v>
+      </c>
+      <c r="U37">
+        <v>6064.629251116025</v>
+      </c>
+      <c r="V37">
+        <v>33.97551401185448</v>
+      </c>
+      <c r="W37">
+        <v>3962.508431769269</v>
+      </c>
+      <c r="X37">
+        <v>22.19892678862336</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38">
+        <v>26850</v>
+      </c>
+      <c r="E38">
+        <v>8.741483856132689</v>
+      </c>
+      <c r="F38">
+        <v>7.460271512345912</v>
+      </c>
+      <c r="G38">
+        <v>9.203214946692526</v>
+      </c>
+      <c r="H38">
+        <v>10.0466953627209</v>
+      </c>
+      <c r="I38">
+        <v>11.63999999999999</v>
+      </c>
+      <c r="J38">
+        <v>1001</v>
+      </c>
+      <c r="K38">
+        <v>8602</v>
+      </c>
+      <c r="L38">
+        <v>0.8</v>
+      </c>
+      <c r="M38">
+        <v>26.82317682317682</v>
+      </c>
+      <c r="N38">
+        <v>3.121367123924669</v>
+      </c>
+      <c r="O38">
+        <v>20746.92228980272</v>
+      </c>
+      <c r="P38">
+        <v>-2.545715110347879</v>
+      </c>
+      <c r="Q38">
+        <v>12736.81056389008</v>
+      </c>
+      <c r="R38">
+        <v>47.43691085247703</v>
+      </c>
+      <c r="S38">
+        <v>7998.836665149406</v>
+      </c>
+      <c r="T38">
+        <v>29.79082556852665</v>
+      </c>
+      <c r="U38">
+        <v>5128.321889138073</v>
+      </c>
+      <c r="V38">
+        <v>19.09989530405241</v>
+      </c>
+      <c r="W38">
+        <v>3350.743777584922</v>
+      </c>
+      <c r="X38">
+        <v>12.47949265394757</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39">
+        <v>8220</v>
+      </c>
+      <c r="E39">
+        <v>7.717713294879559</v>
+      </c>
+      <c r="F39">
+        <v>0.1809860916023212</v>
+      </c>
+      <c r="G39">
+        <v>0.1938096902323707</v>
+      </c>
+      <c r="H39">
+        <v>4.881653593222268</v>
+      </c>
+      <c r="I39">
+        <v>8.239999999999952</v>
+      </c>
+      <c r="J39">
+        <v>312</v>
+      </c>
+      <c r="K39">
+        <v>3789</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>26.34615384615385</v>
+      </c>
+      <c r="N39">
+        <v>2.169437846397466</v>
+      </c>
+      <c r="O39">
+        <v>3863.078267138034</v>
+      </c>
+      <c r="P39">
+        <v>-7.273008604933695</v>
+      </c>
+      <c r="Q39">
+        <v>2371.594947661309</v>
+      </c>
+      <c r="R39">
+        <v>28.85152004454147</v>
+      </c>
+      <c r="S39">
+        <v>1489.383902436132</v>
+      </c>
+      <c r="T39">
+        <v>18.1190255770819</v>
+      </c>
+      <c r="U39">
+        <v>954.8938661882819</v>
+      </c>
+      <c r="V39">
+        <v>11.61671370058737</v>
+      </c>
+      <c r="W39">
+        <v>623.9087072832236</v>
+      </c>
+      <c r="X39">
+        <v>7.590130258919996</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40">
+        <v>8370</v>
+      </c>
+      <c r="E40">
+        <v>-1.006587948407372</v>
+      </c>
+      <c r="F40">
+        <v>-17.18868535973797</v>
+      </c>
+      <c r="G40">
+        <v>-8.405360777978018</v>
+      </c>
+      <c r="H40">
+        <v>-14.71293950230449</v>
+      </c>
+      <c r="I40">
+        <v>-9.730000000000032</v>
+      </c>
+      <c r="J40">
+        <v>-316</v>
+      </c>
+      <c r="K40">
+        <v>3251</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>-26.4873417721519</v>
+      </c>
+      <c r="N40">
+        <v>2.574592433097509</v>
+      </c>
+      <c r="O40">
+        <v>1351.193455929799</v>
+      </c>
+      <c r="P40">
+        <v>-16.67041719240293</v>
+      </c>
+      <c r="Q40">
+        <v>829.5155706928456</v>
+      </c>
+      <c r="R40">
+        <v>9.910580295016077</v>
+      </c>
+      <c r="S40">
+        <v>520.9435696548314</v>
+      </c>
+      <c r="T40">
+        <v>6.223937510810411</v>
+      </c>
+      <c r="U40">
+        <v>333.9943573177958</v>
+      </c>
+      <c r="V40">
+        <v>3.990374639400188</v>
+      </c>
+      <c r="W40">
+        <v>218.2252866968874</v>
+      </c>
+      <c r="X40">
+        <v>2.607231621229241</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41">
+        <v>71300</v>
+      </c>
+      <c r="E41">
+        <v>12.77267181963586</v>
+      </c>
+      <c r="F41">
+        <v>6.551581023534737</v>
+      </c>
+      <c r="G41">
+        <v>14.84869244860295</v>
+      </c>
+      <c r="H41">
+        <v>18.6343574974628</v>
+      </c>
+      <c r="I41">
+        <v>17.49999999999999</v>
+      </c>
+      <c r="J41">
+        <v>2476</v>
+      </c>
+      <c r="K41">
+        <v>14151</v>
+      </c>
+      <c r="L41">
+        <v>0.9</v>
+      </c>
+      <c r="M41">
+        <v>28.79644588045234</v>
+      </c>
+      <c r="N41">
+        <v>5.038513179280616</v>
+      </c>
+      <c r="O41">
+        <v>56499.90039173105</v>
+      </c>
+      <c r="P41">
+        <v>-2.29971845607867</v>
+      </c>
+      <c r="Q41">
+        <v>34686.03767421642</v>
+      </c>
+      <c r="R41">
+        <v>48.64801917842416</v>
+      </c>
+      <c r="S41">
+        <v>21783.15744946886</v>
+      </c>
+      <c r="T41">
+        <v>30.5514129726071</v>
+      </c>
+      <c r="U41">
+        <v>13965.91127424473</v>
+      </c>
+      <c r="V41">
+        <v>19.58753334396176</v>
+      </c>
+      <c r="W41">
+        <v>9125.049345984751</v>
+      </c>
+      <c r="X41">
+        <v>12.79810567459292</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42">
+        <v>44950</v>
+      </c>
+      <c r="E42">
+        <v>16.14736166183457</v>
+      </c>
+      <c r="F42">
+        <v>12.80101871493521</v>
+      </c>
+      <c r="G42">
+        <v>7.352942221797221</v>
+      </c>
+      <c r="H42">
+        <v>8.077552133957639</v>
+      </c>
+      <c r="I42">
+        <v>9.249999999999957</v>
+      </c>
+      <c r="J42">
+        <v>1922</v>
+      </c>
+      <c r="K42">
+        <v>20767</v>
+      </c>
+      <c r="L42">
+        <v>0.9</v>
+      </c>
+      <c r="M42">
+        <v>23.38709677419355</v>
+      </c>
+      <c r="N42">
+        <v>2.164491741705591</v>
+      </c>
+      <c r="O42">
+        <v>42219.51882293896</v>
+      </c>
+      <c r="P42">
+        <v>-0.6247216037781889</v>
+      </c>
+      <c r="Q42">
+        <v>25919.12216351578</v>
+      </c>
+      <c r="R42">
+        <v>57.66211827256013</v>
+      </c>
+      <c r="S42">
+        <v>16277.4521651279</v>
+      </c>
+      <c r="T42">
+        <v>36.2123518690276</v>
+      </c>
+      <c r="U42">
+        <v>10436.01935285475</v>
+      </c>
+      <c r="V42">
+        <v>23.21695072937653</v>
+      </c>
+      <c r="W42">
+        <v>6818.687996827573</v>
+      </c>
+      <c r="X42">
+        <v>15.16949498738058</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43">
+        <v>5280</v>
+      </c>
+      <c r="E43">
+        <v>12.8862673598292</v>
+      </c>
+      <c r="F43">
+        <v>4.871333864136218</v>
+      </c>
+      <c r="G43">
+        <v>-1.05315363873919</v>
+      </c>
+      <c r="H43">
+        <v>-0.4678851724109592</v>
+      </c>
+      <c r="I43">
+        <v>-1.579999999999998</v>
+      </c>
+      <c r="J43">
+        <v>-42</v>
+      </c>
+      <c r="K43">
+        <v>2583</v>
+      </c>
+      <c r="L43">
+        <v>2.1</v>
+      </c>
+      <c r="M43">
+        <v>-125.7142857142857</v>
+      </c>
+      <c r="N43">
+        <v>2.044134727061556</v>
+      </c>
+      <c r="O43">
+        <v>2323.506946727759</v>
+      </c>
+      <c r="P43">
+        <v>-7.880620223953771</v>
+      </c>
+      <c r="Q43">
+        <v>1426.431709290194</v>
+      </c>
+      <c r="R43">
+        <v>27.01575206989004</v>
+      </c>
+      <c r="S43">
+        <v>895.8125112537872</v>
+      </c>
+      <c r="T43">
+        <v>16.96614604647324</v>
+      </c>
+      <c r="U43">
+        <v>574.335381799015</v>
+      </c>
+      <c r="V43">
+        <v>10.87756404922377</v>
+      </c>
+      <c r="W43">
+        <v>375.2593437798726</v>
+      </c>
+      <c r="X43">
+        <v>7.107184541285466</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44">
+        <v>46300</v>
+      </c>
+      <c r="E44">
+        <v>13.76126028758577</v>
+      </c>
+      <c r="F44">
+        <v>16.66606638243547</v>
+      </c>
+      <c r="G44">
+        <v>13.78973793185716</v>
+      </c>
+      <c r="H44">
+        <v>9.514113381344245</v>
+      </c>
+      <c r="I44">
+        <v>9.949999999999974</v>
+      </c>
+      <c r="J44">
+        <v>2124</v>
+      </c>
+      <c r="K44">
+        <v>20879</v>
+      </c>
+      <c r="L44">
+        <v>0.5</v>
+      </c>
+      <c r="M44">
+        <v>21.7984934086629</v>
+      </c>
+      <c r="N44">
+        <v>2.21753915417405</v>
+      </c>
+      <c r="O44">
+        <v>75987.2392869766</v>
+      </c>
+      <c r="P44">
+        <v>5.079008813253649</v>
+      </c>
+      <c r="Q44">
+        <v>46649.573298248</v>
+      </c>
+      <c r="R44">
+        <v>100.7550179227819</v>
+      </c>
+      <c r="S44">
+        <v>29296.37018936988</v>
+      </c>
+      <c r="T44">
+        <v>63.27509760123085</v>
+      </c>
+      <c r="U44">
+        <v>18782.88341216321</v>
+      </c>
+      <c r="V44">
+        <v>40.56778274765273</v>
+      </c>
+      <c r="W44">
+        <v>12272.36337323335</v>
+      </c>
+      <c r="X44">
+        <v>26.50618439143271</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45">
+        <v>11850</v>
+      </c>
+      <c r="E45">
+        <v>11.11869713005345</v>
+      </c>
+      <c r="F45">
+        <v>7.672052723707523</v>
+      </c>
+      <c r="G45">
+        <v>4.345699453579428</v>
+      </c>
+      <c r="H45">
+        <v>11.1948007007024</v>
+      </c>
+      <c r="I45">
+        <v>12.88000000000002</v>
+      </c>
+      <c r="J45">
+        <v>530</v>
+      </c>
+      <c r="K45">
+        <v>4115</v>
+      </c>
+      <c r="L45">
+        <v>1.1</v>
+      </c>
+      <c r="M45">
+        <v>22.35849056603774</v>
+      </c>
+      <c r="N45">
+        <v>2.879708383961118</v>
+      </c>
+      <c r="O45">
+        <v>6296.734551582196</v>
+      </c>
+      <c r="P45">
+        <v>-6.127214810571269</v>
+      </c>
+      <c r="Q45">
+        <v>3865.648795244339</v>
+      </c>
+      <c r="R45">
+        <v>32.62150882062733</v>
+      </c>
+      <c r="S45">
+        <v>2427.663751681585</v>
+      </c>
+      <c r="T45">
+        <v>20.48661393824123</v>
+      </c>
+      <c r="U45">
+        <v>1556.456479660244</v>
+      </c>
+      <c r="V45">
+        <v>13.13465383679531</v>
+      </c>
+      <c r="W45">
+        <v>1016.957784055914</v>
+      </c>
+      <c r="X45">
+        <v>8.581922228319952</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" t="s">
+        <v>121</v>
+      </c>
+      <c r="D46">
+        <v>1630</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>-3.324212623918683</v>
+      </c>
+      <c r="I46">
+        <v>-18.23000000000003</v>
+      </c>
+      <c r="J46">
+        <v>-166</v>
+      </c>
+      <c r="K46">
+        <v>787</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>-9.819277108433734</v>
+      </c>
+      <c r="N46">
+        <v>2.071156289707751</v>
+      </c>
+      <c r="O46">
+        <v>787</v>
+      </c>
+      <c r="P46">
+        <v>-7.022318409979034</v>
+      </c>
+      <c r="Q46">
+        <v>483.1497305365775</v>
+      </c>
+      <c r="R46">
+        <v>29.64108776298021</v>
+      </c>
+      <c r="S46">
+        <v>303.4225687810412</v>
+      </c>
+      <c r="T46">
+        <v>18.61488152030928</v>
+      </c>
+      <c r="U46">
+        <v>194.5343637179084</v>
+      </c>
+      <c r="V46">
+        <v>11.93462354097598</v>
+      </c>
+      <c r="W46">
+        <v>127.1048937343086</v>
+      </c>
+      <c r="X46">
+        <v>7.797846241368628</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47">
+        <v>37900</v>
+      </c>
+      <c r="E47">
+        <v>13.25957157769272</v>
+      </c>
+      <c r="F47">
+        <v>14.49259047881405</v>
+      </c>
+      <c r="G47">
+        <v>11.06073938306021</v>
+      </c>
+      <c r="H47">
+        <v>11.72036267095088</v>
+      </c>
+      <c r="I47">
+        <v>8.429999999999964</v>
+      </c>
+      <c r="J47">
+        <v>961</v>
+      </c>
+      <c r="K47">
+        <v>10956</v>
+      </c>
+      <c r="L47">
+        <v>0.8</v>
+      </c>
+      <c r="M47">
+        <v>39.43808532778356</v>
+      </c>
+      <c r="N47">
+        <v>3.45929171230376</v>
+      </c>
+      <c r="O47">
+        <v>31279.34340389993</v>
+      </c>
+      <c r="P47">
+        <v>-1.901618571781194</v>
+      </c>
+      <c r="Q47">
+        <v>19202.80347770689</v>
+      </c>
+      <c r="R47">
+        <v>50.66702764566462</v>
+      </c>
+      <c r="S47">
+        <v>12059.54094713549</v>
+      </c>
+      <c r="T47">
+        <v>31.81936925365565</v>
+      </c>
+      <c r="U47">
+        <v>7731.775306977927</v>
+      </c>
+      <c r="V47">
+        <v>20.40046255139295</v>
+      </c>
+      <c r="W47">
+        <v>5051.788588858512</v>
+      </c>
+      <c r="X47">
+        <v>13.32925749039185</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48">
+        <v>3865</v>
+      </c>
+      <c r="E48">
+        <v>1.322623422257337</v>
+      </c>
+      <c r="F48">
+        <v>-1.576148099845298</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0.001</v>
+      </c>
+      <c r="K48">
+        <v>534</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>3865000</v>
+      </c>
+      <c r="N48">
+        <v>7.237827715355805</v>
+      </c>
+      <c r="O48">
+        <v>534</v>
+      </c>
+      <c r="P48">
+        <v>-17.95744518722007</v>
+      </c>
+      <c r="Q48">
+        <v>327.8296773907654</v>
+      </c>
+      <c r="R48">
+        <v>8.482009764314757</v>
+      </c>
+      <c r="S48">
+        <v>205.8801165553698</v>
+      </c>
+      <c r="T48">
+        <v>5.326781799621469</v>
+      </c>
+      <c r="U48">
+        <v>131.9966330690764</v>
+      </c>
+      <c r="V48">
+        <v>3.415178087168858</v>
+      </c>
+      <c r="W48">
+        <v>86.24398126317766</v>
+      </c>
+      <c r="X48">
+        <v>2.231409605774325</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49">
+        <v>10100</v>
+      </c>
+      <c r="E49">
+        <v>6.786090547831165</v>
+      </c>
+      <c r="F49">
+        <v>8.063858202242528</v>
+      </c>
+      <c r="G49">
+        <v>6.805380515713665</v>
+      </c>
+      <c r="H49">
+        <v>6.188691576477694</v>
+      </c>
+      <c r="I49">
+        <v>5.640000000000015</v>
+      </c>
+      <c r="J49">
+        <v>207</v>
+      </c>
+      <c r="K49">
+        <v>3664</v>
+      </c>
+      <c r="L49">
+        <v>1.2</v>
+      </c>
+      <c r="M49">
+        <v>48.79227053140097</v>
+      </c>
+      <c r="N49">
+        <v>2.756550218340611</v>
+      </c>
+      <c r="O49">
+        <v>7077.612498493862</v>
+      </c>
+      <c r="P49">
+        <v>-3.493505469534608</v>
+      </c>
+      <c r="Q49">
+        <v>4345.040116251108</v>
+      </c>
+      <c r="R49">
+        <v>43.02019917080305</v>
+      </c>
+      <c r="S49">
+        <v>2728.726003976888</v>
+      </c>
+      <c r="T49">
+        <v>27.01708914828602</v>
+      </c>
+      <c r="U49">
+        <v>1749.47756548465</v>
+      </c>
+      <c r="V49">
+        <v>17.32156005430347</v>
+      </c>
+      <c r="W49">
+        <v>1143.073932037709</v>
+      </c>
+      <c r="X49">
+        <v>11.31756368354167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" t="s">
+        <v>125</v>
+      </c>
+      <c r="D50">
+        <v>8190</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>21.08431887353571</v>
+      </c>
+      <c r="H50">
+        <v>11.42332578814282</v>
+      </c>
+      <c r="I50">
+        <v>8.379999999999953</v>
+      </c>
+      <c r="J50">
+        <v>201</v>
+      </c>
+      <c r="K50">
+        <v>2403</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>40.74626865671642</v>
+      </c>
+      <c r="N50">
+        <v>3.408239700374532</v>
+      </c>
+      <c r="O50">
+        <v>16279.19037239439</v>
+      </c>
+      <c r="P50">
+        <v>7.11120126855298</v>
+      </c>
+      <c r="Q50">
+        <v>9994.010726526041</v>
+      </c>
+      <c r="R50">
+        <v>122.026992997876</v>
+      </c>
+      <c r="S50">
+        <v>6276.332605422491</v>
+      </c>
+      <c r="T50">
+        <v>76.63409774630637</v>
+      </c>
+      <c r="U50">
+        <v>4023.966888102215</v>
+      </c>
+      <c r="V50">
+        <v>49.13268483641288</v>
+      </c>
+      <c r="W50">
+        <v>2629.180130068321</v>
+      </c>
+      <c r="X50">
+        <v>32.10232149045569</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51">
+        <v>12100</v>
+      </c>
+      <c r="E51">
+        <v>9.74245714093901</v>
+      </c>
+      <c r="F51">
+        <v>7.851392924021297</v>
+      </c>
+      <c r="G51">
+        <v>4.626642257435066</v>
+      </c>
+      <c r="H51">
+        <v>4.981607558663327</v>
+      </c>
+      <c r="I51">
+        <v>3.709999999999994</v>
+      </c>
+      <c r="J51">
+        <v>180</v>
+      </c>
+      <c r="K51">
+        <v>4426</v>
+      </c>
+      <c r="L51">
+        <v>0.4</v>
+      </c>
+      <c r="M51">
+        <v>67.22222222222223</v>
+      </c>
+      <c r="N51">
+        <v>2.733845458653412</v>
+      </c>
+      <c r="O51">
+        <v>6957.196800549079</v>
+      </c>
+      <c r="P51">
+        <v>-5.383932893903831</v>
+      </c>
+      <c r="Q51">
+        <v>4271.115323348445</v>
+      </c>
+      <c r="R51">
+        <v>35.29847374668137</v>
+      </c>
+      <c r="S51">
+        <v>2682.300539692304</v>
+      </c>
+      <c r="T51">
+        <v>22.16777305530829</v>
+      </c>
+      <c r="U51">
+        <v>1719.712646575709</v>
+      </c>
+      <c r="V51">
+        <v>14.2125012113695</v>
+      </c>
+      <c r="W51">
+        <v>1123.626124552049</v>
+      </c>
+      <c r="X51">
+        <v>9.286166318611979</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52" t="s">
+        <v>127</v>
+      </c>
+      <c r="D52">
+        <v>9000</v>
+      </c>
+      <c r="E52">
+        <v>-5.09734733799533</v>
+      </c>
+      <c r="F52">
+        <v>-5.09734733799533</v>
+      </c>
+      <c r="G52">
+        <v>-17.93077931195371</v>
+      </c>
+      <c r="H52">
+        <v>-10.90209775125378</v>
+      </c>
+      <c r="I52">
+        <v>-0.04000000000004889</v>
+      </c>
+      <c r="J52">
+        <v>-1</v>
+      </c>
+      <c r="K52">
+        <v>2283</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <v>-9000</v>
+      </c>
+      <c r="N52">
+        <v>3.942181340341656</v>
+      </c>
+      <c r="O52">
+        <v>316.4528462940438</v>
+      </c>
+      <c r="P52">
+        <v>-28.45049233979544</v>
+      </c>
+      <c r="Q52">
+        <v>194.2745964606102</v>
+      </c>
+      <c r="R52">
+        <v>2.158606627340113</v>
+      </c>
+      <c r="S52">
+        <v>122.0062713095435</v>
+      </c>
+      <c r="T52">
+        <v>1.355625236772706</v>
+      </c>
+      <c r="U52">
+        <v>78.22230381262119</v>
+      </c>
+      <c r="V52">
+        <v>0.8691367090291243</v>
+      </c>
+      <c r="W52">
+        <v>51.10890139787031</v>
+      </c>
+      <c r="X52">
+        <v>0.567876682198559</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53">
+        <v>37300</v>
+      </c>
+      <c r="E53">
+        <v>8.231231343791805</v>
+      </c>
+      <c r="F53">
+        <v>8.231231343791805</v>
+      </c>
+      <c r="G53">
+        <v>11.05921434618064</v>
+      </c>
+      <c r="H53">
+        <v>11.9397700792331</v>
+      </c>
+      <c r="I53">
+        <v>10.35999999999996</v>
+      </c>
+      <c r="J53">
+        <v>663</v>
+      </c>
+      <c r="K53">
+        <v>6398</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>56.25942684766214</v>
+      </c>
+      <c r="N53">
+        <v>5.829946858393248</v>
+      </c>
+      <c r="O53">
+        <v>18263.76054077786</v>
+      </c>
+      <c r="P53">
+        <v>-6.891755736623184</v>
+      </c>
+      <c r="Q53">
+        <v>11212.36465547827</v>
+      </c>
+      <c r="R53">
+        <v>30.05995886187205</v>
+      </c>
+      <c r="S53">
+        <v>7041.470316244775</v>
+      </c>
+      <c r="T53">
+        <v>18.87793650467768</v>
+      </c>
+      <c r="U53">
+        <v>4514.522281952306</v>
+      </c>
+      <c r="V53">
+        <v>12.10327689531449</v>
+      </c>
+      <c r="W53">
+        <v>2949.699291898894</v>
+      </c>
+      <c r="X53">
+        <v>7.908040997047973</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>75</v>
+      </c>
+      <c r="C54" t="s">
+        <v>129</v>
+      </c>
+      <c r="D54">
+        <v>43200</v>
+      </c>
+      <c r="E54">
+        <v>7.454602486441559</v>
+      </c>
+      <c r="F54">
+        <v>8.604000010079204</v>
+      </c>
+      <c r="G54">
+        <v>7.033945590327164</v>
+      </c>
+      <c r="H54">
+        <v>5.843754278958158</v>
+      </c>
+      <c r="I54">
+        <v>7.189999999999998</v>
+      </c>
+      <c r="J54">
+        <v>520</v>
+      </c>
+      <c r="K54">
+        <v>7242</v>
+      </c>
+      <c r="L54">
+        <v>0.1</v>
+      </c>
+      <c r="M54">
+        <v>83.07692307692308</v>
+      </c>
+      <c r="N54">
+        <v>5.965202982601491</v>
+      </c>
+      <c r="O54">
+        <v>14291.37027792688</v>
+      </c>
+      <c r="P54">
+        <v>-10.47197325345388</v>
+      </c>
+      <c r="Q54">
+        <v>8773.661624877792</v>
+      </c>
+      <c r="R54">
+        <v>20.30940190943933</v>
+      </c>
+      <c r="S54">
+        <v>5509.941907407365</v>
+      </c>
+      <c r="T54">
+        <v>12.75449515603557</v>
+      </c>
+      <c r="U54">
+        <v>3532.608162228124</v>
+      </c>
+      <c r="V54">
+        <v>8.177333708861397</v>
+      </c>
+      <c r="W54">
+        <v>2308.136087031198</v>
+      </c>
+      <c r="X54">
+        <v>5.342907608868513</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" t="s">
+        <v>130</v>
+      </c>
+      <c r="D55">
+        <v>80700</v>
+      </c>
+      <c r="E55">
+        <v>7.118929602918357</v>
+      </c>
+      <c r="F55">
+        <v>7.118929602918357</v>
+      </c>
+      <c r="G55">
+        <v>8.359150513787284</v>
+      </c>
+      <c r="H55">
+        <v>8.359150513787284</v>
+      </c>
+      <c r="I55">
+        <v>6.930000000000007</v>
+      </c>
+      <c r="J55">
+        <v>1063</v>
+      </c>
+      <c r="K55">
+        <v>15325</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>75.91721542803387</v>
+      </c>
+      <c r="N55">
+        <v>5.265905383360522</v>
+      </c>
+      <c r="O55">
+        <v>34202.38570145993</v>
+      </c>
+      <c r="P55">
+        <v>-8.226290441365759</v>
+      </c>
+      <c r="Q55">
+        <v>20997.29788483921</v>
+      </c>
+      <c r="R55">
+        <v>26.0189564867896</v>
+      </c>
+      <c r="S55">
+        <v>13186.50028967843</v>
+      </c>
+      <c r="T55">
+        <v>16.34014905784192</v>
+      </c>
+      <c r="U55">
+        <v>8454.306658282081</v>
+      </c>
+      <c r="V55">
+        <v>10.47621642909799</v>
+      </c>
+      <c r="W55">
+        <v>5523.876238937614</v>
+      </c>
+      <c r="X55">
+        <v>6.844951968943761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
time and folder add
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\python\stock1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView minimized="1" xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="today" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -412,12 +417,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -425,8 +430,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -472,15 +484,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -522,7 +542,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -554,9 +574,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,6 +609,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -763,14 +785,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -841,7 +863,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -858,16 +880,16 @@
         <v>10.32497616399473</v>
       </c>
       <c r="F2">
-        <v>0.6600709489047745</v>
+        <v>0.66007094890477447</v>
       </c>
       <c r="G2">
-        <v>1.755630050070565</v>
+        <v>1.7556300500705651</v>
       </c>
       <c r="H2">
         <v>28.27399615653999</v>
       </c>
       <c r="I2">
-        <v>38.12000000000003</v>
+        <v>38.120000000000033</v>
       </c>
       <c r="J2">
         <v>4572</v>
@@ -876,7 +898,7 @@
         <v>11881</v>
       </c>
       <c r="L2">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="M2">
         <v>8.683289588801399</v>
@@ -891,13 +913,13 @@
         <v>-9.808689657847081</v>
       </c>
       <c r="Q2">
-        <v>8680.494817696692</v>
+        <v>8680.4948176966918</v>
       </c>
       <c r="R2">
-        <v>21.8652262410496</v>
+        <v>21.865226241049601</v>
       </c>
       <c r="S2">
-        <v>5451.432277424497</v>
+        <v>5451.4322774244974</v>
       </c>
       <c r="T2">
         <v>13.73156744943198</v>
@@ -906,16 +928,16 @@
         <v>3495.095680260109</v>
       </c>
       <c r="V2">
-        <v>8.803767456574581</v>
+        <v>8.8037674565745814</v>
       </c>
       <c r="W2">
-        <v>2283.626175552685</v>
+        <v>2283.6261755526848</v>
       </c>
       <c r="X2">
-        <v>5.752206991316588</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+        <v>5.7522069913165881</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -929,7 +951,7 @@
         <v>1880</v>
       </c>
       <c r="E3">
-        <v>34.35131625501245</v>
+        <v>34.351316255012449</v>
       </c>
       <c r="F3">
         <v>18.11424148373618</v>
@@ -938,10 +960,10 @@
         <v>11.91931581011643</v>
       </c>
       <c r="H3">
-        <v>12.77337607124542</v>
+        <v>12.773376071245419</v>
       </c>
       <c r="I3">
-        <v>14.76999999999997</v>
+        <v>14.769999999999969</v>
       </c>
       <c r="J3">
         <v>299</v>
@@ -953,19 +975,19 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>6.287625418060201</v>
+        <v>6.2876254180602009</v>
       </c>
       <c r="N3">
-        <v>0.958694543600204</v>
+        <v>0.95869454360020401</v>
       </c>
       <c r="O3">
-        <v>6046.834177686939</v>
+        <v>6046.8341776869393</v>
       </c>
       <c r="P3">
-        <v>12.39241962998265</v>
+        <v>12.392419629982649</v>
       </c>
       <c r="Q3">
-        <v>3712.23164364525</v>
+        <v>3712.2316436452502</v>
       </c>
       <c r="R3">
         <v>197.4591299811303</v>
@@ -980,16 +1002,16 @@
         <v>1494.6849291792</v>
       </c>
       <c r="V3">
-        <v>79.50451750953194</v>
+        <v>79.504517509531937</v>
       </c>
       <c r="W3">
-        <v>976.5974785055705</v>
+        <v>976.59747850557051</v>
       </c>
       <c r="X3">
-        <v>51.94667438859418</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
+        <v>51.946674388594182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1003,19 +1025,19 @@
         <v>28350</v>
       </c>
       <c r="E4">
-        <v>25.18787091785846</v>
+        <v>25.187870917858461</v>
       </c>
       <c r="F4">
         <v>22.63709255896887</v>
       </c>
       <c r="G4">
-        <v>16.54584517318082</v>
+        <v>16.545845173180819</v>
       </c>
       <c r="H4">
-        <v>25.01326749741341</v>
+        <v>25.013267497413409</v>
       </c>
       <c r="I4">
-        <v>31.53999999999999</v>
+        <v>31.539999999999988</v>
       </c>
       <c r="J4">
         <v>2004</v>
@@ -1027,10 +1049,10 @@
         <v>3.4</v>
       </c>
       <c r="M4">
-        <v>14.14670658682635</v>
+        <v>14.146706586826349</v>
       </c>
       <c r="N4">
-        <v>4.461756373937677</v>
+        <v>4.4617563739376767</v>
       </c>
       <c r="O4">
         <v>29377.52246516888</v>
@@ -1039,31 +1061,31 @@
         <v>0.3566626304315923</v>
       </c>
       <c r="Q4">
-        <v>18035.25039755857</v>
+        <v>18035.250397558571</v>
       </c>
       <c r="R4">
-        <v>63.61640351872511</v>
+        <v>63.616403518725107</v>
       </c>
       <c r="S4">
         <v>11326.30664651117</v>
       </c>
       <c r="T4">
-        <v>39.95169892949266</v>
+        <v>39.951698929492657</v>
       </c>
       <c r="U4">
-        <v>7261.674257141283</v>
+        <v>7261.6742571412833</v>
       </c>
       <c r="V4">
-        <v>25.6143712773943</v>
+        <v>25.614371277394302</v>
       </c>
       <c r="W4">
-        <v>4744.63388959664</v>
+        <v>4744.6338895966401</v>
       </c>
       <c r="X4">
-        <v>16.73592200915922</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24">
+        <v>16.735922009159221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1077,19 +1099,19 @@
         <v>13700</v>
       </c>
       <c r="E5">
-        <v>6.784710160772605</v>
+        <v>6.7847101607726046</v>
       </c>
       <c r="F5">
-        <v>3.397155874696452</v>
+        <v>3.3971558746964519</v>
       </c>
       <c r="G5">
-        <v>5.960450358089915</v>
+        <v>5.9604503580899149</v>
       </c>
       <c r="H5">
-        <v>7.723227615342381</v>
+        <v>7.7232276153423811</v>
       </c>
       <c r="I5">
-        <v>9.029999999999959</v>
+        <v>9.0299999999999585</v>
       </c>
       <c r="J5">
         <v>2276</v>
@@ -1101,43 +1123,43 @@
         <v>1.7</v>
       </c>
       <c r="M5">
-        <v>6.019332161687171</v>
+        <v>6.0193321616871707</v>
       </c>
       <c r="N5">
-        <v>0.543542947827812</v>
+        <v>0.54354294782781198</v>
       </c>
       <c r="O5">
-        <v>44970.18318433803</v>
+        <v>44970.183184338028</v>
       </c>
       <c r="P5">
-        <v>12.62126701630899</v>
+        <v>12.621267016308989</v>
       </c>
       <c r="Q5">
         <v>27607.79147102089</v>
       </c>
       <c r="R5">
-        <v>201.5167260658459</v>
+        <v>201.51672606584589</v>
       </c>
       <c r="S5">
-        <v>17337.95235113828</v>
+        <v>17337.952351138279</v>
       </c>
       <c r="T5">
         <v>126.5543967236371</v>
       </c>
       <c r="U5">
-        <v>11115.94151466707</v>
+        <v>11115.941514667071</v>
       </c>
       <c r="V5">
-        <v>81.13825923114649</v>
+        <v>81.138259231146492</v>
       </c>
       <c r="W5">
-        <v>7262.935647849655</v>
+        <v>7262.9356478496547</v>
       </c>
       <c r="X5">
-        <v>53.01412881642084</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
+        <v>53.014128816420843</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1151,7 +1173,7 @@
         <v>7830</v>
       </c>
       <c r="E6">
-        <v>7.766207062970892</v>
+        <v>7.7662070629708921</v>
       </c>
       <c r="F6">
         <v>4.215437490805499</v>
@@ -1163,7 +1185,7 @@
         <v>1.171708580322999</v>
       </c>
       <c r="I6">
-        <v>4.550000000000026</v>
+        <v>4.5500000000000256</v>
       </c>
       <c r="J6">
         <v>537</v>
@@ -1178,7 +1200,7 @@
         <v>14.58100558659218</v>
       </c>
       <c r="N6">
-        <v>0.6630536031840122</v>
+        <v>0.66305360318401219</v>
       </c>
       <c r="O6">
         <v>12815.14189750114</v>
@@ -1187,31 +1209,31 @@
         <v>5.050026362187543</v>
       </c>
       <c r="Q6">
-        <v>7867.385456881421</v>
+        <v>7867.3854568814213</v>
       </c>
       <c r="R6">
-        <v>100.4774643279875</v>
+        <v>100.47746432798751</v>
       </c>
       <c r="S6">
-        <v>4940.791961668796</v>
+        <v>4940.7919616687959</v>
       </c>
       <c r="T6">
-        <v>63.10079133676623</v>
+        <v>63.100791336766228</v>
       </c>
       <c r="U6">
         <v>3167.707083843829</v>
       </c>
       <c r="V6">
-        <v>40.456029167865</v>
+        <v>40.456029167864997</v>
       </c>
       <c r="W6">
-        <v>2069.716961972006</v>
+        <v>2069.7169619720062</v>
       </c>
       <c r="X6">
-        <v>26.43316681956584</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24">
+        <v>26.433166819565841</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1225,19 +1247,19 @@
         <v>14450</v>
       </c>
       <c r="E7">
-        <v>8.191662932123933</v>
+        <v>8.1916629321239327</v>
       </c>
       <c r="F7">
-        <v>9.002955936466662</v>
+        <v>9.0029559364666625</v>
       </c>
       <c r="G7">
-        <v>9.618336740356312</v>
+        <v>9.6183367403563125</v>
       </c>
       <c r="H7">
-        <v>10.10468881870398</v>
+        <v>10.104688818703981</v>
       </c>
       <c r="I7">
-        <v>10.00000000000004</v>
+        <v>10.000000000000041</v>
       </c>
       <c r="J7">
         <v>1490</v>
@@ -1249,16 +1271,16 @@
         <v>0.7</v>
       </c>
       <c r="M7">
-        <v>9.697986577181208</v>
+        <v>9.6979865771812079</v>
       </c>
       <c r="N7">
-        <v>0.9693432615549742</v>
+        <v>0.96934326155497419</v>
       </c>
       <c r="O7">
-        <v>37344.12886514056</v>
+        <v>37344.128865140563</v>
       </c>
       <c r="P7">
-        <v>9.960181645373511</v>
+        <v>9.9601816453735115</v>
       </c>
       <c r="Q7">
         <v>22926.05565224382</v>
@@ -1267,25 +1289,25 @@
         <v>158.6578245830022</v>
       </c>
       <c r="S7">
-        <v>14397.7782835466</v>
+        <v>14397.778283546601</v>
       </c>
       <c r="T7">
-        <v>99.6386040383848</v>
+        <v>99.638604038384798</v>
       </c>
       <c r="U7">
-        <v>9230.897518906857</v>
+        <v>9230.8975189068569</v>
       </c>
       <c r="V7">
-        <v>63.88164372945921</v>
+        <v>63.881643729459213</v>
       </c>
       <c r="W7">
-        <v>6031.285299878041</v>
+        <v>6031.2852998780409</v>
       </c>
       <c r="X7">
-        <v>41.73899861507294</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
+        <v>41.738998615072937</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1302,13 +1324,13 @@
         <v>12.51383096407281</v>
       </c>
       <c r="F8">
-        <v>12.73578739073582</v>
+        <v>12.735787390735821</v>
       </c>
       <c r="G8">
         <v>14.969282939232</v>
       </c>
       <c r="H8">
-        <v>11.38565937649192</v>
+        <v>11.385659376491921</v>
       </c>
       <c r="I8">
         <v>15.80999999999996</v>
@@ -1329,22 +1351,22 @@
         <v>1.634442894159857</v>
       </c>
       <c r="O8">
-        <v>40484.83033276202</v>
+        <v>40484.830332762023</v>
       </c>
       <c r="P8">
-        <v>9.457329341636234</v>
+        <v>9.4573293416362336</v>
       </c>
       <c r="Q8">
-        <v>24854.17390863154</v>
+        <v>24854.173908631539</v>
       </c>
       <c r="R8">
-        <v>151.5498409062899</v>
+        <v>151.54984090628989</v>
       </c>
       <c r="S8">
         <v>15608.65465848954</v>
       </c>
       <c r="T8">
-        <v>95.17472352737524</v>
+        <v>95.174723527375235</v>
       </c>
       <c r="U8">
         <v>10007.23088819738</v>
@@ -1353,13 +1375,13 @@
         <v>61.0197005377889</v>
       </c>
       <c r="W8">
-        <v>6538.526121089239</v>
+        <v>6538.5261210892386</v>
       </c>
       <c r="X8">
-        <v>39.86906171395877</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
+        <v>39.869061713958772</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1373,19 +1395,19 @@
         <v>8340</v>
       </c>
       <c r="E9">
-        <v>12.87673684478015</v>
+        <v>12.876736844780149</v>
       </c>
       <c r="F9">
-        <v>3.839137463505551</v>
+        <v>3.8391374635055509</v>
       </c>
       <c r="G9">
-        <v>12.48736101508194</v>
+        <v>12.487361015081939</v>
       </c>
       <c r="H9">
         <v>18.87827195790587</v>
       </c>
       <c r="I9">
-        <v>21.73999999999999</v>
+        <v>21.739999999999991</v>
       </c>
       <c r="J9">
         <v>703</v>
@@ -1400,40 +1422,40 @@
         <v>11.86344238975818</v>
       </c>
       <c r="N9">
-        <v>2.578052550231839</v>
+        <v>2.5780525502318392</v>
       </c>
       <c r="O9">
         <v>10493.28738518514</v>
       </c>
       <c r="P9">
-        <v>2.323303217970518</v>
+        <v>2.3233032179705182</v>
       </c>
       <c r="Q9">
-        <v>6441.968198977213</v>
+        <v>6441.9681989772134</v>
       </c>
       <c r="R9">
-        <v>77.24182492778432</v>
+        <v>77.241824927784322</v>
       </c>
       <c r="S9">
-        <v>4045.616535413684</v>
+        <v>4045.6165354136838</v>
       </c>
       <c r="T9">
         <v>48.50859155172283</v>
       </c>
       <c r="U9">
-        <v>2593.78015855927</v>
+        <v>2593.7801585592701</v>
       </c>
       <c r="V9">
         <v>31.10048151749724</v>
       </c>
       <c r="W9">
-        <v>1694.724495574991</v>
+        <v>1694.7244955749909</v>
       </c>
       <c r="X9">
         <v>20.32043759682244</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1447,19 +1469,19 @@
         <v>2375</v>
       </c>
       <c r="E10">
-        <v>-0.1354724601163184</v>
+        <v>-0.13547246011631839</v>
       </c>
       <c r="F10">
-        <v>-7.255873447235714</v>
+        <v>-7.2558734472357136</v>
       </c>
       <c r="G10">
-        <v>-12.03146453983929</v>
+        <v>-12.031464539839289</v>
       </c>
       <c r="H10">
-        <v>-6.247253650647892</v>
+        <v>-6.2472536506478917</v>
       </c>
       <c r="I10">
-        <v>4.039999999999964</v>
+        <v>4.0399999999999636</v>
       </c>
       <c r="J10">
         <v>130</v>
@@ -1477,37 +1499,37 @@
         <v>0.9522854851643946</v>
       </c>
       <c r="O10">
-        <v>692.1019392907139</v>
+        <v>692.10193929071386</v>
       </c>
       <c r="P10">
-        <v>-11.60032970611693</v>
+        <v>-11.600329706116931</v>
       </c>
       <c r="Q10">
-        <v>424.8905533318311</v>
+        <v>424.89055333183109</v>
       </c>
       <c r="R10">
-        <v>17.89012856134026</v>
+        <v>17.890128561340259</v>
       </c>
       <c r="S10">
-        <v>266.8352582946997</v>
+        <v>266.83525829469971</v>
       </c>
       <c r="T10">
         <v>11.23516877030314</v>
       </c>
       <c r="U10">
-        <v>171.0770144699486</v>
+        <v>171.07701446994861</v>
       </c>
       <c r="V10">
-        <v>7.20324271452415</v>
+        <v>7.2032427145241504</v>
       </c>
       <c r="W10">
         <v>111.7783271243394</v>
       </c>
       <c r="X10">
-        <v>4.706455878919554</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24">
+        <v>4.7064558789195541</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1521,19 +1543,19 @@
         <v>20300</v>
       </c>
       <c r="E11">
-        <v>6.344578431437967</v>
+        <v>6.3445784314379674</v>
       </c>
       <c r="F11">
-        <v>7.143662310234333</v>
+        <v>7.1436623102343333</v>
       </c>
       <c r="G11">
-        <v>8.916260803268102</v>
+        <v>8.9162608032681021</v>
       </c>
       <c r="H11">
-        <v>0.09557694835909558</v>
+        <v>9.5576948359095582E-2</v>
       </c>
       <c r="I11">
-        <v>-0.2599999999999767</v>
+        <v>-0.25999999999997669</v>
       </c>
       <c r="J11">
         <v>-92</v>
@@ -1548,25 +1570,25 @@
         <v>-220.6521739130435</v>
       </c>
       <c r="N11">
-        <v>0.5270536919721674</v>
+        <v>0.52705369197216745</v>
       </c>
       <c r="O11">
-        <v>90483.29555142291</v>
+        <v>90483.295551422911</v>
       </c>
       <c r="P11">
         <v>16.12005616023897</v>
       </c>
       <c r="Q11">
-        <v>55548.89436306414</v>
+        <v>55548.894363064137</v>
       </c>
       <c r="R11">
-        <v>273.6398737096756</v>
+        <v>273.63987370967561</v>
       </c>
       <c r="S11">
-        <v>34885.22740532007</v>
+        <v>34885.227405320067</v>
       </c>
       <c r="T11">
-        <v>171.8484108636457</v>
+        <v>171.84841086364571</v>
       </c>
       <c r="U11">
         <v>22366.08681981641</v>
@@ -1578,10 +1600,10 @@
         <v>14613.55738982675</v>
       </c>
       <c r="X11">
-        <v>71.98796743757019</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24">
+        <v>71.987967437570191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1595,10 +1617,10 @@
         <v>12650</v>
       </c>
       <c r="E12">
-        <v>9.11548705561944</v>
+        <v>9.1154870556194396</v>
       </c>
       <c r="F12">
-        <v>8.02974707468978</v>
+        <v>8.0297470746897801</v>
       </c>
       <c r="G12">
         <v>12.54457416663756</v>
@@ -1619,43 +1641,43 @@
         <v>1</v>
       </c>
       <c r="M12">
-        <v>11.08676599474146</v>
+        <v>11.086765994741461</v>
       </c>
       <c r="N12">
         <v>1.268933694452804</v>
       </c>
       <c r="O12">
-        <v>32501.03704899139</v>
+        <v>32501.037048991391</v>
       </c>
       <c r="P12">
-        <v>9.89569231915619</v>
+        <v>9.8956923191561899</v>
       </c>
       <c r="Q12">
         <v>19952.81739819506</v>
       </c>
       <c r="R12">
-        <v>157.7297818039135</v>
+        <v>157.72978180391351</v>
       </c>
       <c r="S12">
-        <v>12530.55673373921</v>
+        <v>12530.556733739209</v>
       </c>
       <c r="T12">
-        <v>99.05578445643646</v>
+        <v>99.055784456436456</v>
       </c>
       <c r="U12">
-        <v>8033.759291610811</v>
+        <v>8033.7592916108106</v>
       </c>
       <c r="V12">
-        <v>63.50797858980879</v>
+        <v>63.507978589808793</v>
       </c>
       <c r="W12">
-        <v>5249.098933121828</v>
+        <v>5249.0989331218279</v>
       </c>
       <c r="X12">
-        <v>41.49485322625951</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24">
+        <v>41.494853226259508</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1681,7 +1703,7 @@
         <v>25.52748725977094</v>
       </c>
       <c r="I13">
-        <v>21.96999999999994</v>
+        <v>21.969999999999938</v>
       </c>
       <c r="J13">
         <v>4102</v>
@@ -1696,7 +1718,7 @@
         <v>11.72598732325695</v>
       </c>
       <c r="N13">
-        <v>2.575773803148763</v>
+        <v>2.5757738031487629</v>
       </c>
       <c r="O13">
         <v>189120.147008489</v>
@@ -1711,25 +1733,25 @@
         <v>241.37913671536</v>
       </c>
       <c r="S13">
-        <v>72914.0035750494</v>
+        <v>72914.003575049399</v>
       </c>
       <c r="T13">
         <v>151.5883650208927</v>
       </c>
       <c r="U13">
-        <v>46747.60796001743</v>
+        <v>46747.607960017427</v>
       </c>
       <c r="V13">
-        <v>97.18837413725036</v>
+        <v>97.188374137250364</v>
       </c>
       <c r="W13">
         <v>30543.95957881934</v>
       </c>
       <c r="X13">
-        <v>63.50095546532089</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24">
+        <v>63.500955465320892</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1743,13 +1765,13 @@
         <v>8230</v>
       </c>
       <c r="E14">
-        <v>8.753508289263223</v>
+        <v>8.7535082892632232</v>
       </c>
       <c r="F14">
-        <v>14.63533513288652</v>
+        <v>14.635335132886521</v>
       </c>
       <c r="G14">
-        <v>13.36101936106328</v>
+        <v>13.361019361063279</v>
       </c>
       <c r="H14">
         <v>11.11912785693265</v>
@@ -1767,13 +1789,13 @@
         <v>1.2</v>
       </c>
       <c r="M14">
-        <v>11.19727891156463</v>
+        <v>11.197278911564631</v>
       </c>
       <c r="N14">
-        <v>1.307386814932486</v>
+        <v>1.3073868149324861</v>
       </c>
       <c r="O14">
-        <v>22061.40459774504</v>
+        <v>22061.404597745041</v>
       </c>
       <c r="P14">
         <v>10.36295807612626</v>
@@ -1782,28 +1804,28 @@
         <v>13543.78867428072</v>
       </c>
       <c r="R14">
-        <v>164.5660835271048</v>
+        <v>164.56608352710481</v>
       </c>
       <c r="S14">
-        <v>8505.626498050413</v>
+        <v>8505.6264980504129</v>
       </c>
       <c r="T14">
         <v>103.3490461488507</v>
       </c>
       <c r="U14">
-        <v>5453.241812129189</v>
+        <v>5453.2418121291894</v>
       </c>
       <c r="V14">
-        <v>66.26053234664872</v>
+        <v>66.260532346648716</v>
       </c>
       <c r="W14">
-        <v>3563.040008927537</v>
+        <v>3563.0400089275372</v>
       </c>
       <c r="X14">
         <v>43.29331724091783</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1817,7 +1839,7 @@
         <v>5100</v>
       </c>
       <c r="E15">
-        <v>10.03245933433847</v>
+        <v>10.032459334338469</v>
       </c>
       <c r="F15">
         <v>8.489499228947949</v>
@@ -1826,10 +1848,10 @@
         <v>5.808990692691296</v>
       </c>
       <c r="H15">
-        <v>5.804327403657638</v>
+        <v>5.8043274036576378</v>
       </c>
       <c r="I15">
-        <v>9.419999999999987</v>
+        <v>9.4199999999999875</v>
       </c>
       <c r="J15">
         <v>528</v>
@@ -1841,31 +1863,31 @@
         <v>2.7</v>
       </c>
       <c r="M15">
-        <v>9.659090909090908</v>
+        <v>9.6590909090909083</v>
       </c>
       <c r="N15">
-        <v>0.8006279434850864</v>
+        <v>0.80062794348508637</v>
       </c>
       <c r="O15">
-        <v>11203.79488308754</v>
+        <v>11203.794883087539</v>
       </c>
       <c r="P15">
-        <v>8.188100880939597</v>
+        <v>8.1881008809395972</v>
       </c>
       <c r="Q15">
-        <v>6878.158168679583</v>
+        <v>6878.1581686795826</v>
       </c>
       <c r="R15">
         <v>134.8658464446977</v>
       </c>
       <c r="S15">
-        <v>4319.547933319323</v>
+        <v>4319.5479333193234</v>
       </c>
       <c r="T15">
-        <v>84.69701830037889</v>
+        <v>84.697018300378886</v>
       </c>
       <c r="U15">
-        <v>2769.406745625659</v>
+        <v>2769.4067456256589</v>
       </c>
       <c r="V15">
         <v>54.30209305148351</v>
@@ -1874,10 +1896,10 @@
         <v>1809.475423171325</v>
       </c>
       <c r="X15">
-        <v>35.47991025826128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24">
+        <v>35.479910258261278</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1891,19 +1913,19 @@
         <v>22000</v>
       </c>
       <c r="E16">
-        <v>5.825241907004738</v>
+        <v>5.8252419070047381</v>
       </c>
       <c r="F16">
-        <v>5.747773299362734</v>
+        <v>5.7477732993627342</v>
       </c>
       <c r="G16">
-        <v>3.759207507267291</v>
+        <v>3.7592075072672908</v>
       </c>
       <c r="H16">
-        <v>7.121663423233443</v>
+        <v>7.1216634232334428</v>
       </c>
       <c r="I16">
-        <v>9.810000000000016</v>
+        <v>9.8100000000000165</v>
       </c>
       <c r="J16">
         <v>1178</v>
@@ -1915,31 +1937,31 @@
         <v>4.5</v>
       </c>
       <c r="M16">
-        <v>18.67572156196944</v>
+        <v>18.675721561969439</v>
       </c>
       <c r="N16">
-        <v>1.832875114554695</v>
+        <v>1.8328751145546951</v>
       </c>
       <c r="O16">
-        <v>17360.26164738289</v>
+        <v>17360.261647382889</v>
       </c>
       <c r="P16">
-        <v>-2.340755874146894</v>
+        <v>-2.3407558741468941</v>
       </c>
       <c r="Q16">
         <v>10657.69471026369</v>
       </c>
       <c r="R16">
-        <v>48.44406686483495</v>
+        <v>48.444066864834952</v>
       </c>
       <c r="S16">
-        <v>6693.132380889335</v>
+        <v>6693.1323808893349</v>
       </c>
       <c r="T16">
-        <v>30.42332900404243</v>
+        <v>30.423329004042429</v>
       </c>
       <c r="U16">
-        <v>4291.191173507039</v>
+        <v>4291.1911735070389</v>
       </c>
       <c r="V16">
         <v>19.50541442503199</v>
@@ -1951,7 +1973,7 @@
         <v>12.74445080218549</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1968,16 +1990,16 @@
         <v>11.67346950326535</v>
       </c>
       <c r="F17">
-        <v>16.1039328701859</v>
+        <v>16.103932870185901</v>
       </c>
       <c r="G17">
-        <v>8.909004525030113</v>
+        <v>8.9090045250301131</v>
       </c>
       <c r="H17">
-        <v>8.460523091841907</v>
+        <v>8.4605230918419068</v>
       </c>
       <c r="I17">
-        <v>9.200000000000003</v>
+        <v>9.2000000000000028</v>
       </c>
       <c r="J17">
         <v>547</v>
@@ -1989,43 +2011,43 @@
         <v>1.4</v>
       </c>
       <c r="M17">
-        <v>10.05484460694698</v>
+        <v>10.054844606946981</v>
       </c>
       <c r="N17">
-        <v>0.9246805648957633</v>
+        <v>0.92468056489576334</v>
       </c>
       <c r="O17">
-        <v>13963.96797336251</v>
+        <v>13963.967973362511</v>
       </c>
       <c r="P17">
-        <v>9.765185443834689</v>
+        <v>9.7651854438346888</v>
       </c>
       <c r="Q17">
-        <v>8572.665010865941</v>
+        <v>8572.6650108659414</v>
       </c>
       <c r="R17">
-        <v>155.866636561199</v>
+        <v>155.86663656119899</v>
       </c>
       <c r="S17">
-        <v>5383.71414593881</v>
+        <v>5383.7141459388104</v>
       </c>
       <c r="T17">
-        <v>97.885711744342</v>
+        <v>97.885711744342004</v>
       </c>
       <c r="U17">
         <v>3451.67931979076</v>
       </c>
       <c r="V17">
-        <v>62.75780581437744</v>
+        <v>62.757805814377441</v>
       </c>
       <c r="W17">
-        <v>2255.258786993051</v>
+        <v>2255.2587869930512</v>
       </c>
       <c r="X17">
-        <v>41.00470521805548</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24">
+        <v>41.004705218055477</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2039,19 +2061,19 @@
         <v>2980</v>
       </c>
       <c r="E18">
-        <v>39.19724373085737</v>
+        <v>39.197243730857373</v>
       </c>
       <c r="F18">
-        <v>33.32555038443081</v>
+        <v>33.325550384430812</v>
       </c>
       <c r="G18">
-        <v>21.27892711259751</v>
+        <v>21.278927112597511</v>
       </c>
       <c r="H18">
-        <v>21.58904631415018</v>
+        <v>21.589046314150181</v>
       </c>
       <c r="I18">
-        <v>20.67000000000004</v>
+        <v>20.670000000000041</v>
       </c>
       <c r="J18">
         <v>181</v>
@@ -2066,40 +2088,40 @@
         <v>16.46408839779005</v>
       </c>
       <c r="N18">
-        <v>3.425287356321839</v>
+        <v>3.4252873563218391</v>
       </c>
       <c r="O18">
-        <v>5989.253785547922</v>
+        <v>5989.2537855479222</v>
       </c>
       <c r="P18">
-        <v>7.229836846536308</v>
+        <v>7.2298368465363083</v>
       </c>
       <c r="Q18">
         <v>3676.882277767033</v>
       </c>
       <c r="R18">
-        <v>123.3853113344642</v>
+        <v>123.38531133446421</v>
       </c>
       <c r="S18">
-        <v>2309.116605708419</v>
+        <v>2309.1166057084188</v>
       </c>
       <c r="T18">
-        <v>77.4871344197456</v>
+        <v>77.487134419745601</v>
       </c>
       <c r="U18">
-        <v>1480.451936869936</v>
+        <v>1480.4519368699359</v>
       </c>
       <c r="V18">
-        <v>49.67959519697771</v>
+        <v>49.679595196977708</v>
       </c>
       <c r="W18">
-        <v>967.2979237101326</v>
+        <v>967.29792371013264</v>
       </c>
       <c r="X18">
-        <v>32.45966186946754</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24">
+        <v>32.459661869467539</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2122,10 +2144,10 @@
         <v>29.39297451711403</v>
       </c>
       <c r="H19">
-        <v>41.08137332404019</v>
+        <v>41.081373324040193</v>
       </c>
       <c r="I19">
-        <v>28.90000000000003</v>
+        <v>28.900000000000031</v>
       </c>
       <c r="J19">
         <v>4307</v>
@@ -2137,16 +2159,16 @@
         <v>0.6</v>
       </c>
       <c r="M19">
-        <v>15.48641745994892</v>
+        <v>15.486417459948919</v>
       </c>
       <c r="N19">
-        <v>4.475608937797759</v>
+        <v>4.4756089377977588</v>
       </c>
       <c r="O19">
-        <v>196056.2393309899</v>
+        <v>196056.23933098989</v>
       </c>
       <c r="P19">
-        <v>11.38468561879398</v>
+        <v>11.384685618793981</v>
       </c>
       <c r="Q19">
         <v>120361.5237646538</v>
@@ -2155,25 +2177,25 @@
         <v>180.4520596171721</v>
       </c>
       <c r="S19">
-        <v>75588.16742485332</v>
+        <v>75588.167424853324</v>
       </c>
       <c r="T19">
-        <v>113.3255883431084</v>
+        <v>113.32558834310839</v>
       </c>
       <c r="U19">
-        <v>48462.10390238895</v>
+        <v>48462.103902388953</v>
       </c>
       <c r="V19">
-        <v>72.65682743986349</v>
+        <v>72.656827439863491</v>
       </c>
       <c r="W19">
-        <v>31664.17721234264</v>
+        <v>31664.177212342642</v>
       </c>
       <c r="X19">
         <v>47.47252955373709</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2187,19 +2209,19 @@
         <v>39850</v>
       </c>
       <c r="E20">
-        <v>8.003743285250167</v>
+        <v>8.0037432852501667</v>
       </c>
       <c r="F20">
-        <v>9.637970928865741</v>
+        <v>9.6379709288657409</v>
       </c>
       <c r="G20">
-        <v>9.940922606544959</v>
+        <v>9.9409226065449587</v>
       </c>
       <c r="H20">
         <v>10.53175146909021</v>
       </c>
       <c r="I20">
-        <v>11.79999999999998</v>
+        <v>11.799999999999979</v>
       </c>
       <c r="J20">
         <v>3006</v>
@@ -2217,7 +2239,7 @@
         <v>1.563542197983286</v>
       </c>
       <c r="O20">
-        <v>65752.53342123679</v>
+        <v>65752.533421236789</v>
       </c>
       <c r="P20">
         <v>5.135265675195444</v>
@@ -2232,22 +2254,22 @@
         <v>25350.44802354883</v>
       </c>
       <c r="T20">
-        <v>63.61467509046131</v>
+        <v>63.614675090461311</v>
       </c>
       <c r="U20">
-        <v>16253.02065049658</v>
+        <v>16253.020650496581</v>
       </c>
       <c r="V20">
-        <v>40.78549724089481</v>
+        <v>40.785497240894813</v>
       </c>
       <c r="W20">
-        <v>10619.40123668091</v>
+        <v>10619.401236680909</v>
       </c>
       <c r="X20">
         <v>26.64843472190945</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2261,10 +2283,10 @@
         <v>4220</v>
       </c>
       <c r="E21">
-        <v>7.527198037421655</v>
+        <v>7.5271980374216554</v>
       </c>
       <c r="F21">
-        <v>-1.464164464733344</v>
+        <v>-1.4641644647333441</v>
       </c>
       <c r="G21">
         <v>-15.31744609928846</v>
@@ -2273,7 +2295,7 @@
         <v>-19.82504108442026</v>
       </c>
       <c r="I21">
-        <v>-3.720000000000027</v>
+        <v>-3.7200000000000268</v>
       </c>
       <c r="J21">
         <v>-86</v>
@@ -2285,43 +2307,43 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <v>-49.06976744186046</v>
+        <v>-49.069767441860463</v>
       </c>
       <c r="N21">
-        <v>1.82053494391717</v>
+        <v>1.8205349439171701</v>
       </c>
       <c r="O21">
-        <v>439.5951617579238</v>
+        <v>439.59516175792379</v>
       </c>
       <c r="P21">
-        <v>-20.2420385376653</v>
+        <v>-20.242038537665302</v>
       </c>
       <c r="Q21">
-        <v>269.8732959955833</v>
+        <v>269.87329599558331</v>
       </c>
       <c r="R21">
-        <v>6.395101800843205</v>
+        <v>6.3951018008432046</v>
       </c>
       <c r="S21">
-        <v>169.4829646814569</v>
+        <v>169.48296468145691</v>
       </c>
       <c r="T21">
-        <v>4.016183997190922</v>
+        <v>4.0161839971909217</v>
       </c>
       <c r="U21">
-        <v>108.6612008717265</v>
+        <v>108.66120087172651</v>
       </c>
       <c r="V21">
-        <v>2.574909973263661</v>
+        <v>2.5749099732636611</v>
       </c>
       <c r="W21">
-        <v>70.99707283526953</v>
+        <v>70.997072835269535</v>
       </c>
       <c r="X21">
         <v>1.682395090883164</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2335,19 +2357,19 @@
         <v>10450</v>
       </c>
       <c r="E22">
-        <v>4.763907634449509</v>
+        <v>4.7639076344495086</v>
       </c>
       <c r="F22">
-        <v>9.30689726518024</v>
+        <v>9.3068972651802397</v>
       </c>
       <c r="G22">
         <v>11.83297375633879</v>
       </c>
       <c r="H22">
-        <v>7.163996652458891</v>
+        <v>7.1639966524588914</v>
       </c>
       <c r="I22">
-        <v>6.889999999999972</v>
+        <v>6.8899999999999721</v>
       </c>
       <c r="J22">
         <v>842</v>
@@ -2359,22 +2381,22 @@
         <v>1.4</v>
       </c>
       <c r="M22">
-        <v>12.41092636579572</v>
+        <v>12.410926365795721</v>
       </c>
       <c r="N22">
-        <v>0.8550855085508551</v>
+        <v>0.85508550855085508</v>
       </c>
       <c r="O22">
-        <v>37394.30604425666</v>
+        <v>37394.306044256657</v>
       </c>
       <c r="P22">
         <v>13.59753793552569</v>
       </c>
       <c r="Q22">
-        <v>22956.86008752848</v>
+        <v>22956.860087528479</v>
       </c>
       <c r="R22">
-        <v>219.6828716509903</v>
+        <v>219.68287165099031</v>
       </c>
       <c r="S22">
         <v>14417.12375823732</v>
@@ -2383,19 +2405,19 @@
         <v>137.9629067773906</v>
       </c>
       <c r="U22">
-        <v>9243.300550180695</v>
+        <v>9243.3005501806947</v>
       </c>
       <c r="V22">
-        <v>88.4526368438344</v>
+        <v>88.452636843834398</v>
       </c>
       <c r="W22">
-        <v>6039.389194438955</v>
+        <v>6039.3891944389552</v>
       </c>
       <c r="X22">
-        <v>57.79319803290866</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24">
+        <v>57.793198032908663</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2409,16 +2431,16 @@
         <v>36350</v>
       </c>
       <c r="E23">
-        <v>4.861462892713917</v>
+        <v>4.8614628927139174</v>
       </c>
       <c r="F23">
-        <v>4.861462892713917</v>
+        <v>4.8614628927139174</v>
       </c>
       <c r="G23">
-        <v>10.40719402213277</v>
+        <v>10.407194022132771</v>
       </c>
       <c r="H23">
-        <v>10.63011322024147</v>
+        <v>10.630113220241469</v>
       </c>
       <c r="I23">
         <v>12.04000000000001</v>
@@ -2439,37 +2461,37 @@
         <v>1.942396067115528</v>
       </c>
       <c r="O23">
-        <v>50366.33505369631</v>
+        <v>50366.335053696312</v>
       </c>
       <c r="P23">
-        <v>3.315050783030626</v>
+        <v>3.3150507830306259</v>
       </c>
       <c r="Q23">
-        <v>30920.56062173869</v>
+        <v>30920.560621738688</v>
       </c>
       <c r="R23">
-        <v>85.06344049996888</v>
+        <v>85.063440499968877</v>
       </c>
       <c r="S23">
-        <v>19418.40249311199</v>
+        <v>19418.402493111989</v>
       </c>
       <c r="T23">
-        <v>53.42063959590644</v>
+        <v>53.420639595906437</v>
       </c>
       <c r="U23">
         <v>12449.78772868335</v>
       </c>
       <c r="V23">
-        <v>34.24975991384692</v>
+        <v>34.249759913846923</v>
       </c>
       <c r="W23">
-        <v>8134.444300872496</v>
+        <v>8134.4443008724957</v>
       </c>
       <c r="X23">
-        <v>22.37811362000686</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24">
+        <v>22.378113620006861</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2483,19 +2505,19 @@
         <v>11250</v>
       </c>
       <c r="E24">
-        <v>11.01976456805946</v>
+        <v>11.019764568059459</v>
       </c>
       <c r="F24">
         <v>13.10552477381094</v>
       </c>
       <c r="G24">
-        <v>5.162086082275977</v>
+        <v>5.1620860822759767</v>
       </c>
       <c r="H24">
-        <v>4.957648096370477</v>
+        <v>4.9576480963704768</v>
       </c>
       <c r="I24">
-        <v>5.179999999999993</v>
+        <v>5.1799999999999926</v>
       </c>
       <c r="J24">
         <v>612</v>
@@ -2504,37 +2526,37 @@
         <v>11818</v>
       </c>
       <c r="L24">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="M24">
-        <v>18.38235294117647</v>
+        <v>18.382352941176471</v>
       </c>
       <c r="N24">
-        <v>0.9519377221188018</v>
+        <v>0.95193772211880179</v>
       </c>
       <c r="O24">
-        <v>19549.51155876396</v>
+        <v>19549.511558763959</v>
       </c>
       <c r="P24">
-        <v>5.681346699416046</v>
+        <v>5.6813466994160464</v>
       </c>
       <c r="Q24">
         <v>12001.70424617346</v>
       </c>
       <c r="R24">
-        <v>106.6818155215418</v>
+        <v>106.68181552154179</v>
       </c>
       <c r="S24">
-        <v>7537.182993106501</v>
+        <v>7537.1829931065013</v>
       </c>
       <c r="T24">
-        <v>66.99718216094668</v>
+        <v>66.997182160946679</v>
       </c>
       <c r="U24">
-        <v>4832.340269479088</v>
+        <v>4832.3402694790884</v>
       </c>
       <c r="V24">
-        <v>42.95413572870301</v>
+        <v>42.954135728703008</v>
       </c>
       <c r="W24">
         <v>3157.35525950995</v>
@@ -2543,7 +2565,7 @@
         <v>28.06538008453289</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2557,16 +2579,16 @@
         <v>6410</v>
       </c>
       <c r="E25">
-        <v>4.907650159011212</v>
+        <v>4.9076501590112116</v>
       </c>
       <c r="F25">
         <v>6.311045998066092</v>
       </c>
       <c r="G25">
-        <v>6.109339139414985</v>
+        <v>6.1093391394149847</v>
       </c>
       <c r="H25">
-        <v>9.438734374630513</v>
+        <v>9.4387343746305135</v>
       </c>
       <c r="I25">
         <v>13.36</v>
@@ -2581,10 +2603,10 @@
         <v>0</v>
       </c>
       <c r="M25">
-        <v>13.6965811965812</v>
+        <v>13.696581196581199</v>
       </c>
       <c r="N25">
-        <v>1.827773025377816</v>
+        <v>1.8277730253778159</v>
       </c>
       <c r="O25">
         <v>6345.587879201983</v>
@@ -2593,31 +2615,31 @@
         <v>-0.1009442340125455</v>
       </c>
       <c r="Q25">
-        <v>3895.640500549695</v>
+        <v>3895.6405005496949</v>
       </c>
       <c r="R25">
-        <v>60.77442278548666</v>
+        <v>60.774422785486657</v>
       </c>
       <c r="S25">
-        <v>2446.498824311696</v>
+        <v>2446.4988243116959</v>
       </c>
       <c r="T25">
-        <v>38.16690833559589</v>
+        <v>38.166908335595892</v>
       </c>
       <c r="U25">
-        <v>1568.532275091016</v>
+        <v>1568.5322750910159</v>
       </c>
       <c r="V25">
-        <v>24.47008229471164</v>
+        <v>24.470082294711641</v>
       </c>
       <c r="W25">
-        <v>1024.847869209257</v>
+        <v>1024.8478692092569</v>
       </c>
       <c r="X25">
         <v>15.98826629031602</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2631,10 +2653,10 @@
         <v>7940</v>
       </c>
       <c r="E26">
-        <v>-5.62941063390349</v>
+        <v>-5.6294106339034897</v>
       </c>
       <c r="F26">
-        <v>-20.67834516482944</v>
+        <v>-20.678345164829441</v>
       </c>
       <c r="G26">
         <v>-14.09437256107617</v>
@@ -2658,10 +2680,10 @@
         <v>184.6511627906977</v>
       </c>
       <c r="N26">
-        <v>4.978056426332288</v>
+        <v>4.9780564263322882</v>
       </c>
       <c r="O26">
-        <v>349.1216884400737</v>
+        <v>349.12168844007368</v>
       </c>
       <c r="P26">
         <v>-26.83293526112881</v>
@@ -2670,16 +2692,16 @@
         <v>214.3304316318889</v>
       </c>
       <c r="R26">
-        <v>2.699375713247971</v>
+        <v>2.6993757132479712</v>
       </c>
       <c r="S26">
-        <v>134.601524172378</v>
+        <v>134.60152417237799</v>
       </c>
       <c r="T26">
         <v>1.695233301919119</v>
       </c>
       <c r="U26">
-        <v>86.29754195782922</v>
+        <v>86.297541957829225</v>
       </c>
       <c r="V26">
         <v>1.086870805514222</v>
@@ -2688,10 +2710,10 @@
         <v>56.38510179100124</v>
       </c>
       <c r="X26">
-        <v>0.7101398210453557</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24">
+        <v>0.71013982104535567</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2708,7 +2730,7 @@
         <v>7.830830248293978</v>
       </c>
       <c r="F27">
-        <v>5.673093905494596</v>
+        <v>5.6730939054945964</v>
       </c>
       <c r="G27">
         <v>7.184947541800824</v>
@@ -2732,40 +2754,40 @@
         <v>15.41684572410829</v>
       </c>
       <c r="N27">
-        <v>2.074748789127449</v>
+        <v>2.0747487891274492</v>
       </c>
       <c r="O27">
-        <v>138428.1384477472</v>
+        <v>138428.13844774719</v>
       </c>
       <c r="P27">
-        <v>-0.3591903644818872</v>
+        <v>-0.35919036448188718</v>
       </c>
       <c r="Q27">
-        <v>84982.86885604713</v>
+        <v>84982.868856047135</v>
       </c>
       <c r="R27">
-        <v>59.22151139794225</v>
+        <v>59.221511397942251</v>
       </c>
       <c r="S27">
-        <v>53370.03984675104</v>
+        <v>53370.039846751039</v>
       </c>
       <c r="T27">
-        <v>37.19166539843278</v>
+        <v>37.191665398432782</v>
       </c>
       <c r="U27">
-        <v>34217.31872120335</v>
+        <v>34217.318721203352</v>
       </c>
       <c r="V27">
-        <v>23.84482140850408</v>
+        <v>23.844821408504082</v>
       </c>
       <c r="W27">
-        <v>22356.91718835968</v>
+        <v>22356.917188359679</v>
       </c>
       <c r="X27">
-        <v>15.5797332323064</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24">
+        <v>15.579733232306401</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2782,16 +2804,16 @@
         <v>16.00472807946176</v>
       </c>
       <c r="F28">
-        <v>8.790483559269205</v>
+        <v>8.7904835592692052</v>
       </c>
       <c r="G28">
-        <v>7.908283717566206</v>
+        <v>7.9082837175662064</v>
       </c>
       <c r="H28">
-        <v>6.748555312217832</v>
+        <v>6.7485553122178317</v>
       </c>
       <c r="I28">
-        <v>4.929999999999964</v>
+        <v>4.9299999999999642</v>
       </c>
       <c r="J28">
         <v>315</v>
@@ -2803,43 +2825,43 @@
         <v>1.4</v>
       </c>
       <c r="M28">
-        <v>21.55555555555556</v>
+        <v>21.555555555555561</v>
       </c>
       <c r="N28">
-        <v>1.06276412584129</v>
+        <v>1.0627641258412901</v>
       </c>
       <c r="O28">
-        <v>13676.68169548652</v>
+        <v>13676.681695486521</v>
       </c>
       <c r="P28">
-        <v>7.253406924150685</v>
+        <v>7.2534069241506849</v>
       </c>
       <c r="Q28">
-        <v>8396.296157317476</v>
+        <v>8396.2961573174762</v>
       </c>
       <c r="R28">
-        <v>123.6567917130703</v>
+        <v>123.65679171307031</v>
       </c>
       <c r="S28">
         <v>5272.952849358534</v>
       </c>
       <c r="T28">
-        <v>77.65762664740109</v>
+        <v>77.657626647401088</v>
       </c>
       <c r="U28">
-        <v>3380.666545621138</v>
+        <v>3380.6665456211381</v>
       </c>
       <c r="V28">
-        <v>49.78890347011985</v>
+        <v>49.788903470119848</v>
       </c>
       <c r="W28">
-        <v>2208.860449228435</v>
+        <v>2208.8604492284348</v>
       </c>
       <c r="X28">
-        <v>32.53108172648652</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24">
+        <v>32.531081726486519</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2853,7 +2875,7 @@
         <v>4350</v>
       </c>
       <c r="E29">
-        <v>13.61023543555848</v>
+        <v>13.610235435558479</v>
       </c>
       <c r="F29">
         <v>-3.31800189359133</v>
@@ -2862,10 +2884,10 @@
         <v>-11.7636537790312</v>
       </c>
       <c r="H29">
-        <v>-13.13740660872928</v>
+        <v>-13.137406608729281</v>
       </c>
       <c r="I29">
-        <v>8.909999999999968</v>
+        <v>8.9099999999999682</v>
       </c>
       <c r="J29">
         <v>77</v>
@@ -2877,7 +2899,7 @@
         <v>0</v>
       </c>
       <c r="M29">
-        <v>56.49350649350649</v>
+        <v>56.493506493506487</v>
       </c>
       <c r="N29">
         <v>5.040556199304751</v>
@@ -2886,7 +2908,7 @@
         <v>246.8800273034721</v>
       </c>
       <c r="P29">
-        <v>-24.94153647794843</v>
+        <v>-24.941536477948429</v>
       </c>
       <c r="Q29">
         <v>151.562920796106</v>
@@ -2895,25 +2917,25 @@
         <v>3.484205075772552</v>
       </c>
       <c r="S29">
-        <v>95.18293782103318</v>
+        <v>95.182937821033178</v>
       </c>
       <c r="T29">
-        <v>2.1881135131272</v>
+        <v>2.1881135131271998</v>
       </c>
       <c r="U29">
-        <v>61.02496699636698</v>
+        <v>61.024966996366977</v>
       </c>
       <c r="V29">
-        <v>1.402872804514183</v>
+        <v>1.4028728045141829</v>
       </c>
       <c r="W29">
-        <v>39.87250271350831</v>
+        <v>39.872502713508311</v>
       </c>
       <c r="X29">
-        <v>0.9166092577818002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24">
+        <v>0.91660925778180025</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2927,19 +2949,19 @@
         <v>16450</v>
       </c>
       <c r="E30">
-        <v>8.010916726028213</v>
+        <v>8.0109167260282135</v>
       </c>
       <c r="F30">
-        <v>7.140539757216771</v>
+        <v>7.1405397572167706</v>
       </c>
       <c r="G30">
-        <v>8.631246856550362</v>
+        <v>8.6312468565503622</v>
       </c>
       <c r="H30">
         <v>11.66866476625067</v>
       </c>
       <c r="I30">
-        <v>12.01999999999997</v>
+        <v>12.019999999999969</v>
       </c>
       <c r="J30">
         <v>1191</v>
@@ -2951,43 +2973,43 @@
         <v>1.2</v>
       </c>
       <c r="M30">
-        <v>13.81192275398825</v>
+        <v>13.811922753988251</v>
       </c>
       <c r="N30">
         <v>1.740924965604826</v>
       </c>
       <c r="O30">
-        <v>21623.87351885062</v>
+        <v>21623.873518850622</v>
       </c>
       <c r="P30">
-        <v>2.772461639693957</v>
+        <v>2.7724616396939572</v>
       </c>
       <c r="Q30">
-        <v>13275.18254611145</v>
+        <v>13275.182546111449</v>
       </c>
       <c r="R30">
-        <v>80.70019784870182</v>
+        <v>80.700197848701819</v>
       </c>
       <c r="S30">
-        <v>8336.939326665804</v>
+        <v>8336.9393266658044</v>
       </c>
       <c r="T30">
-        <v>50.68048222897146</v>
+        <v>50.680482228971456</v>
       </c>
       <c r="U30">
         <v>5345.090820973488</v>
       </c>
       <c r="V30">
-        <v>32.49295331898777</v>
+        <v>32.492953318987773</v>
       </c>
       <c r="W30">
-        <v>3492.37629699827</v>
+        <v>3492.3762969982699</v>
       </c>
       <c r="X30">
         <v>21.23025104558219</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3004,13 +3026,13 @@
         <v>3.245641701310845</v>
       </c>
       <c r="F31">
-        <v>-3.847251041198177</v>
+        <v>-3.8472510411981768</v>
       </c>
       <c r="G31">
         <v>-2.839361416564969</v>
       </c>
       <c r="H31">
-        <v>8.279621130351202</v>
+        <v>8.2796211303512024</v>
       </c>
       <c r="I31">
         <v>16.68999999999998</v>
@@ -3025,43 +3047,43 @@
         <v>0</v>
       </c>
       <c r="M31">
-        <v>18.98530762167126</v>
+        <v>18.985307621671261</v>
       </c>
       <c r="N31">
         <v>3.167126225490196</v>
       </c>
       <c r="O31">
-        <v>9788.445939846259</v>
+        <v>9788.4459398462586</v>
       </c>
       <c r="P31">
         <v>-13.41875564018973</v>
       </c>
       <c r="Q31">
-        <v>6009.256694038851</v>
+        <v>6009.2566940388506</v>
       </c>
       <c r="R31">
-        <v>14.53266431448331</v>
+        <v>14.532664314483309</v>
       </c>
       <c r="S31">
         <v>3773.869646051467</v>
       </c>
       <c r="T31">
-        <v>9.126649688153488</v>
+        <v>9.1266496881534884</v>
       </c>
       <c r="U31">
-        <v>2419.554133030669</v>
+        <v>2419.5541330306692</v>
       </c>
       <c r="V31">
-        <v>5.851400563556635</v>
+        <v>5.8514005635566351</v>
       </c>
       <c r="W31">
-        <v>1580.888667100614</v>
+        <v>1580.8886671006139</v>
       </c>
       <c r="X31">
-        <v>3.823189037728209</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24">
+        <v>3.8231890377282092</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3075,19 +3097,19 @@
         <v>3815</v>
       </c>
       <c r="E32">
-        <v>7.40278118335462</v>
+        <v>7.4027811833546204</v>
       </c>
       <c r="F32">
-        <v>1.759180402786711</v>
+        <v>1.7591804027867111</v>
       </c>
       <c r="G32">
-        <v>7.292597363726841</v>
+        <v>7.2925973637268413</v>
       </c>
       <c r="H32">
-        <v>12.45842177154051</v>
+        <v>12.458421771540509</v>
       </c>
       <c r="I32">
-        <v>13.45000000000002</v>
+        <v>13.450000000000021</v>
       </c>
       <c r="J32">
         <v>154</v>
@@ -3102,28 +3124,28 @@
         <v>24.77272727272727</v>
       </c>
       <c r="N32">
-        <v>3.331877729257642</v>
+        <v>3.3318777292576418</v>
       </c>
       <c r="O32">
-        <v>2314.744579978288</v>
+        <v>2314.7445799782881</v>
       </c>
       <c r="P32">
-        <v>-4.873645580114694</v>
+        <v>-4.8736455801146938</v>
       </c>
       <c r="Q32">
         <v>1421.052376210308</v>
       </c>
       <c r="R32">
-        <v>37.24907932399235</v>
+        <v>37.249079323992348</v>
       </c>
       <c r="S32">
-        <v>892.4342395540081</v>
+        <v>892.43423955400806</v>
       </c>
       <c r="T32">
-        <v>23.39277167900414</v>
+        <v>23.392771679004142</v>
       </c>
       <c r="U32">
-        <v>572.1694587491148</v>
+        <v>572.16945874911482</v>
       </c>
       <c r="V32">
         <v>14.99788882697549</v>
@@ -3132,10 +3154,10 @@
         <v>373.8441726305046</v>
       </c>
       <c r="X32">
-        <v>9.799323004731445</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24">
+        <v>9.7993230047314448</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3152,16 +3174,16 @@
         <v>13.5933167707806</v>
       </c>
       <c r="F33">
-        <v>12.21742437679663</v>
+        <v>12.217424376796631</v>
       </c>
       <c r="G33">
-        <v>8.671327916870027</v>
+        <v>8.6713279168700268</v>
       </c>
       <c r="H33">
         <v>12.49589919685522</v>
       </c>
       <c r="I33">
-        <v>14.15999999999998</v>
+        <v>14.159999999999981</v>
       </c>
       <c r="J33">
         <v>431</v>
@@ -3173,13 +3195,13 @@
         <v>1.5</v>
       </c>
       <c r="M33">
-        <v>19.46635730858469</v>
+        <v>19.466357308584691</v>
       </c>
       <c r="N33">
-        <v>2.755336617405583</v>
+        <v>2.7553366174055829</v>
       </c>
       <c r="O33">
-        <v>6994.183733613721</v>
+        <v>6994.1837336137214</v>
       </c>
       <c r="P33">
         <v>-1.803161063388903</v>
@@ -3188,28 +3210,28 @@
         <v>4293.822091764654</v>
       </c>
       <c r="R33">
-        <v>51.17785568253461</v>
+        <v>51.177855682534613</v>
       </c>
       <c r="S33">
-        <v>2696.560603531956</v>
+        <v>2696.5606035319561</v>
       </c>
       <c r="T33">
-        <v>32.14017405878374</v>
+        <v>32.140174058783742</v>
       </c>
       <c r="U33">
-        <v>1728.855250755642</v>
+        <v>1728.8552507556419</v>
       </c>
       <c r="V33">
         <v>20.60614124857738</v>
       </c>
       <c r="W33">
-        <v>1129.599720735962</v>
+        <v>1129.5997207359619</v>
       </c>
       <c r="X33">
         <v>13.46364387051206</v>
       </c>
     </row>
-    <row r="34" spans="1:24">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3229,7 +3251,7 @@
         <v>3.485399252989851</v>
       </c>
       <c r="G34">
-        <v>10.86178997558132</v>
+        <v>10.861789975581321</v>
       </c>
       <c r="H34">
         <v>15.99093727193822</v>
@@ -3247,31 +3269,31 @@
         <v>1</v>
       </c>
       <c r="M34">
-        <v>25.36945812807882</v>
+        <v>25.369458128078819</v>
       </c>
       <c r="N34">
-        <v>3.532639762204184</v>
+        <v>3.5326397622041839</v>
       </c>
       <c r="O34">
-        <v>24528.89538028485</v>
+        <v>24528.895380284848</v>
       </c>
       <c r="P34">
-        <v>-2.282589174755523</v>
+        <v>-2.2825891747555231</v>
       </c>
       <c r="Q34">
-        <v>15058.61396867157</v>
+        <v>15058.613968671571</v>
       </c>
       <c r="R34">
-        <v>48.7333785393902</v>
+        <v>48.733378539390202</v>
       </c>
       <c r="S34">
-        <v>9456.951010987859</v>
+        <v>9456.9510109878593</v>
       </c>
       <c r="T34">
         <v>30.60501945303514</v>
       </c>
       <c r="U34">
-        <v>6063.167796069704</v>
+        <v>6063.1677960697043</v>
       </c>
       <c r="V34">
         <v>19.62190225265276</v>
@@ -3283,7 +3305,7 @@
         <v>12.82056163766004</v>
       </c>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3297,16 +3319,16 @@
         <v>11650</v>
       </c>
       <c r="E35">
-        <v>13.24684556536035</v>
+        <v>13.246845565360349</v>
       </c>
       <c r="F35">
-        <v>5.246899430256832</v>
+        <v>5.2468994302568319</v>
       </c>
       <c r="G35">
-        <v>2.835992848178577</v>
+        <v>2.8359928481785772</v>
       </c>
       <c r="H35">
-        <v>1.287819412956864</v>
+        <v>1.2878194129568641</v>
       </c>
       <c r="I35">
         <v>5.430000000000021</v>
@@ -3321,10 +3343,10 @@
         <v>0.5</v>
       </c>
       <c r="M35">
-        <v>71.47239263803681</v>
+        <v>71.472392638036808</v>
       </c>
       <c r="N35">
-        <v>3.876871880199667</v>
+        <v>3.8768718801996669</v>
       </c>
       <c r="O35">
         <v>3974.622898663406</v>
@@ -3336,28 +3358,28 @@
         <v>2440.073675316055</v>
       </c>
       <c r="R35">
-        <v>20.94483841473009</v>
+        <v>20.944838414730089</v>
       </c>
       <c r="S35">
-        <v>1532.389186592629</v>
+        <v>1532.3891865926289</v>
       </c>
       <c r="T35">
-        <v>13.15355524972214</v>
+        <v>13.153555249722141</v>
       </c>
       <c r="U35">
-        <v>982.4659931513528</v>
+        <v>982.46599315135279</v>
       </c>
       <c r="V35">
-        <v>8.433184490569552</v>
+        <v>8.4331844905695519</v>
       </c>
       <c r="W35">
-        <v>641.9237880159619</v>
+        <v>641.92378801596192</v>
       </c>
       <c r="X35">
         <v>5.510075433613407</v>
       </c>
     </row>
-    <row r="36" spans="1:24">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3371,16 +3393,16 @@
         <v>17250</v>
       </c>
       <c r="E36">
-        <v>9.811511319139655</v>
+        <v>9.8115113191396546</v>
       </c>
       <c r="F36">
-        <v>9.811511319139655</v>
+        <v>9.8115113191396546</v>
       </c>
       <c r="G36">
         <v>13.16202353973539</v>
       </c>
       <c r="H36">
-        <v>9.152411695708295</v>
+        <v>9.1524116957082953</v>
       </c>
       <c r="I36">
         <v>14.06999999999999</v>
@@ -3395,43 +3417,43 @@
         <v>0.3</v>
       </c>
       <c r="M36">
-        <v>22.22938144329897</v>
+        <v>22.229381443298969</v>
       </c>
       <c r="N36">
-        <v>3.129535558780842</v>
+        <v>3.1295355587808422</v>
       </c>
       <c r="O36">
-        <v>18980.87622240321</v>
+        <v>18980.876222403211</v>
       </c>
       <c r="P36">
-        <v>0.9607843224635815</v>
+        <v>0.96078432246358147</v>
       </c>
       <c r="Q36">
-        <v>11652.61147674999</v>
+        <v>11652.611476749989</v>
       </c>
       <c r="R36">
-        <v>67.55137087971008</v>
+        <v>67.551370879710078</v>
       </c>
       <c r="S36">
-        <v>7317.94945504011</v>
+        <v>7317.9494550401096</v>
       </c>
       <c r="T36">
-        <v>42.42289539153688</v>
+        <v>42.422895391536883</v>
       </c>
       <c r="U36">
-        <v>4691.782310970249</v>
+        <v>4691.7823109702485</v>
       </c>
       <c r="V36">
-        <v>27.19873803461014</v>
+        <v>27.198738034610141</v>
       </c>
       <c r="W36">
-        <v>3065.517478059244</v>
+        <v>3065.5174780592438</v>
       </c>
       <c r="X36">
         <v>17.7711158148362</v>
       </c>
     </row>
-    <row r="37" spans="1:24">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3445,19 +3467,19 @@
         <v>17850</v>
       </c>
       <c r="E37">
-        <v>4.310988145912432</v>
+        <v>4.3109881459124324</v>
       </c>
       <c r="F37">
-        <v>4.76951311414723</v>
+        <v>4.7695131141472302</v>
       </c>
       <c r="G37">
-        <v>7.854132035005819</v>
+        <v>7.8541320350058186</v>
       </c>
       <c r="H37">
-        <v>9.67928990222093</v>
+        <v>9.6792899022209298</v>
       </c>
       <c r="I37">
-        <v>9.289999999999978</v>
+        <v>9.2899999999999778</v>
       </c>
       <c r="J37">
         <v>1070</v>
@@ -3472,40 +3494,40 @@
         <v>16.68224299065421</v>
       </c>
       <c r="N37">
-        <v>1.549613681743207</v>
+        <v>1.5496136817432069</v>
       </c>
       <c r="O37">
-        <v>24534.80778105288</v>
+        <v>24534.807781052881</v>
       </c>
       <c r="P37">
-        <v>3.232024379889409</v>
+        <v>3.2320243798894088</v>
       </c>
       <c r="Q37">
         <v>15062.24366986331</v>
       </c>
       <c r="R37">
-        <v>84.38231747822581</v>
+        <v>84.382317478225815</v>
       </c>
       <c r="S37">
-        <v>9459.230497428391</v>
+        <v>9459.2304974283907</v>
       </c>
       <c r="T37">
-        <v>52.9928879407753</v>
+        <v>52.992887940775297</v>
       </c>
       <c r="U37">
-        <v>6064.629251116025</v>
+        <v>6064.6292511160254</v>
       </c>
       <c r="V37">
-        <v>33.97551401185448</v>
+        <v>33.975514011854479</v>
       </c>
       <c r="W37">
         <v>3962.508431769269</v>
       </c>
       <c r="X37">
-        <v>22.19892678862336</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24">
+        <v>22.198926788623361</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3519,13 +3541,13 @@
         <v>26850</v>
       </c>
       <c r="E38">
-        <v>8.741483856132689</v>
+        <v>8.7414838561326889</v>
       </c>
       <c r="F38">
         <v>7.460271512345912</v>
       </c>
       <c r="G38">
-        <v>9.203214946692526</v>
+        <v>9.2032149466925262</v>
       </c>
       <c r="H38">
         <v>10.0466953627209</v>
@@ -3543,43 +3565,43 @@
         <v>0.8</v>
       </c>
       <c r="M38">
-        <v>26.82317682317682</v>
+        <v>26.823176823176819</v>
       </c>
       <c r="N38">
         <v>3.121367123924669</v>
       </c>
       <c r="O38">
-        <v>20746.92228980272</v>
+        <v>20746.922289802718</v>
       </c>
       <c r="P38">
-        <v>-2.545715110347879</v>
+        <v>-2.5457151103478788</v>
       </c>
       <c r="Q38">
         <v>12736.81056389008</v>
       </c>
       <c r="R38">
-        <v>47.43691085247703</v>
+        <v>47.436910852477027</v>
       </c>
       <c r="S38">
-        <v>7998.836665149406</v>
+        <v>7998.8366651494061</v>
       </c>
       <c r="T38">
         <v>29.79082556852665</v>
       </c>
       <c r="U38">
-        <v>5128.321889138073</v>
+        <v>5128.3218891380729</v>
       </c>
       <c r="V38">
         <v>19.09989530405241</v>
       </c>
       <c r="W38">
-        <v>3350.743777584922</v>
+        <v>3350.7437775849221</v>
       </c>
       <c r="X38">
         <v>12.47949265394757</v>
       </c>
     </row>
-    <row r="39" spans="1:24">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3593,19 +3615,19 @@
         <v>8220</v>
       </c>
       <c r="E39">
-        <v>7.717713294879559</v>
+        <v>7.7177132948795588</v>
       </c>
       <c r="F39">
-        <v>0.1809860916023212</v>
+        <v>0.18098609160232121</v>
       </c>
       <c r="G39">
-        <v>0.1938096902323707</v>
+        <v>0.19380969023237071</v>
       </c>
       <c r="H39">
-        <v>4.881653593222268</v>
+        <v>4.8816535932222678</v>
       </c>
       <c r="I39">
-        <v>8.239999999999952</v>
+        <v>8.2399999999999523</v>
       </c>
       <c r="J39">
         <v>312</v>
@@ -3620,40 +3642,40 @@
         <v>26.34615384615385</v>
       </c>
       <c r="N39">
-        <v>2.169437846397466</v>
+        <v>2.1694378463974662</v>
       </c>
       <c r="O39">
-        <v>3863.078267138034</v>
+        <v>3863.0782671380339</v>
       </c>
       <c r="P39">
-        <v>-7.273008604933695</v>
+        <v>-7.2730086049336951</v>
       </c>
       <c r="Q39">
-        <v>2371.594947661309</v>
+        <v>2371.5949476613091</v>
       </c>
       <c r="R39">
         <v>28.85152004454147</v>
       </c>
       <c r="S39">
-        <v>1489.383902436132</v>
+        <v>1489.3839024361321</v>
       </c>
       <c r="T39">
-        <v>18.1190255770819</v>
+        <v>18.119025577081899</v>
       </c>
       <c r="U39">
-        <v>954.8938661882819</v>
+        <v>954.89386618828189</v>
       </c>
       <c r="V39">
         <v>11.61671370058737</v>
       </c>
       <c r="W39">
-        <v>623.9087072832236</v>
+        <v>623.90870728322363</v>
       </c>
       <c r="X39">
-        <v>7.590130258919996</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24">
+        <v>7.5901302589199959</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3667,19 +3689,19 @@
         <v>8370</v>
       </c>
       <c r="E40">
-        <v>-1.006587948407372</v>
+        <v>-1.0065879484073721</v>
       </c>
       <c r="F40">
-        <v>-17.18868535973797</v>
+        <v>-17.188685359737971</v>
       </c>
       <c r="G40">
-        <v>-8.405360777978018</v>
+        <v>-8.4053607779780179</v>
       </c>
       <c r="H40">
         <v>-14.71293950230449</v>
       </c>
       <c r="I40">
-        <v>-9.730000000000032</v>
+        <v>-9.7300000000000324</v>
       </c>
       <c r="J40">
         <v>-316</v>
@@ -3703,31 +3725,31 @@
         <v>-16.67041719240293</v>
       </c>
       <c r="Q40">
-        <v>829.5155706928456</v>
+        <v>829.51557069284559</v>
       </c>
       <c r="R40">
-        <v>9.910580295016077</v>
+        <v>9.9105802950160768</v>
       </c>
       <c r="S40">
-        <v>520.9435696548314</v>
+        <v>520.94356965483144</v>
       </c>
       <c r="T40">
-        <v>6.223937510810411</v>
+        <v>6.2239375108104111</v>
       </c>
       <c r="U40">
-        <v>333.9943573177958</v>
+        <v>333.99435731779579</v>
       </c>
       <c r="V40">
         <v>3.990374639400188</v>
       </c>
       <c r="W40">
-        <v>218.2252866968874</v>
+        <v>218.22528669688739</v>
       </c>
       <c r="X40">
         <v>2.607231621229241</v>
       </c>
     </row>
-    <row r="41" spans="1:24">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3744,16 +3766,16 @@
         <v>12.77267181963586</v>
       </c>
       <c r="F41">
-        <v>6.551581023534737</v>
+        <v>6.5515810235347374</v>
       </c>
       <c r="G41">
         <v>14.84869244860295</v>
       </c>
       <c r="H41">
-        <v>18.6343574974628</v>
+        <v>18.634357497462801</v>
       </c>
       <c r="I41">
-        <v>17.49999999999999</v>
+        <v>17.499999999999989</v>
       </c>
       <c r="J41">
         <v>2476</v>
@@ -3765,43 +3787,43 @@
         <v>0.9</v>
       </c>
       <c r="M41">
-        <v>28.79644588045234</v>
+        <v>28.796445880452339</v>
       </c>
       <c r="N41">
-        <v>5.038513179280616</v>
+        <v>5.0385131792806161</v>
       </c>
       <c r="O41">
-        <v>56499.90039173105</v>
+        <v>56499.900391731047</v>
       </c>
       <c r="P41">
-        <v>-2.29971845607867</v>
+        <v>-2.2997184560786699</v>
       </c>
       <c r="Q41">
-        <v>34686.03767421642</v>
+        <v>34686.037674216423</v>
       </c>
       <c r="R41">
-        <v>48.64801917842416</v>
+        <v>48.648019178424157</v>
       </c>
       <c r="S41">
-        <v>21783.15744946886</v>
+        <v>21783.157449468861</v>
       </c>
       <c r="T41">
         <v>30.5514129726071</v>
       </c>
       <c r="U41">
-        <v>13965.91127424473</v>
+        <v>13965.911274244731</v>
       </c>
       <c r="V41">
-        <v>19.58753334396176</v>
+        <v>19.587533343961759</v>
       </c>
       <c r="W41">
-        <v>9125.049345984751</v>
+        <v>9125.0493459847512</v>
       </c>
       <c r="X41">
         <v>12.79810567459292</v>
       </c>
     </row>
-    <row r="42" spans="1:24">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3815,19 +3837,19 @@
         <v>44950</v>
       </c>
       <c r="E42">
-        <v>16.14736166183457</v>
+        <v>16.147361661834569</v>
       </c>
       <c r="F42">
-        <v>12.80101871493521</v>
+        <v>12.801018714935211</v>
       </c>
       <c r="G42">
-        <v>7.352942221797221</v>
+        <v>7.3529422217972211</v>
       </c>
       <c r="H42">
-        <v>8.077552133957639</v>
+        <v>8.0775521339576386</v>
       </c>
       <c r="I42">
-        <v>9.249999999999957</v>
+        <v>9.2499999999999574</v>
       </c>
       <c r="J42">
         <v>1922</v>
@@ -3839,25 +3861,25 @@
         <v>0.9</v>
       </c>
       <c r="M42">
-        <v>23.38709677419355</v>
+        <v>23.387096774193552</v>
       </c>
       <c r="N42">
-        <v>2.164491741705591</v>
+        <v>2.1644917417055911</v>
       </c>
       <c r="O42">
-        <v>42219.51882293896</v>
+        <v>42219.518822938961</v>
       </c>
       <c r="P42">
-        <v>-0.6247216037781889</v>
+        <v>-0.62472160377818886</v>
       </c>
       <c r="Q42">
-        <v>25919.12216351578</v>
+        <v>25919.122163515782</v>
       </c>
       <c r="R42">
-        <v>57.66211827256013</v>
+        <v>57.662118272560129</v>
       </c>
       <c r="S42">
-        <v>16277.4521651279</v>
+        <v>16277.452165127899</v>
       </c>
       <c r="T42">
         <v>36.2123518690276</v>
@@ -3866,16 +3888,16 @@
         <v>10436.01935285475</v>
       </c>
       <c r="V42">
-        <v>23.21695072937653</v>
+        <v>23.216950729376531</v>
       </c>
       <c r="W42">
-        <v>6818.687996827573</v>
+        <v>6818.6879968275734</v>
       </c>
       <c r="X42">
-        <v>15.16949498738058</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24">
+        <v>15.169494987380579</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3889,19 +3911,19 @@
         <v>5280</v>
       </c>
       <c r="E43">
-        <v>12.8862673598292</v>
+        <v>12.886267359829199</v>
       </c>
       <c r="F43">
-        <v>4.871333864136218</v>
+        <v>4.8713338641362176</v>
       </c>
       <c r="G43">
         <v>-1.05315363873919</v>
       </c>
       <c r="H43">
-        <v>-0.4678851724109592</v>
+        <v>-0.46788517241095923</v>
       </c>
       <c r="I43">
-        <v>-1.579999999999998</v>
+        <v>-1.5799999999999981</v>
       </c>
       <c r="J43">
         <v>-42</v>
@@ -3913,7 +3935,7 @@
         <v>2.1</v>
       </c>
       <c r="M43">
-        <v>-125.7142857142857</v>
+        <v>-125.71428571428569</v>
       </c>
       <c r="N43">
         <v>2.044134727061556</v>
@@ -3922,34 +3944,34 @@
         <v>2323.506946727759</v>
       </c>
       <c r="P43">
-        <v>-7.880620223953771</v>
+        <v>-7.8806202239537706</v>
       </c>
       <c r="Q43">
         <v>1426.431709290194</v>
       </c>
       <c r="R43">
-        <v>27.01575206989004</v>
+        <v>27.015752069890041</v>
       </c>
       <c r="S43">
-        <v>895.8125112537872</v>
+        <v>895.81251125378719</v>
       </c>
       <c r="T43">
-        <v>16.96614604647324</v>
+        <v>16.966146046473241</v>
       </c>
       <c r="U43">
-        <v>574.335381799015</v>
+        <v>574.33538179901495</v>
       </c>
       <c r="V43">
         <v>10.87756404922377</v>
       </c>
       <c r="W43">
-        <v>375.2593437798726</v>
+        <v>375.25934377987261</v>
       </c>
       <c r="X43">
-        <v>7.107184541285466</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24">
+        <v>7.1071845412854664</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3966,16 +3988,16 @@
         <v>13.76126028758577</v>
       </c>
       <c r="F44">
-        <v>16.66606638243547</v>
+        <v>16.666066382435471</v>
       </c>
       <c r="G44">
-        <v>13.78973793185716</v>
+        <v>13.789737931857159</v>
       </c>
       <c r="H44">
-        <v>9.514113381344245</v>
+        <v>9.5141133813442451</v>
       </c>
       <c r="I44">
-        <v>9.949999999999974</v>
+        <v>9.9499999999999744</v>
       </c>
       <c r="J44">
         <v>2124</v>
@@ -3990,40 +4012,40 @@
         <v>21.7984934086629</v>
       </c>
       <c r="N44">
-        <v>2.21753915417405</v>
+        <v>2.2175391541740499</v>
       </c>
       <c r="O44">
-        <v>75987.2392869766</v>
+        <v>75987.239286976604</v>
       </c>
       <c r="P44">
-        <v>5.079008813253649</v>
+        <v>5.0790088132536493</v>
       </c>
       <c r="Q44">
-        <v>46649.573298248</v>
+        <v>46649.573298247997</v>
       </c>
       <c r="R44">
         <v>100.7550179227819</v>
       </c>
       <c r="S44">
-        <v>29296.37018936988</v>
+        <v>29296.370189369882</v>
       </c>
       <c r="T44">
-        <v>63.27509760123085</v>
+        <v>63.275097601230847</v>
       </c>
       <c r="U44">
         <v>18782.88341216321</v>
       </c>
       <c r="V44">
-        <v>40.56778274765273</v>
+        <v>40.567782747652728</v>
       </c>
       <c r="W44">
-        <v>12272.36337323335</v>
+        <v>12272.363373233349</v>
       </c>
       <c r="X44">
-        <v>26.50618439143271</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24">
+        <v>26.506184391432711</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4040,7 +4062,7 @@
         <v>11.11869713005345</v>
       </c>
       <c r="F45">
-        <v>7.672052723707523</v>
+        <v>7.6720527237075231</v>
       </c>
       <c r="G45">
         <v>4.345699453579428</v>
@@ -4058,46 +4080,46 @@
         <v>4115</v>
       </c>
       <c r="L45">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M45">
-        <v>22.35849056603774</v>
+        <v>22.358490566037741</v>
       </c>
       <c r="N45">
-        <v>2.879708383961118</v>
+        <v>2.8797083839611179</v>
       </c>
       <c r="O45">
-        <v>6296.734551582196</v>
+        <v>6296.7345515821962</v>
       </c>
       <c r="P45">
-        <v>-6.127214810571269</v>
+        <v>-6.1272148105712692</v>
       </c>
       <c r="Q45">
         <v>3865.648795244339</v>
       </c>
       <c r="R45">
-        <v>32.62150882062733</v>
+        <v>32.621508820627326</v>
       </c>
       <c r="S45">
-        <v>2427.663751681585</v>
+        <v>2427.6637516815849</v>
       </c>
       <c r="T45">
-        <v>20.48661393824123</v>
+        <v>20.486613938241231</v>
       </c>
       <c r="U45">
         <v>1556.456479660244</v>
       </c>
       <c r="V45">
-        <v>13.13465383679531</v>
+        <v>13.134653836795311</v>
       </c>
       <c r="W45">
         <v>1016.957784055914</v>
       </c>
       <c r="X45">
-        <v>8.581922228319952</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24">
+        <v>8.5819222283199519</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -4120,10 +4142,10 @@
         <v>0</v>
       </c>
       <c r="H46">
-        <v>-3.324212623918683</v>
+        <v>-3.3242126239186831</v>
       </c>
       <c r="I46">
-        <v>-18.23000000000003</v>
+        <v>-18.230000000000029</v>
       </c>
       <c r="J46">
         <v>-166</v>
@@ -4135,34 +4157,34 @@
         <v>0</v>
       </c>
       <c r="M46">
-        <v>-9.819277108433734</v>
+        <v>-9.8192771084337345</v>
       </c>
       <c r="N46">
-        <v>2.071156289707751</v>
+        <v>2.0711562897077509</v>
       </c>
       <c r="O46">
         <v>787</v>
       </c>
       <c r="P46">
-        <v>-7.022318409979034</v>
+        <v>-7.0223184099790341</v>
       </c>
       <c r="Q46">
-        <v>483.1497305365775</v>
+        <v>483.14973053657752</v>
       </c>
       <c r="R46">
-        <v>29.64108776298021</v>
+        <v>29.641087762980209</v>
       </c>
       <c r="S46">
-        <v>303.4225687810412</v>
+        <v>303.42256878104121</v>
       </c>
       <c r="T46">
-        <v>18.61488152030928</v>
+        <v>18.614881520309279</v>
       </c>
       <c r="U46">
-        <v>194.5343637179084</v>
+        <v>194.53436371790841</v>
       </c>
       <c r="V46">
-        <v>11.93462354097598</v>
+        <v>11.934623540975981</v>
       </c>
       <c r="W46">
         <v>127.1048937343086</v>
@@ -4171,7 +4193,7 @@
         <v>7.797846241368628</v>
       </c>
     </row>
-    <row r="47" spans="1:24">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4191,13 +4213,13 @@
         <v>14.49259047881405</v>
       </c>
       <c r="G47">
-        <v>11.06073938306021</v>
+        <v>11.060739383060209</v>
       </c>
       <c r="H47">
         <v>11.72036267095088</v>
       </c>
       <c r="I47">
-        <v>8.429999999999964</v>
+        <v>8.4299999999999642</v>
       </c>
       <c r="J47">
         <v>961</v>
@@ -4209,13 +4231,13 @@
         <v>0.8</v>
       </c>
       <c r="M47">
-        <v>39.43808532778356</v>
+        <v>39.438085327783561</v>
       </c>
       <c r="N47">
-        <v>3.45929171230376</v>
+        <v>3.4592917123037599</v>
       </c>
       <c r="O47">
-        <v>31279.34340389993</v>
+        <v>31279.343403899929</v>
       </c>
       <c r="P47">
         <v>-1.901618571781194</v>
@@ -4224,28 +4246,28 @@
         <v>19202.80347770689</v>
       </c>
       <c r="R47">
-        <v>50.66702764566462</v>
+        <v>50.667027645664618</v>
       </c>
       <c r="S47">
-        <v>12059.54094713549</v>
+        <v>12059.540947135491</v>
       </c>
       <c r="T47">
-        <v>31.81936925365565</v>
+        <v>31.819369253655651</v>
       </c>
       <c r="U47">
-        <v>7731.775306977927</v>
+        <v>7731.7753069779274</v>
       </c>
       <c r="V47">
-        <v>20.40046255139295</v>
+        <v>20.400462551392948</v>
       </c>
       <c r="W47">
-        <v>5051.788588858512</v>
+        <v>5051.7885888585124</v>
       </c>
       <c r="X47">
         <v>13.32925749039185</v>
       </c>
     </row>
-    <row r="48" spans="1:24">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4262,7 +4284,7 @@
         <v>1.322623422257337</v>
       </c>
       <c r="F48">
-        <v>-1.576148099845298</v>
+        <v>-1.5761480998452979</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -4274,7 +4296,7 @@
         <v>0</v>
       </c>
       <c r="J48">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="K48">
         <v>534</v>
@@ -4295,10 +4317,10 @@
         <v>-17.95744518722007</v>
       </c>
       <c r="Q48">
-        <v>327.8296773907654</v>
+        <v>327.82967739076543</v>
       </c>
       <c r="R48">
-        <v>8.482009764314757</v>
+        <v>8.4820097643147569</v>
       </c>
       <c r="S48">
         <v>205.8801165553698</v>
@@ -4307,19 +4329,19 @@
         <v>5.326781799621469</v>
       </c>
       <c r="U48">
-        <v>131.9966330690764</v>
+        <v>131.99663306907641</v>
       </c>
       <c r="V48">
         <v>3.415178087168858</v>
       </c>
       <c r="W48">
-        <v>86.24398126317766</v>
+        <v>86.243981263177659</v>
       </c>
       <c r="X48">
-        <v>2.231409605774325</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24">
+        <v>2.2314096057743251</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4333,19 +4355,19 @@
         <v>10100</v>
       </c>
       <c r="E49">
-        <v>6.786090547831165</v>
+        <v>6.7860905478311651</v>
       </c>
       <c r="F49">
-        <v>8.063858202242528</v>
+        <v>8.0638582022425283</v>
       </c>
       <c r="G49">
-        <v>6.805380515713665</v>
+        <v>6.8053805157136651</v>
       </c>
       <c r="H49">
-        <v>6.188691576477694</v>
+        <v>6.1886915764776944</v>
       </c>
       <c r="I49">
-        <v>5.640000000000015</v>
+        <v>5.6400000000000148</v>
       </c>
       <c r="J49">
         <v>207</v>
@@ -4357,43 +4379,43 @@
         <v>1.2</v>
       </c>
       <c r="M49">
-        <v>48.79227053140097</v>
+        <v>48.792270531400973</v>
       </c>
       <c r="N49">
-        <v>2.756550218340611</v>
+        <v>2.7565502183406112</v>
       </c>
       <c r="O49">
-        <v>7077.612498493862</v>
+        <v>7077.6124984938624</v>
       </c>
       <c r="P49">
-        <v>-3.493505469534608</v>
+        <v>-3.4935054695346079</v>
       </c>
       <c r="Q49">
         <v>4345.040116251108</v>
       </c>
       <c r="R49">
-        <v>43.02019917080305</v>
+        <v>43.020199170803053</v>
       </c>
       <c r="S49">
         <v>2728.726003976888</v>
       </c>
       <c r="T49">
-        <v>27.01708914828602</v>
+        <v>27.017089148286018</v>
       </c>
       <c r="U49">
-        <v>1749.47756548465</v>
+        <v>1749.4775654846501</v>
       </c>
       <c r="V49">
-        <v>17.32156005430347</v>
+        <v>17.321560054303468</v>
       </c>
       <c r="W49">
         <v>1143.073932037709</v>
       </c>
       <c r="X49">
-        <v>11.31756368354167</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24">
+        <v>11.317563683541669</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4413,13 +4435,13 @@
         <v>0</v>
       </c>
       <c r="G50">
-        <v>21.08431887353571</v>
+        <v>21.084318873535711</v>
       </c>
       <c r="H50">
-        <v>11.42332578814282</v>
+        <v>11.423325788142821</v>
       </c>
       <c r="I50">
-        <v>8.379999999999953</v>
+        <v>8.3799999999999528</v>
       </c>
       <c r="J50">
         <v>201</v>
@@ -4431,43 +4453,43 @@
         <v>0</v>
       </c>
       <c r="M50">
-        <v>40.74626865671642</v>
+        <v>40.746268656716417</v>
       </c>
       <c r="N50">
-        <v>3.408239700374532</v>
+        <v>3.4082397003745322</v>
       </c>
       <c r="O50">
-        <v>16279.19037239439</v>
+        <v>16279.190372394391</v>
       </c>
       <c r="P50">
-        <v>7.11120126855298</v>
+        <v>7.1112012685529802</v>
       </c>
       <c r="Q50">
-        <v>9994.010726526041</v>
+        <v>9994.0107265260413</v>
       </c>
       <c r="R50">
-        <v>122.026992997876</v>
+        <v>122.02699299787599</v>
       </c>
       <c r="S50">
-        <v>6276.332605422491</v>
+        <v>6276.3326054224908</v>
       </c>
       <c r="T50">
-        <v>76.63409774630637</v>
+        <v>76.634097746306367</v>
       </c>
       <c r="U50">
-        <v>4023.966888102215</v>
+        <v>4023.9668881022149</v>
       </c>
       <c r="V50">
-        <v>49.13268483641288</v>
+        <v>49.132684836412878</v>
       </c>
       <c r="W50">
         <v>2629.180130068321</v>
       </c>
       <c r="X50">
-        <v>32.10232149045569</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24">
+        <v>32.102321490455687</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4481,19 +4503,19 @@
         <v>12100</v>
       </c>
       <c r="E51">
-        <v>9.74245714093901</v>
+        <v>9.7424571409390097</v>
       </c>
       <c r="F51">
-        <v>7.851392924021297</v>
+        <v>7.8513929240212974</v>
       </c>
       <c r="G51">
-        <v>4.626642257435066</v>
+        <v>4.6266422574350656</v>
       </c>
       <c r="H51">
-        <v>4.981607558663327</v>
+        <v>4.9816075586633266</v>
       </c>
       <c r="I51">
-        <v>3.709999999999994</v>
+        <v>3.7099999999999942</v>
       </c>
       <c r="J51">
         <v>180</v>
@@ -4505,43 +4527,43 @@
         <v>0.4</v>
       </c>
       <c r="M51">
-        <v>67.22222222222223</v>
+        <v>67.222222222222229</v>
       </c>
       <c r="N51">
-        <v>2.733845458653412</v>
+        <v>2.7338454586534122</v>
       </c>
       <c r="O51">
-        <v>6957.196800549079</v>
+        <v>6957.1968005490789</v>
       </c>
       <c r="P51">
-        <v>-5.383932893903831</v>
+        <v>-5.3839328939038307</v>
       </c>
       <c r="Q51">
-        <v>4271.115323348445</v>
+        <v>4271.1153233484447</v>
       </c>
       <c r="R51">
-        <v>35.29847374668137</v>
+        <v>35.298473746681367</v>
       </c>
       <c r="S51">
         <v>2682.300539692304</v>
       </c>
       <c r="T51">
-        <v>22.16777305530829</v>
+        <v>22.167773055308292</v>
       </c>
       <c r="U51">
         <v>1719.712646575709</v>
       </c>
       <c r="V51">
-        <v>14.2125012113695</v>
+        <v>14.212501211369499</v>
       </c>
       <c r="W51">
-        <v>1123.626124552049</v>
+        <v>1123.6261245520491</v>
       </c>
       <c r="X51">
-        <v>9.286166318611979</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24">
+        <v>9.2861663186119792</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -4555,10 +4577,10 @@
         <v>9000</v>
       </c>
       <c r="E52">
-        <v>-5.09734733799533</v>
+        <v>-5.0973473379953296</v>
       </c>
       <c r="F52">
-        <v>-5.09734733799533</v>
+        <v>-5.0973473379953296</v>
       </c>
       <c r="G52">
         <v>-17.93077931195371</v>
@@ -4567,7 +4589,7 @@
         <v>-10.90209775125378</v>
       </c>
       <c r="I52">
-        <v>-0.04000000000004889</v>
+        <v>-4.0000000000048892E-2</v>
       </c>
       <c r="J52">
         <v>-1</v>
@@ -4582,40 +4604,40 @@
         <v>-9000</v>
       </c>
       <c r="N52">
-        <v>3.942181340341656</v>
+        <v>3.9421813403416559</v>
       </c>
       <c r="O52">
-        <v>316.4528462940438</v>
+        <v>316.45284629404381</v>
       </c>
       <c r="P52">
-        <v>-28.45049233979544</v>
+        <v>-28.450492339795439</v>
       </c>
       <c r="Q52">
-        <v>194.2745964606102</v>
+        <v>194.27459646061021</v>
       </c>
       <c r="R52">
         <v>2.158606627340113</v>
       </c>
       <c r="S52">
-        <v>122.0062713095435</v>
+        <v>122.00627130954349</v>
       </c>
       <c r="T52">
         <v>1.355625236772706</v>
       </c>
       <c r="U52">
-        <v>78.22230381262119</v>
+        <v>78.222303812621192</v>
       </c>
       <c r="V52">
-        <v>0.8691367090291243</v>
+        <v>0.86913670902912432</v>
       </c>
       <c r="W52">
-        <v>51.10890139787031</v>
+        <v>51.108901397870312</v>
       </c>
       <c r="X52">
-        <v>0.567876682198559</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24">
+        <v>0.56787668219855902</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4638,7 +4660,7 @@
         <v>11.05921434618064</v>
       </c>
       <c r="H53">
-        <v>11.9397700792331</v>
+        <v>11.939770079233099</v>
       </c>
       <c r="I53">
         <v>10.35999999999996</v>
@@ -4653,28 +4675,28 @@
         <v>0</v>
       </c>
       <c r="M53">
-        <v>56.25942684766214</v>
+        <v>56.259426847662141</v>
       </c>
       <c r="N53">
-        <v>5.829946858393248</v>
+        <v>5.8299468583932477</v>
       </c>
       <c r="O53">
-        <v>18263.76054077786</v>
+        <v>18263.760540777861</v>
       </c>
       <c r="P53">
-        <v>-6.891755736623184</v>
+        <v>-6.8917557366231836</v>
       </c>
       <c r="Q53">
         <v>11212.36465547827</v>
       </c>
       <c r="R53">
-        <v>30.05995886187205</v>
+        <v>30.059958861872051</v>
       </c>
       <c r="S53">
-        <v>7041.470316244775</v>
+        <v>7041.4703162447749</v>
       </c>
       <c r="T53">
-        <v>18.87793650467768</v>
+        <v>18.877936504677681</v>
       </c>
       <c r="U53">
         <v>4514.522281952306</v>
@@ -4686,10 +4708,10 @@
         <v>2949.699291898894</v>
       </c>
       <c r="X53">
-        <v>7.908040997047973</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24">
+        <v>7.9080409970479728</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4703,19 +4725,19 @@
         <v>43200</v>
       </c>
       <c r="E54">
-        <v>7.454602486441559</v>
+        <v>7.4546024864415594</v>
       </c>
       <c r="F54">
-        <v>8.604000010079204</v>
+        <v>8.6040000100792042</v>
       </c>
       <c r="G54">
-        <v>7.033945590327164</v>
+        <v>7.0339455903271642</v>
       </c>
       <c r="H54">
-        <v>5.843754278958158</v>
+        <v>5.8437542789581576</v>
       </c>
       <c r="I54">
-        <v>7.189999999999998</v>
+        <v>7.1899999999999977</v>
       </c>
       <c r="J54">
         <v>520</v>
@@ -4730,40 +4752,40 @@
         <v>83.07692307692308</v>
       </c>
       <c r="N54">
-        <v>5.965202982601491</v>
+        <v>5.9652029826014914</v>
       </c>
       <c r="O54">
-        <v>14291.37027792688</v>
+        <v>14291.370277926881</v>
       </c>
       <c r="P54">
         <v>-10.47197325345388</v>
       </c>
       <c r="Q54">
-        <v>8773.661624877792</v>
+        <v>8773.6616248777918</v>
       </c>
       <c r="R54">
         <v>20.30940190943933</v>
       </c>
       <c r="S54">
-        <v>5509.941907407365</v>
+        <v>5509.9419074073649</v>
       </c>
       <c r="T54">
-        <v>12.75449515603557</v>
+        <v>12.754495156035571</v>
       </c>
       <c r="U54">
         <v>3532.608162228124</v>
       </c>
       <c r="V54">
-        <v>8.177333708861397</v>
+        <v>8.1773337088613971</v>
       </c>
       <c r="W54">
-        <v>2308.136087031198</v>
+        <v>2308.1360870311978</v>
       </c>
       <c r="X54">
-        <v>5.342907608868513</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24">
+        <v>5.3429076088685132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4777,19 +4799,19 @@
         <v>80700</v>
       </c>
       <c r="E55">
-        <v>7.118929602918357</v>
+        <v>7.1189296029183566</v>
       </c>
       <c r="F55">
-        <v>7.118929602918357</v>
+        <v>7.1189296029183566</v>
       </c>
       <c r="G55">
-        <v>8.359150513787284</v>
+        <v>8.3591505137872844</v>
       </c>
       <c r="H55">
-        <v>8.359150513787284</v>
+        <v>8.3591505137872844</v>
       </c>
       <c r="I55">
-        <v>6.930000000000007</v>
+        <v>6.9300000000000068</v>
       </c>
       <c r="J55">
         <v>1063</v>
@@ -4804,19 +4826,19 @@
         <v>75.91721542803387</v>
       </c>
       <c r="N55">
-        <v>5.265905383360522</v>
+        <v>5.2659053833605221</v>
       </c>
       <c r="O55">
-        <v>34202.38570145993</v>
+        <v>34202.385701459927</v>
       </c>
       <c r="P55">
-        <v>-8.226290441365759</v>
+        <v>-8.2262904413657587</v>
       </c>
       <c r="Q55">
-        <v>20997.29788483921</v>
+        <v>20997.297884839209</v>
       </c>
       <c r="R55">
-        <v>26.0189564867896</v>
+        <v>26.018956486789602</v>
       </c>
       <c r="S55">
         <v>13186.50028967843</v>
@@ -4825,19 +4847,20 @@
         <v>16.34014905784192</v>
       </c>
       <c r="U55">
-        <v>8454.306658282081</v>
+        <v>8454.3066582820811</v>
       </c>
       <c r="V55">
         <v>10.47621642909799</v>
       </c>
       <c r="W55">
-        <v>5523.876238937614</v>
+        <v>5523.8762389376143</v>
       </c>
       <c r="X55">
-        <v>6.844951968943761</v>
+        <v>6.8449519689437608</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>